<commit_message>
Not applicable (NA) recoded as 888
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="822" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E41EE56-B052-564D-8F96-8ACB4C593296}"/>
+  <xr:revisionPtr revIDLastSave="823" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{19F43EE7-CAA4-0040-8BCD-883EB651042F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="395">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>Evaluate the effectiveness of the commonly used the Lexia Reading Core5 intervention, with 4- to 6-year-old pupils in Northern Ireland</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Phonological skills</t>
@@ -747,9 +744,6 @@
     <t>word reading, sentence reading, spelling</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>The covariate was inferred based on the description; these seem to be very rigorous but I can't be sure because I don't know them enough</t>
   </si>
   <si>
@@ -1246,6 +1240,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>888</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1253,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1888,7 +1885,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1900,19 +1897,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1926,11 +1923,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="BE1" sqref="BE1"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="28.5" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
@@ -1945,7 +1942,7 @@
     <col min="63" max="63" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" ht="32">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:61" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" ht="80">
       <c r="A2" s="2">
         <v>7</v>
       </c>
@@ -2157,137 +2154,137 @@
       <c r="J2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="4">
+        <v>888</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R2" s="4"/>
       <c r="S2" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="16" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="Y2" s="8">
         <v>5</v>
       </c>
       <c r="Z2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>888</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AA2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE2" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AD2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="AF2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AH2" s="4">
+        <v>888</v>
       </c>
       <c r="AI2" s="4"/>
       <c r="AJ2" s="4"/>
-      <c r="AK2" s="4" t="s">
-        <v>69</v>
+      <c r="AK2" s="4">
+        <v>888</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ2" s="4"/>
       <c r="AR2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="AT2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BC2" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="BD2" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE2" s="8"/>
       <c r="BF2" s="8"/>
       <c r="BG2" s="8"/>
       <c r="BH2" s="10"/>
       <c r="BI2" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:61" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" ht="112">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -2302,153 +2299,153 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="4">
+        <v>888</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R3" s="4"/>
       <c r="S3" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T3" s="4"/>
       <c r="U3" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="X3" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Z3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="Z3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AD3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AD3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>69</v>
+      <c r="AF3" s="4">
+        <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="AH3" s="4" t="s">
-        <v>69</v>
+        <v>372</v>
+      </c>
+      <c r="AH3" s="4">
+        <v>888</v>
       </c>
       <c r="AI3" s="4"/>
       <c r="AJ3" s="4"/>
-      <c r="AK3" s="4" t="s">
-        <v>69</v>
+      <c r="AK3" s="4">
+        <v>888</v>
       </c>
       <c r="AL3" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AM3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AN3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO3" s="5" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>888</v>
       </c>
       <c r="AP3" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AQ3" s="4"/>
-      <c r="AR3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AU3" s="4" t="s">
-        <v>69</v>
+      <c r="AR3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AU3" s="4">
+        <v>888</v>
       </c>
       <c r="AV3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW3" s="4"/>
-      <c r="AX3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ3" s="4" t="s">
-        <v>69</v>
+      <c r="AX3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ3" s="4">
+        <v>888</v>
       </c>
       <c r="BA3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="BB3" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC3" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BD3" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE3" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BF3" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BG3" s="8"/>
       <c r="BH3" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BI3" s="8"/>
     </row>
-    <row r="4" spans="1:61" ht="160" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:61" ht="160">
       <c r="A4" s="2">
         <v>9</v>
       </c>
@@ -2463,157 +2460,157 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="4">
+        <v>888</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R4" s="4"/>
       <c r="S4" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T4" s="4"/>
       <c r="U4" s="16" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Y4" s="11">
         <v>43528</v>
       </c>
       <c r="Z4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC4" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AA4" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AD4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE4" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AD4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="AF4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>888</v>
+      </c>
+      <c r="AH4" s="4">
+        <v>888</v>
       </c>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
-      <c r="AK4" s="4" t="s">
-        <v>69</v>
+      <c r="AK4" s="4">
+        <v>888</v>
       </c>
       <c r="AL4" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>888</v>
+      </c>
+      <c r="AP4" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="AM4" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="AN4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>376</v>
-      </c>
       <c r="AQ4" s="4"/>
-      <c r="AR4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>69</v>
+      <c r="AR4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AS4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>888</v>
       </c>
       <c r="AV4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW4" s="4"/>
-      <c r="AX4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>69</v>
+      <c r="AX4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ4" s="4">
+        <v>888</v>
       </c>
       <c r="BA4" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BB4" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC4" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BD4" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE4" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BF4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="BG4" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="BH4" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="BG4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="BH4" s="10" t="s">
+      <c r="BI4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="BI4" s="8" t="s">
-        <v>110</v>
-      </c>
     </row>
-    <row r="5" spans="1:61" ht="208" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:61" ht="208">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -2628,149 +2625,149 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="4">
+        <v>888</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O5" s="4"/>
       <c r="P5" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R5" s="4"/>
       <c r="S5" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T5" s="4"/>
       <c r="U5" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="W5" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="W5" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="X5" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y5" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Z5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AB5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="AB5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="AD5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="AF5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH5" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>888</v>
       </c>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
-      <c r="AK5" s="4" t="s">
-        <v>69</v>
+      <c r="AK5" s="4">
+        <v>888</v>
       </c>
       <c r="AL5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO5" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ5" s="4"/>
       <c r="AR5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS5" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="AS5" s="4" t="s">
+      <c r="AT5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW5" s="4"/>
+      <c r="AX5" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AT5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AW5" s="4"/>
-      <c r="AX5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA5" s="4" t="s">
+      <c r="BB5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="BB5" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="BC5" s="8" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="BD5" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE5" s="8"/>
       <c r="BF5" s="8"/>
       <c r="BG5" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BH5" s="10"/>
       <c r="BI5" s="8"/>
     </row>
-    <row r="6" spans="1:61" ht="128" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:61" ht="128">
       <c r="A6" s="2">
         <v>13</v>
       </c>
@@ -2785,139 +2782,139 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="K6" s="4">
+        <v>888</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R6" s="4"/>
       <c r="S6" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T6" s="4"/>
       <c r="U6" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC6" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="V6" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="W6" s="8" t="s">
+      <c r="AD6" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE6" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="X6" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y6" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE6" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="AF6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG6" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="4" t="s">
-        <v>69</v>
+      <c r="AK6" s="4">
+        <v>888</v>
       </c>
       <c r="AL6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO6" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ6" s="4"/>
       <c r="AR6" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AS6" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AT6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AU6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW6" s="4"/>
-      <c r="AX6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ6" s="4" t="s">
-        <v>69</v>
+      <c r="AX6" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ6" s="4">
+        <v>888</v>
       </c>
       <c r="BA6" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="BB6" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC6" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="BD6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE6" s="8"/>
       <c r="BF6" s="8"/>
@@ -2925,7 +2922,7 @@
       <c r="BH6" s="10"/>
       <c r="BI6" s="8"/>
     </row>
-    <row r="7" spans="1:61" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:61" ht="96">
       <c r="A7" s="2">
         <v>15</v>
       </c>
@@ -2940,149 +2937,149 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="K7" s="4">
+        <v>888</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>260</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O7" s="4"/>
       <c r="P7" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="W7" s="8">
         <v>6</v>
       </c>
       <c r="X7" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y7" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AA7" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="AD7" s="4" t="s">
-        <v>69</v>
+        <v>261</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>888</v>
       </c>
       <c r="AE7" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
-      <c r="AK7" s="4" t="s">
-        <v>69</v>
+      <c r="AK7" s="4">
+        <v>888</v>
       </c>
       <c r="AL7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AO7" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AU7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW7" s="4"/>
-      <c r="AX7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ7" s="4" t="s">
-        <v>69</v>
+      <c r="AX7" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ7" s="4">
+        <v>888</v>
       </c>
       <c r="BA7" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="BB7" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC7" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="BD7" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE7" s="8"/>
       <c r="BF7" s="8"/>
       <c r="BG7" s="8"/>
       <c r="BH7" s="10"/>
       <c r="BI7" s="8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:61" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:61" ht="80">
       <c r="A8" s="2">
         <v>16</v>
       </c>
@@ -3097,151 +3094,151 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I8" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="K8" s="4">
+        <v>888</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="O8" s="4"/>
       <c r="P8" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="T8" s="4"/>
       <c r="U8" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="V8" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="X8" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="W8" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="X8" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="Y8" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AA8" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE8" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="AB8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC8" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="AD8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE8" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="AF8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AK8" s="4" t="s">
-        <v>69</v>
+      <c r="AK8" s="4">
+        <v>888</v>
       </c>
       <c r="AL8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ8" s="4"/>
       <c r="AR8" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AS8" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AT8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AU8" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW8" s="4"/>
-      <c r="AX8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ8" s="4" t="s">
-        <v>69</v>
+      <c r="AX8" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY8" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ8" s="4">
+        <v>888</v>
       </c>
       <c r="BA8" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="BB8" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC8" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="BD8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE8" s="8"/>
       <c r="BF8" s="8"/>
       <c r="BG8" s="8"/>
       <c r="BH8" s="10"/>
       <c r="BI8" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
-    <row r="9" spans="1:61" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:61" ht="112">
       <c r="A9" s="2">
         <v>18</v>
       </c>
@@ -3256,153 +3253,153 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I9" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="K9" s="4">
+        <v>888</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>292</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="O9" s="4"/>
       <c r="P9" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R9" s="4"/>
       <c r="S9" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="X9" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Y9" s="11">
         <v>43528</v>
       </c>
       <c r="Z9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA9" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB9" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="AC9" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="AD9" s="4" t="s">
-        <v>69</v>
+        <v>295</v>
+      </c>
+      <c r="AD9" s="4">
+        <v>888</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>69</v>
+        <v>296</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>888</v>
       </c>
       <c r="AG9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH9" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AH9" s="4">
+        <v>888</v>
       </c>
       <c r="AI9" s="4"/>
       <c r="AJ9" s="4"/>
-      <c r="AK9" s="4" t="s">
-        <v>69</v>
+      <c r="AK9" s="4">
+        <v>888</v>
       </c>
       <c r="AL9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AM9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AN9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AO9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ9" s="4"/>
       <c r="AR9" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="AS9" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="AT9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW9" s="4"/>
+      <c r="AX9" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY9" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ9" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA9" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="BB9" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BC9" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="AS9" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="AT9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV9" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW9" s="4"/>
-      <c r="AX9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA9" s="4" t="s">
+      <c r="BD9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE9" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="BB9" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="BC9" s="8" t="s">
+      <c r="BF9" s="8" t="s">
         <v>301</v>
-      </c>
-      <c r="BD9" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE9" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="BF9" s="8" t="s">
-        <v>303</v>
       </c>
       <c r="BG9" s="8"/>
       <c r="BH9" s="10"/>
       <c r="BI9" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:61" ht="160" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:61" ht="160">
       <c r="A10" s="2">
         <v>20</v>
       </c>
@@ -3417,137 +3414,137 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I10" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="K10" s="4">
+        <v>888</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>321</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>323</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T10" s="4"/>
       <c r="U10" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V10" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA10" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AD10" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE10" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="W10" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="X10" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="Y10" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="Z10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA10" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC10" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="AD10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE10" s="4" t="s">
-        <v>328</v>
-      </c>
       <c r="AF10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="4"/>
-      <c r="AK10" s="4" t="s">
-        <v>69</v>
+      <c r="AK10" s="4">
+        <v>888</v>
       </c>
       <c r="AL10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO10" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AP10" s="4"/>
       <c r="AQ10" s="4"/>
       <c r="AR10" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AS10" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AT10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW10" s="4"/>
-      <c r="AX10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ10" s="4" t="s">
-        <v>69</v>
+      <c r="AX10" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY10" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ10" s="4">
+        <v>888</v>
       </c>
       <c r="BA10" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="BB10" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC10" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="BD10" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE10" s="8"/>
       <c r="BF10" s="8"/>
@@ -3555,7 +3552,7 @@
       <c r="BH10" s="10"/>
       <c r="BI10" s="8"/>
     </row>
-    <row r="11" spans="1:61" ht="96" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:61" ht="96">
       <c r="A11" s="2">
         <v>21</v>
       </c>
@@ -3570,139 +3567,139 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I11" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="K11" s="4">
+        <v>888</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>332</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R11" s="4"/>
       <c r="S11" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T11" s="4"/>
       <c r="U11" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X11" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE11" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="Y11" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA11" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC11" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="AD11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE11" s="4" t="s">
-        <v>339</v>
-      </c>
       <c r="AF11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG11" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI11" s="4"/>
       <c r="AJ11" s="4"/>
-      <c r="AK11" s="4" t="s">
-        <v>69</v>
+      <c r="AK11" s="4">
+        <v>888</v>
       </c>
       <c r="AL11" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AM11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO11" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ11" s="4"/>
       <c r="AR11" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AS11" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="AT11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV11" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW11" s="4"/>
-      <c r="AX11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ11" s="4" t="s">
-        <v>69</v>
+      <c r="AX11" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ11" s="4">
+        <v>888</v>
       </c>
       <c r="BA11" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="BB11" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC11" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="BD11" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE11" s="8"/>
       <c r="BF11" s="8"/>
@@ -3710,7 +3707,7 @@
       <c r="BH11" s="10"/>
       <c r="BI11" s="8"/>
     </row>
-    <row r="12" spans="1:61" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:61" ht="144">
       <c r="A12" s="2">
         <v>19</v>
       </c>
@@ -3725,157 +3722,157 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I12" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="K12" s="4">
+        <v>888</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>306</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T12" s="4"/>
       <c r="U12" s="8">
         <v>7</v>
       </c>
       <c r="V12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="X12" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="W12" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="X12" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="Y12" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA12" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AB12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="AD12" s="4" t="s">
-        <v>69</v>
+        <v>309</v>
+      </c>
+      <c r="AD12" s="4">
+        <v>888</v>
       </c>
       <c r="AE12" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI12" s="4"/>
       <c r="AJ12" s="4"/>
-      <c r="AK12" s="4" t="s">
-        <v>69</v>
+      <c r="AK12" s="4">
+        <v>888</v>
       </c>
       <c r="AL12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP12" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AP12" s="4">
+        <v>888</v>
       </c>
       <c r="AQ12" s="4"/>
       <c r="AR12" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="AS12" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW12" s="4"/>
+      <c r="AX12" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY12" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ12" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA12" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="BB12" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="AS12" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="AT12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW12" s="4"/>
-      <c r="AX12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA12" s="5" t="s">
+      <c r="BC12" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="BB12" s="5" t="s">
+      <c r="BD12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE12" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="BF12" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="BC12" s="10" t="s">
+      <c r="BG12" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="BH12" s="10" t="s">
         <v>316</v>
       </c>
-      <c r="BD12" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="BE12" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="BF12" s="8" t="s">
+      <c r="BI12" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="BG12" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="BH12" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="BI12" s="8" t="s">
-        <v>319</v>
-      </c>
     </row>
-    <row r="13" spans="1:61" ht="112" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:61" ht="112">
       <c r="A13" s="2">
         <v>17</v>
       </c>
@@ -3890,301 +3887,301 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I13" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="K13" s="4">
+        <v>888</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>280</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T13" s="4"/>
       <c r="U13" s="16" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="X13" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA13" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="AD13" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE13" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="AB13" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC13" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE13" s="4" t="s">
-        <v>285</v>
-      </c>
       <c r="AF13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG13" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI13" s="4"/>
       <c r="AJ13" s="4"/>
       <c r="AK13" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="AL13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO13" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ13" s="4"/>
       <c r="AR13" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AS13" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AT13" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AU13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AV13" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW13" s="4"/>
-      <c r="AX13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ13" s="4" t="s">
-        <v>69</v>
+      <c r="AX13" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY13" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ13" s="4">
+        <v>888</v>
       </c>
       <c r="BA13" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BB13" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="BC13" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BD13" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BE13" s="8"/>
       <c r="BF13" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="BG13" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BH13" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="BI13" s="8"/>
     </row>
-    <row r="14" spans="1:61" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:61" ht="16">
       <c r="A14" s="2">
         <v>22</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="12">
         <v>2018</v>
       </c>
       <c r="I14" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="K14" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="L14" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="N14" s="12" t="s">
+        <v>371</v>
+      </c>
+      <c r="O14" s="12" t="s">
         <v>344</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>345</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>373</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>346</v>
       </c>
       <c r="P14" s="12">
         <v>78</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U14" s="2">
         <v>7</v>
       </c>
       <c r="V14" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W14" s="15" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="X14" s="15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y14" s="15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Z14" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="AA14" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="AB14" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="AC14" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="AA14" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="AB14" s="12" t="s">
+      <c r="AD14" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="AC14" s="12" t="s">
+      <c r="AE14" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="AD14" s="13" t="s">
+      <c r="AF14" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="AE14" s="12" t="s">
+      <c r="AG14" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="AF14" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="AG14" s="12" t="s">
-        <v>353</v>
-      </c>
       <c r="AH14" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ14" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="AK14" s="4" t="s">
-        <v>69</v>
+        <v>351</v>
+      </c>
+      <c r="AJ14" s="12">
+        <v>888</v>
+      </c>
+      <c r="AK14" s="4">
+        <v>888</v>
       </c>
       <c r="AL14" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AM14" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AN14" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AO14" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AP14" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ14" s="12"/>
       <c r="AR14" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="AS14" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="AT14" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="AU14" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV14" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="AW14" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="AX14" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="AY14" s="12">
+        <v>888</v>
+      </c>
+      <c r="AZ14" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="BA14" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="AS14" s="12" t="s">
+      <c r="BB14" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="AT14" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="AU14" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="AV14" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="AW14" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="AX14" s="12" t="s">
+      <c r="BC14" s="12" t="s">
         <v>363</v>
       </c>
-      <c r="AY14" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="AZ14" s="12" t="s">
-        <v>364</v>
-      </c>
-      <c r="BA14" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="BB14" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="BC14" s="12" t="s">
-        <v>365</v>
-      </c>
       <c r="BD14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:61" ht="304" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:61" ht="304">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -4199,153 +4196,153 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="4">
+        <v>888</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O15" s="4"/>
       <c r="P15" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R15" s="4"/>
       <c r="S15" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T15" s="4"/>
       <c r="U15" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W15" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X15" s="17" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Y15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC15" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="Z15" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC15" s="4" t="s">
+      <c r="AD15" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE15" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AD15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE15" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="AF15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG15" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI15" s="4"/>
       <c r="AJ15" s="4"/>
-      <c r="AK15" s="4" t="s">
-        <v>69</v>
+      <c r="AK15" s="4">
+        <v>888</v>
       </c>
       <c r="AL15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO15" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP15" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AQ15" s="4"/>
       <c r="AR15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AS15" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AT15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV15" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW15" s="4"/>
+      <c r="AX15" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY15" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ15" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA15" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BB15" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="AT15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW15" s="4"/>
-      <c r="AX15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA15" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="BB15" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="BC15" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BD15" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE15" s="8"/>
       <c r="BF15" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BG15" s="8"/>
       <c r="BH15" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BI15" s="8" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
-    <row r="16" spans="1:61" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:61" ht="96">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -4360,151 +4357,151 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="J16" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="4">
+        <v>888</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R16" s="4"/>
       <c r="S16" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="T16" s="4"/>
       <c r="U16" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="X16" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y16" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>888</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC16" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="X16" s="17" t="s">
-        <v>394</v>
-      </c>
-      <c r="Y16" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB16" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC16" s="4" t="s">
+      <c r="AD16" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE16" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="AD16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE16" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="AF16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG16" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI16" s="4"/>
       <c r="AJ16" s="4"/>
-      <c r="AK16" s="4" t="s">
-        <v>69</v>
+      <c r="AK16" s="4">
+        <v>888</v>
       </c>
       <c r="AL16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN16" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO16" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP16" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AQ16" s="4"/>
       <c r="AR16" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AS16" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW16" s="4"/>
+      <c r="AX16" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY16" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ16" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA16" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="AT16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW16" s="4"/>
-      <c r="AX16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA16" s="4" t="s">
+      <c r="BB16" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="BB16" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="BC16" s="8" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="BD16" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="BE16" s="8"/>
       <c r="BF16" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="BG16" s="8"/>
       <c r="BH16" s="8"/>
       <c r="BI16" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
-    <row r="17" spans="1:63" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:63" ht="96">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -4519,151 +4516,151 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="4">
+        <v>888</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R17" s="4"/>
       <c r="S17" s="16" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="T17" s="4"/>
       <c r="U17" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="W17" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="X17" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="W17" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="X17" s="8" t="s">
+      <c r="Y17" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>888</v>
+      </c>
+      <c r="AB17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC17" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="Y17" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC17" s="4" t="s">
+      <c r="AD17" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE17" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="AD17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE17" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="AF17" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG17" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI17" s="4"/>
       <c r="AJ17" s="4"/>
-      <c r="AK17" s="4" t="s">
-        <v>69</v>
+      <c r="AK17" s="4">
+        <v>888</v>
       </c>
       <c r="AL17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO17" s="5" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AM17" s="4">
+        <v>888</v>
+      </c>
+      <c r="AN17" s="4">
+        <v>888</v>
+      </c>
+      <c r="AO17" s="5">
+        <v>888</v>
       </c>
       <c r="AP17" s="4"/>
       <c r="AQ17" s="4"/>
       <c r="AR17" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AS17" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AT17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW17" s="4"/>
+      <c r="AX17" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY17" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ17" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="AT17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW17" s="4"/>
-      <c r="AX17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA17" s="4" t="s">
+      <c r="BB17" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BC17" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="BB17" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="BC17" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="BD17" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BE17" s="8"/>
       <c r="BF17" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BG17" s="8"/>
       <c r="BH17" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="BI17" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="BI17" s="8" t="s">
-        <v>174</v>
-      </c>
     </row>
-    <row r="18" spans="1:63" ht="112" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:63" ht="112">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -4678,149 +4675,149 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I18" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="4">
+        <v>888</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R18" s="4"/>
       <c r="S18" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T18" s="4"/>
       <c r="U18" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V18" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="W18" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="W18" s="8" t="s">
+      <c r="X18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>888</v>
+      </c>
+      <c r="AB18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC18" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="X18" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB18" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC18" s="4" t="s">
+      <c r="AD18" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE18" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AD18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE18" s="4" t="s">
-        <v>185</v>
-      </c>
       <c r="AF18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG18" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AH18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI18" s="4"/>
       <c r="AJ18" s="4"/>
-      <c r="AK18" s="4" t="s">
-        <v>69</v>
+      <c r="AK18" s="4">
+        <v>888</v>
       </c>
       <c r="AL18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO18" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AQ18" s="4"/>
       <c r="AR18" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AS18" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AT18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AU18" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AV18" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW18" s="4"/>
-      <c r="AX18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ18" s="4" t="s">
-        <v>69</v>
+      <c r="AX18" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY18" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ18" s="4">
+        <v>888</v>
       </c>
       <c r="BA18" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="BB18" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="BB18" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="BC18" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="BD18" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BE18" s="8"/>
       <c r="BF18" s="8"/>
       <c r="BG18" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BH18" s="10"/>
       <c r="BI18" s="8"/>
     </row>
-    <row r="19" spans="1:63" ht="272" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:63" ht="272">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -4835,151 +4832,151 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="4">
+        <v>888</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>192</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R19" s="4"/>
       <c r="S19" s="16" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="V19" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="V19" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="W19" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X19" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y19" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z19" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA19" s="9">
         <v>43499</v>
       </c>
       <c r="AB19" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC19" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AD19" s="4" t="s">
-        <v>69</v>
+        <v>183</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>888</v>
       </c>
       <c r="AE19" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AF19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="AG19" s="5">
+        <v>888</v>
       </c>
       <c r="AH19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AI19" s="4"/>
       <c r="AJ19" s="4"/>
       <c r="AK19" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AL19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP19" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="AL19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AN19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AO19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP19" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="AQ19" s="4"/>
       <c r="AR19" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS19" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="AT19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW19" s="4"/>
+      <c r="AX19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ19" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA19" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="BB19" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BC19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="AS19" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="AT19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW19" s="4"/>
-      <c r="AX19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA19" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="BB19" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="BC19" s="8" t="s">
-        <v>201</v>
-      </c>
       <c r="BD19" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE19" s="8"/>
       <c r="BF19" s="8"/>
       <c r="BG19" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BH19" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BI19" s="8"/>
     </row>
-    <row r="20" spans="1:63" ht="144" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:63" ht="144">
       <c r="A20" s="2">
         <v>10</v>
       </c>
@@ -4994,151 +4991,151 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="4">
+        <v>888</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R20" s="4"/>
       <c r="S20" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T20" s="4"/>
       <c r="U20" s="16" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="V20" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W20" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="X20" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y20" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA20" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC20" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="X20" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="Y20" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="Z20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AA20" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB20" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC20" s="4" t="s">
+      <c r="AD20" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE20" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="AD20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE20" s="4" t="s">
-        <v>213</v>
-      </c>
       <c r="AF20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG20" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI20" s="4"/>
       <c r="AJ20" s="4"/>
-      <c r="AK20" s="4" t="s">
-        <v>69</v>
+      <c r="AK20" s="4">
+        <v>888</v>
       </c>
       <c r="AL20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN20" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO20" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AP20" s="4" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AP20" s="4">
+        <v>888</v>
       </c>
       <c r="AQ20" s="4"/>
       <c r="AR20" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AS20" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="AT20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW20" s="4"/>
+      <c r="AX20" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY20" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ20" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA20" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="AT20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AW20" s="4"/>
-      <c r="AX20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA20" s="4" t="s">
+      <c r="BB20" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="BB20" s="4" t="s">
+      <c r="BC20" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="BC20" s="8" t="s">
-        <v>217</v>
-      </c>
       <c r="BD20" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE20" s="8"/>
       <c r="BF20" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BG20" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BH20" s="10"/>
       <c r="BI20" s="8"/>
     </row>
-    <row r="21" spans="1:63" ht="144" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:63" ht="144">
       <c r="A21" s="2">
         <v>12</v>
       </c>
@@ -5153,153 +5150,153 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I21" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="K21" s="4">
+        <v>888</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>221</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R21" s="4"/>
       <c r="S21" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T21" s="4"/>
       <c r="U21" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="W21" s="8">
         <v>93.4</v>
       </c>
       <c r="X21" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Y21" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z21" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA21" s="11">
         <v>43531</v>
       </c>
       <c r="AB21" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC21" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD21" s="4">
+        <v>888</v>
+      </c>
+      <c r="AE21" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="AD21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE21" s="4" t="s">
-        <v>227</v>
-      </c>
       <c r="AF21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG21" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AH21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI21" s="4"/>
       <c r="AJ21" s="4"/>
-      <c r="AK21" s="4" t="s">
-        <v>69</v>
+      <c r="AK21" s="4">
+        <v>888</v>
       </c>
       <c r="AL21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AM21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AN21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AO21" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AP21" s="4"/>
       <c r="AQ21" s="4"/>
       <c r="AR21" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="AS21" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="AS21" s="4" t="s">
+      <c r="AT21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW21" s="4"/>
+      <c r="AX21" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY21" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ21" s="4">
+        <v>888</v>
+      </c>
+      <c r="BA21" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="AT21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AV21" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AW21" s="4"/>
-      <c r="AX21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA21" s="4" t="s">
-        <v>230</v>
-      </c>
       <c r="BB21" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC21" s="8" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="BD21" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE21" s="8"/>
       <c r="BF21" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="BG21" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="BH21" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="BI21" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="BG21" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="BH21" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="BI21" s="8" t="s">
-        <v>234</v>
-      </c>
     </row>
-    <row r="22" spans="1:63" ht="96" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:63" ht="96">
       <c r="A22" s="2">
         <v>14</v>
       </c>
@@ -5314,155 +5311,155 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="K22" s="4">
+        <v>888</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>251</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R22" s="4"/>
       <c r="S22" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="T22" s="4"/>
       <c r="U22" s="16" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="V22" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W22" s="8">
         <v>25</v>
       </c>
       <c r="X22" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Y22" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z22" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AA22" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AD22" s="4" t="s">
-        <v>69</v>
+        <v>252</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>888</v>
       </c>
       <c r="AE22" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="AF22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG22" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH22" s="4" t="s">
-        <v>69</v>
+        <v>253</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG22" s="5">
+        <v>888</v>
+      </c>
+      <c r="AH22" s="4">
+        <v>888</v>
       </c>
       <c r="AI22" s="4"/>
       <c r="AJ22" s="4"/>
-      <c r="AK22" s="4" t="s">
-        <v>69</v>
+      <c r="AK22" s="4">
+        <v>888</v>
       </c>
       <c r="AL22" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AM22" s="4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AN22" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO22" s="5" t="s">
-        <v>69</v>
+        <v>79</v>
+      </c>
+      <c r="AO22" s="5">
+        <v>888</v>
       </c>
       <c r="AP22" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AQ22" s="4"/>
-      <c r="AR22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AU22" s="4" t="s">
-        <v>69</v>
+      <c r="AR22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AS22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AT22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AU22" s="4">
+        <v>888</v>
       </c>
       <c r="AV22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AW22" s="4"/>
-      <c r="AX22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ22" s="4" t="s">
-        <v>69</v>
+      <c r="AX22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AY22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AZ22" s="4">
+        <v>888</v>
       </c>
       <c r="BA22" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="BB22" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="BC22" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BD22" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BE22" s="8"/>
       <c r="BF22" s="8"/>
       <c r="BG22" s="8" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BH22" s="10" t="s">
-        <v>69</v>
+        <v>394</v>
       </c>
       <c r="BI22" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="BJ22" s="2"/>
       <c r="BK22" s="2"/>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:63">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5625,18 +5622,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5658,25 +5655,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ranges have been fixes (formatting)
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="840" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{97A2988D-3CCB-2448-962B-8AA1F6DEF578}"/>
+  <xr:revisionPtr revIDLastSave="896" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDD6F8C6-6186-1E44-806D-BCB36B2107F1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="382">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Phoneme segmentation</t>
   </si>
   <si>
-    <t>n2=.064-.070; d=.35-.36</t>
-  </si>
-  <si>
     <t>Cazzell et al</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>14-17</t>
   </si>
   <si>
     <t>3</t>
@@ -750,9 +744,6 @@
     <t>Word recognition, word reading aloud and word spelling.</t>
   </si>
   <si>
-    <t>d=.79-1.28</t>
-  </si>
-  <si>
     <t>Wood et al</t>
   </si>
   <si>
@@ -811,9 +802,6 @@
     <t>Word reading aloud</t>
   </si>
   <si>
-    <t>n2= .33</t>
-  </si>
-  <si>
     <t>Computer-assisted learning in young poor readers:The effect of grapho-syllabic training on the development of word reading and reading comprehension</t>
   </si>
   <si>
@@ -839,9 +827,6 @@
   </si>
   <si>
     <t>Silent word reading, word reading aloud and Reading comprehension</t>
-  </si>
-  <si>
-    <t>d=1.09-6.96</t>
   </si>
   <si>
     <t>Kyle et al</t>
@@ -917,9 +902,6 @@
     <t>Reading and Spelling</t>
   </si>
   <si>
-    <t>d = 1.5-12.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Descriptive data was presented in narrative (only the mean of raw scores). </t>
   </si>
   <si>
@@ -1008,9 +990,6 @@
     <t xml:space="preserve">Reading comprehension, Passage comprehension, Word decoding, Sight word reading, and Pseudoword reading. </t>
   </si>
   <si>
-    <t>d=.45-1.34</t>
-  </si>
-  <si>
     <t>Karemaker et al</t>
   </si>
   <si>
@@ -1041,9 +1020,6 @@
     <t>Written word recognition, Written word naming, and Phonological awareness</t>
   </si>
   <si>
-    <t>d=.40-.68</t>
-  </si>
-  <si>
     <t>An evaluation of the effectiveness of a computer-assisted reading intervention</t>
   </si>
   <si>
@@ -1149,9 +1125,6 @@
     <t>Missing information about instruments and sloppy presentation of results make it hard to determine improvements. Rate of reading (WPM) and spelling show some improvements but hypothesis testing analyses were not performed</t>
   </si>
   <si>
-    <t>n2 = .09-.15</t>
-  </si>
-  <si>
     <t>d = .94</t>
   </si>
   <si>
@@ -1198,6 +1171,39 @@
   </si>
   <si>
     <t>888</t>
+  </si>
+  <si>
+    <t>14 - 17</t>
+  </si>
+  <si>
+    <t>3 - 4</t>
+  </si>
+  <si>
+    <t>n2 = .09 - .15</t>
+  </si>
+  <si>
+    <t>d = 1.5 - 12.1</t>
+  </si>
+  <si>
+    <t>n2 = .064 - .070; d = .35 - .36</t>
+  </si>
+  <si>
+    <t>d = .79 - 1.28</t>
+  </si>
+  <si>
+    <t>n2 =  .33</t>
+  </si>
+  <si>
+    <t>d = 1.09 - 6.96</t>
+  </si>
+  <si>
+    <t>d = .45 - 1.34</t>
+  </si>
+  <si>
+    <t>d = .40 - .68</t>
+  </si>
+  <si>
+    <t>3 - 7</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1254,11 +1260,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1830,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2026,7 +2030,7 @@
         <v>57</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>67</v>
@@ -2038,19 +2042,19 @@
         <v>67</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>371</v>
+        <v>196</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>362</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="Q2" s="5">
         <v>5</v>
@@ -2136,11 +2140,11 @@
         <v>71</v>
       </c>
       <c r="AV2" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AW2" s="7"/>
+        <v>375</v>
+      </c>
+      <c r="AW2" s="6"/>
       <c r="AX2" s="5" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="AZ2"/>
       <c r="BA2"/>
@@ -2151,52 +2155,52 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3">
+        <v>888</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="3">
-        <v>888</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="K3" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>80</v>
+        <v>371</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>63</v>
@@ -2208,19 +2212,19 @@
         <v>64</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="V3" s="3">
         <v>888</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="X3" s="3">
         <v>888</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="Z3" s="3">
         <v>888</v>
@@ -2230,7 +2234,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AD3" s="3" t="s">
         <v>67</v>
@@ -2242,10 +2246,10 @@
         <v>888</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AI3" s="3">
         <v>888</v>
@@ -2264,7 +2268,7 @@
       </c>
       <c r="AN3" s="3"/>
       <c r="AO3" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AP3" s="3">
         <v>888</v>
@@ -2277,16 +2281,16 @@
       </c>
       <c r="AS3" s="5"/>
       <c r="AT3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AU3" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV3" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AW3" s="7" t="s">
-        <v>85</v>
+        <v>370</v>
+      </c>
+      <c r="AW3" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="AX3" s="5"/>
       <c r="AZ3"/>
@@ -2298,70 +2302,70 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="3">
+        <v>888</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="3">
-        <v>888</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="I4" s="5" t="s">
         <v>67</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>372</v>
+        <v>196</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>363</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>43528</v>
+        <v>89</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="V4" s="3">
         <v>888</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>67</v>
@@ -2377,10 +2381,10 @@
         <v>888</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>67</v>
@@ -2389,10 +2393,10 @@
         <v>888</v>
       </c>
       <c r="AG4" s="3" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AH4" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AI4" s="3">
         <v>888</v>
@@ -2411,34 +2415,34 @@
       </c>
       <c r="AN4" s="3"/>
       <c r="AO4" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP4" s="3">
+        <v>888</v>
+      </c>
+      <c r="AQ4" s="3">
+        <v>888</v>
+      </c>
+      <c r="AR4" s="3">
+        <v>888</v>
+      </c>
+      <c r="AS4" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AV4" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="AW4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX4" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="AP4" s="3">
-        <v>888</v>
-      </c>
-      <c r="AQ4" s="3">
-        <v>888</v>
-      </c>
-      <c r="AR4" s="3">
-        <v>888</v>
-      </c>
-      <c r="AS4" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="AV4" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AW4" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AX4" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="AZ4"/>
       <c r="BA4"/>
@@ -2449,40 +2453,40 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="3">
+        <v>888</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="3">
-        <v>888</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="K5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="M5" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>60</v>
@@ -2491,28 +2495,28 @@
         <v>61</v>
       </c>
       <c r="P5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S5" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="V5" s="3">
         <v>888</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>59</v>
@@ -2544,10 +2548,10 @@
       </c>
       <c r="AH5" s="5"/>
       <c r="AI5" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AK5" s="3" t="s">
         <v>59</v>
@@ -2570,18 +2574,18 @@
         <v>888</v>
       </c>
       <c r="AS5" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT5" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AU5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="AW5" s="7"/>
+        <v>373</v>
+      </c>
+      <c r="AW5" s="6"/>
       <c r="AX5" s="5"/>
       <c r="AZ5"/>
       <c r="BA5"/>
@@ -2592,49 +2596,49 @@
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="3">
+        <v>888</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="F6" s="3">
-        <v>888</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="K6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="5" t="s">
+      <c r="N6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>228</v>
-      </c>
       <c r="P6" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q6" s="5" t="s">
         <v>62</v>
@@ -2643,19 +2647,19 @@
         <v>63</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="V6" s="3">
         <v>888</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="X6" s="3" t="s">
         <v>59</v>
@@ -2687,10 +2691,10 @@
       </c>
       <c r="AH6" s="5"/>
       <c r="AI6" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK6" s="3" t="s">
         <v>59</v>
@@ -2714,15 +2718,15 @@
       </c>
       <c r="AS6" s="5"/>
       <c r="AT6" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AU6" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="AW6" s="7"/>
+        <v>376</v>
+      </c>
+      <c r="AW6" s="6"/>
       <c r="AX6" s="5"/>
       <c r="AZ6"/>
       <c r="BA6"/>
@@ -2733,70 +2737,70 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" s="3">
+        <v>888</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F7" s="3">
-        <v>888</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>247</v>
-      </c>
       <c r="I7" s="5" t="s">
         <v>67</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O7" s="5">
         <v>6</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="V7" s="3">
         <v>888</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X7" s="3" t="s">
         <v>59</v>
@@ -2828,10 +2832,10 @@
       </c>
       <c r="AH7" s="5"/>
       <c r="AI7" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK7" s="3" t="s">
         <v>59</v>
@@ -2855,17 +2859,17 @@
       </c>
       <c r="AS7" s="5"/>
       <c r="AT7" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AU7" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV7" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AW7" s="7"/>
+        <v>377</v>
+      </c>
+      <c r="AW7" s="6"/>
       <c r="AX7" s="5" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="AZ7"/>
       <c r="BA7"/>
@@ -2876,70 +2880,70 @@
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="F8" s="3">
+        <v>888</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="K8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="S8" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="F8" s="3">
-        <v>888</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="V8" s="3">
         <v>888</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="X8" s="3" t="s">
         <v>67</v>
@@ -2971,10 +2975,10 @@
       </c>
       <c r="AH8" s="5"/>
       <c r="AI8" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK8" s="3" t="s">
         <v>59</v>
@@ -2998,17 +3002,17 @@
       </c>
       <c r="AS8" s="5"/>
       <c r="AT8" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AU8" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AV8" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="AV8" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="AW8" s="7"/>
+      <c r="AW8" s="6"/>
       <c r="AX8" s="5" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="AZ8"/>
       <c r="BA8"/>
@@ -3019,70 +3023,70 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F9" s="3">
+        <v>888</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="K9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="N9" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="F9" s="3">
-        <v>888</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="O9" s="5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Q9" s="8">
-        <v>43528</v>
+      <c r="Q9" s="10" t="s">
+        <v>372</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="V9" s="3">
         <v>888</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="X9" s="3">
         <v>888</v>
@@ -3113,13 +3117,13 @@
         <v>67</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK9" s="3" t="s">
         <v>59</v>
@@ -3132,7 +3136,7 @@
       </c>
       <c r="AN9" s="3"/>
       <c r="AO9" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="AP9" s="3">
         <v>888</v>
@@ -3145,17 +3149,17 @@
       </c>
       <c r="AS9" s="5"/>
       <c r="AT9" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="AU9" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV9" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AW9" s="7"/>
+        <v>374</v>
+      </c>
+      <c r="AW9" s="6"/>
       <c r="AX9" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="AZ9"/>
       <c r="BA9"/>
@@ -3166,70 +3170,70 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" s="3">
+        <v>888</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="F10" s="3">
-        <v>888</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="O10" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="V10" s="3">
         <v>888</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="X10" s="3" t="s">
         <v>59</v>
@@ -3259,10 +3263,10 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="5"/>
       <c r="AI10" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK10" s="3" t="s">
         <v>67</v>
@@ -3286,15 +3290,15 @@
       </c>
       <c r="AS10" s="5"/>
       <c r="AT10" s="4" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="AV10" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="AW10" s="7"/>
+        <v>369</v>
+      </c>
+      <c r="AV10" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="AW10" s="6"/>
       <c r="AX10" s="5"/>
       <c r="AZ10"/>
       <c r="BA10"/>
@@ -3305,49 +3309,49 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="F11" s="3">
         <v>888</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>67</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>373</v>
+        <v>196</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>364</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>62</v>
@@ -3356,19 +3360,19 @@
         <v>63</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="V11" s="3">
         <v>888</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>67</v>
@@ -3384,7 +3388,7 @@
         <v>888</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AD11" s="3" t="s">
         <v>59</v>
@@ -3400,10 +3404,10 @@
       </c>
       <c r="AH11" s="5"/>
       <c r="AI11" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK11" s="3" t="s">
         <v>59</v>
@@ -3427,15 +3431,15 @@
       </c>
       <c r="AS11" s="5"/>
       <c r="AT11" s="4" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="AV11" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="AW11" s="7"/>
+        <v>369</v>
+      </c>
+      <c r="AV11" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="AW11" s="6"/>
       <c r="AX11" s="5"/>
       <c r="AZ11"/>
       <c r="BA11"/>
@@ -3446,70 +3450,70 @@
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="F12" s="3">
         <v>888</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>67</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M12" s="5">
         <v>7</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="V12" s="3">
         <v>888</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="X12" s="3" t="s">
         <v>67</v>
@@ -3540,13 +3544,13 @@
         <v>888</v>
       </c>
       <c r="AH12" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK12" s="3" t="s">
         <v>59</v>
@@ -3559,7 +3563,7 @@
       </c>
       <c r="AN12" s="3"/>
       <c r="AO12" s="5" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="AP12" s="3">
         <v>888</v>
@@ -3571,22 +3575,22 @@
         <v>888</v>
       </c>
       <c r="AS12" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="AU12" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="AV12" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="AW12" s="7" t="s">
-        <v>304</v>
+        <v>295</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="AW12" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="AX12" s="5" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="AZ12"/>
       <c r="BA12"/>
@@ -3597,70 +3601,70 @@
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F13" s="3">
+        <v>888</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" s="3">
-        <v>888</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>268</v>
-      </c>
       <c r="K13" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>368</v>
+        <v>78</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>359</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>344</v>
+        <v>365</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>336</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>62</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="V13" s="3">
         <v>888</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>67</v>
@@ -3673,7 +3677,7 @@
       </c>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="AC13" s="3" t="s">
         <v>59</v>
@@ -3692,10 +3696,10 @@
       </c>
       <c r="AH13" s="5"/>
       <c r="AI13" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AK13" s="3" t="s">
         <v>59</v>
@@ -3708,7 +3712,7 @@
       </c>
       <c r="AN13" s="3"/>
       <c r="AO13" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="AP13" s="3">
         <v>888</v>
@@ -3720,19 +3724,19 @@
         <v>888</v>
       </c>
       <c r="AS13" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT13" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AU13" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="AV13" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AW13" s="7" t="s">
-        <v>274</v>
+        <v>370</v>
+      </c>
+      <c r="AW13" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="AX13" s="5"/>
       <c r="AZ13"/>
@@ -3743,138 +3747,138 @@
       <c r="A14" s="2">
         <v>22</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="B14" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C14" s="7">
         <v>2018</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>357</v>
+      <c r="D14" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>349</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="7">
         <v>78</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M14" s="2">
         <v>7</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="O14" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="P14" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="R14" s="9" t="s">
+      <c r="O14" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="R14" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="V14" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="X14" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="Z14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>888</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>888</v>
+      </c>
+      <c r="AC14" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="AD14" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE14" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="AJ14" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="S14" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="T14" s="9" t="s">
+      <c r="AK14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="AL14" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="AM14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="AN14" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="AP14" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="AQ14" s="7">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="AT14" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="U14" s="9" t="s">
+      <c r="AU14" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="V14" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="W14" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="X14" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="Y14" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="Z14" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="AA14" s="9">
-        <v>888</v>
-      </c>
-      <c r="AB14" s="3">
-        <v>888</v>
-      </c>
-      <c r="AC14" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="AD14" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="AE14" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="AF14" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="AG14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH14" s="2"/>
-      <c r="AI14" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="AJ14" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="AK14" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="AL14" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="AM14" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="AN14" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="AP14" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="AQ14" s="9">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="AT14" s="9" t="s">
+      <c r="AV14" s="7" t="s">
         <v>341</v>
-      </c>
-      <c r="AU14" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="AV14" s="9" t="s">
-        <v>349</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -3887,70 +3891,70 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3">
+        <v>888</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="3">
-        <v>888</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="I15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="K15" s="3" t="s">
         <v>59</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="P15" s="13" t="s">
-        <v>344</v>
+        <v>196</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>336</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="V15" s="3">
         <v>888</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="X15" s="3" t="s">
         <v>59</v>
@@ -3978,14 +3982,14 @@
         <v>67</v>
       </c>
       <c r="AG15" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AH15" s="5"/>
       <c r="AI15" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ15" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AK15" s="3" t="s">
         <v>59</v>
@@ -3998,7 +4002,7 @@
       </c>
       <c r="AN15" s="3"/>
       <c r="AO15" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AP15" s="3">
         <v>888</v>
@@ -4011,19 +4015,19 @@
       </c>
       <c r="AS15" s="5"/>
       <c r="AT15" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AU15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AV15" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="AW15" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AV15" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AW15" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="AX15" s="5" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="AZ15"/>
       <c r="BA15"/>
@@ -4034,52 +4038,52 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3">
+        <v>888</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="3">
-        <v>888</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="I16" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="K16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="M16" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="P16" s="13" t="s">
-        <v>377</v>
+        <v>136</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>368</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>63</v>
@@ -4088,16 +4092,16 @@
         <v>888</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="V16" s="3">
         <v>888</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>67</v>
@@ -4125,14 +4129,14 @@
         <v>67</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AH16" s="5"/>
       <c r="AI16" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ16" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="AK16" s="3" t="s">
         <v>59</v>
@@ -4145,7 +4149,7 @@
       </c>
       <c r="AN16" s="3"/>
       <c r="AO16" s="5" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="AP16" s="3">
         <v>888</v>
@@ -4158,17 +4162,17 @@
       </c>
       <c r="AS16" s="5"/>
       <c r="AT16" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AU16" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AV16" s="5" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="AW16" s="5"/>
       <c r="AX16" s="5" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="AZ16"/>
       <c r="BA16"/>
@@ -4179,52 +4183,52 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="F17" s="3">
+        <v>888</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="3">
-        <v>888</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="I17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="K17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="O17" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="P17" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>368</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="P17" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="Q17" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R17" s="3" t="s">
         <v>63</v>
@@ -4236,13 +4240,13 @@
         <v>64</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="V17" s="3">
         <v>888</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>59</v>
@@ -4272,10 +4276,10 @@
       <c r="AG17" s="3"/>
       <c r="AH17" s="5"/>
       <c r="AI17" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ17" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AK17" s="3" t="s">
         <v>59</v>
@@ -4288,7 +4292,7 @@
       </c>
       <c r="AN17" s="3"/>
       <c r="AO17" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AP17" s="3">
         <v>888</v>
@@ -4301,19 +4305,19 @@
       </c>
       <c r="AS17" s="5"/>
       <c r="AT17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AU17" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AW17" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="AW17" s="7" t="s">
-        <v>160</v>
-      </c>
       <c r="AX17" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AZ17"/>
       <c r="BA17"/>
@@ -4324,49 +4328,49 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="F18" s="3">
+        <v>888</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F18" s="3">
-        <v>888</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="I18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="K18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="M18" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="O18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="P18" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>62</v>
@@ -4381,13 +4385,13 @@
         <v>64</v>
       </c>
       <c r="U18" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V18" s="3">
         <v>888</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="X18" s="3" t="s">
         <v>59</v>
@@ -4419,10 +4423,10 @@
       </c>
       <c r="AH18" s="5"/>
       <c r="AI18" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ18" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AK18" s="3" t="s">
         <v>59</v>
@@ -4445,18 +4449,18 @@
         <v>888</v>
       </c>
       <c r="AS18" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT18" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AU18" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AV18" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="AW18" s="7"/>
+        <v>356</v>
+      </c>
+      <c r="AW18" s="6"/>
       <c r="AX18" s="5"/>
       <c r="AZ18"/>
       <c r="BA18"/>
@@ -4467,70 +4471,70 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="F19" s="3">
+        <v>888</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F19" s="3">
-        <v>888</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="I19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="K19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="N19" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="M19" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="O19" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q19" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="Q19" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="R19" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="S19" s="6">
-        <v>43499</v>
+        <v>90</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>335</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="V19" s="3">
         <v>888</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="X19" s="3" t="s">
         <v>59</v>
@@ -4543,7 +4547,7 @@
       </c>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AC19" s="3" t="s">
         <v>59</v>
@@ -4558,14 +4562,14 @@
         <v>67</v>
       </c>
       <c r="AG19" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AH19" s="5"/>
       <c r="AI19" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AJ19" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AK19" s="3" t="s">
         <v>67</v>
@@ -4588,19 +4592,19 @@
         <v>888</v>
       </c>
       <c r="AS19" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT19" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AU19" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV19" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="AW19" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
+      </c>
+      <c r="AW19" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="AX19" s="5"/>
       <c r="AZ19"/>
@@ -4612,70 +4616,70 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="F20" s="3">
+        <v>888</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F20" s="3">
-        <v>888</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="I20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="K20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>371</v>
+      <c r="M20" s="10" t="s">
+        <v>362</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U20" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="V20" s="3">
         <v>888</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>59</v>
@@ -4707,10 +4711,10 @@
       </c>
       <c r="AH20" s="5"/>
       <c r="AI20" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AJ20" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AK20" s="3" t="s">
         <v>67</v>
@@ -4723,7 +4727,7 @@
       </c>
       <c r="AN20" s="3"/>
       <c r="AO20" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="AP20" s="3">
         <v>888</v>
@@ -4735,18 +4739,18 @@
         <v>888</v>
       </c>
       <c r="AS20" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT20" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU20" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV20" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="AU20" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="AV20" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="AW20" s="7"/>
+      <c r="AW20" s="6"/>
       <c r="AX20" s="5"/>
       <c r="AZ20"/>
       <c r="BA20"/>
@@ -4757,70 +4761,70 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="3">
+        <v>888</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="H21" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="F21" s="3">
-        <v>888</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="K21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="N21" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="O21" s="5">
         <v>93.4</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="S21" s="8">
-        <v>43531</v>
+      <c r="S21" s="10" t="s">
+        <v>381</v>
       </c>
       <c r="T21" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="V21" s="3">
         <v>888</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>59</v>
@@ -4850,10 +4854,10 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="5"/>
       <c r="AI21" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AJ21" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AK21" s="3" t="s">
         <v>59</v>
@@ -4866,34 +4870,34 @@
       </c>
       <c r="AN21" s="3"/>
       <c r="AO21" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="AP21" s="3">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="3">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="3">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="AT21" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="AU21" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AV21" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="AW21" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AX21" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="AP21" s="3">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="3">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="3">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AT21" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AU21" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="AV21" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="AW21" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="AX21" s="5" t="s">
-        <v>220</v>
       </c>
       <c r="AZ21"/>
       <c r="BA21"/>
@@ -4904,40 +4908,40 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="F22" s="3">
+        <v>888</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="I22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L22" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="F22" s="3">
-        <v>888</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>373</v>
+      <c r="M22" s="10" t="s">
+        <v>364</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>60</v>
@@ -4946,28 +4950,28 @@
         <v>25</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="T22" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="V22" s="3">
         <v>888</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="X22" s="3">
         <v>888</v>
@@ -4983,10 +4987,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AD22" s="3" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AE22" s="3" t="s">
         <v>67</v>
@@ -4995,7 +4999,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="3" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="AH22" s="5"/>
       <c r="AI22" s="3">
@@ -5025,22 +5029,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AT22" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AU22" s="3" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="AV22" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="AW22" s="7" t="s">
-        <v>379</v>
+        <v>370</v>
+      </c>
+      <c r="AW22" s="6" t="s">
+        <v>370</v>
       </c>
       <c r="AX22" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22"/>

</xml_diff>

<commit_message>
Fix number of authors
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="896" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDD6F8C6-6186-1E44-806D-BCB36B2107F1}"/>
+  <xr:revisionPtr revIDLastSave="901" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F471066F-D0F0-554C-8227-D124E1C65CA7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,9 +524,6 @@
     <t xml:space="preserve">The authors were interested in comparing the effects of two interventions focused on different skills and some of the results were of the interaction. The results for the pretest-posttest alone were not always provided. </t>
   </si>
   <si>
-    <t>Rosas</t>
-  </si>
-  <si>
     <t>Impact of a computer-based intervention in
 Chilean children at risk of manifesting reading
 difficulties</t>
@@ -666,9 +663,6 @@
     <t>All the parent's variables were integrated into a composite score. Specific p-values were reported for nonsignificant results</t>
   </si>
   <si>
-    <t>Solheim</t>
-  </si>
-  <si>
     <t>Effectiveness of an early reading intervention in a semi-transparent orthography: A group randomised controlled trial</t>
   </si>
   <si>
@@ -1204,6 +1198,12 @@
   </si>
   <si>
     <t>3 - 7</t>
+  </si>
+  <si>
+    <t>Rosas et al</t>
+  </si>
+  <si>
+    <t>Solheim et al</t>
   </si>
 </sst>
 </file>
@@ -1445,7 +1445,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX22" totalsRowShown="0" headerRowDxfId="50">
-  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}"/>
+  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Chai"/>
+        <filter val="Rosas"/>
+        <filter val="Solheim"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX22">
     <sortCondition ref="B1:B22"/>
   </sortState>
@@ -1834,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="AV2" sqref="AV2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="133" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2007,7 +2015,7 @@
       <c r="BA1"/>
       <c r="BB1"/>
     </row>
-    <row r="2" spans="1:54" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>7</v>
       </c>
@@ -2030,7 +2038,7 @@
         <v>57</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>67</v>
@@ -2042,19 +2050,19 @@
         <v>67</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="Q2" s="5">
         <v>5</v>
@@ -2140,17 +2148,17 @@
         <v>71</v>
       </c>
       <c r="AV2" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="AW2" s="6"/>
       <c r="AX2" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="AZ2"/>
       <c r="BA2"/>
       <c r="BB2"/>
     </row>
-    <row r="3" spans="1:54" ht="380" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="380" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -2185,16 +2193,16 @@
         <v>67</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>151</v>
@@ -2224,7 +2232,7 @@
         <v>888</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="Z3" s="3">
         <v>888</v>
@@ -2234,7 +2242,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AD3" s="3" t="s">
         <v>67</v>
@@ -2246,7 +2254,7 @@
         <v>888</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AH3" s="5" t="s">
         <v>82</v>
@@ -2284,10 +2292,10 @@
         <v>76</v>
       </c>
       <c r="AU3" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV3" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AW3" s="6" t="s">
         <v>83</v>
@@ -2332,22 +2340,22 @@
         <v>67</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>89</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>90</v>
@@ -2381,22 +2389,22 @@
         <v>888</v>
       </c>
       <c r="AC4" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG4" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="AD4" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>352</v>
-      </c>
       <c r="AH4" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AI4" s="3">
         <v>888</v>
@@ -2427,16 +2435,16 @@
         <v>888</v>
       </c>
       <c r="AS4" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV4" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AW4" s="6" t="s">
         <v>94</v>
@@ -2448,7 +2456,7 @@
       <c r="BA4"/>
       <c r="BB4"/>
     </row>
-    <row r="5" spans="1:54" ht="208" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -2486,7 +2494,7 @@
         <v>103</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>60</v>
@@ -2574,7 +2582,7 @@
         <v>888</v>
       </c>
       <c r="AS5" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT5" s="3" t="s">
         <v>111</v>
@@ -2583,7 +2591,7 @@
         <v>112</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="AW5" s="6"/>
       <c r="AX5" s="5"/>
@@ -2591,51 +2599,51 @@
       <c r="BA5"/>
       <c r="BB5"/>
     </row>
-    <row r="6" spans="1:54" ht="128" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="128" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="3">
+        <v>888</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="F6" s="3">
-        <v>888</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="I6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="K6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>150</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>151</v>
@@ -2647,19 +2655,19 @@
         <v>63</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="V6" s="3">
         <v>888</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="X6" s="3" t="s">
         <v>59</v>
@@ -2691,10 +2699,10 @@
       </c>
       <c r="AH6" s="5"/>
       <c r="AI6" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK6" s="3" t="s">
         <v>59</v>
@@ -2718,13 +2726,13 @@
       </c>
       <c r="AS6" s="5"/>
       <c r="AT6" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AU6" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="AW6" s="6"/>
       <c r="AX6" s="5"/>
@@ -2732,36 +2740,36 @@
       <c r="BA6"/>
       <c r="BB6"/>
     </row>
-    <row r="7" spans="1:54" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="3">
+        <v>888</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F7" s="3">
-        <v>888</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>244</v>
-      </c>
       <c r="I7" s="5" t="s">
         <v>67</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>67</v>
@@ -2770,7 +2778,7 @@
         <v>78</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>150</v>
@@ -2785,22 +2793,22 @@
         <v>106</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T7" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="V7" s="3">
         <v>888</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="X7" s="3" t="s">
         <v>59</v>
@@ -2832,10 +2840,10 @@
       </c>
       <c r="AH7" s="5"/>
       <c r="AI7" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK7" s="3" t="s">
         <v>59</v>
@@ -2859,67 +2867,67 @@
       </c>
       <c r="AS7" s="5"/>
       <c r="AT7" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AU7" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV7" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="AW7" s="6"/>
       <c r="AX7" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AZ7"/>
       <c r="BA7"/>
       <c r="BB7"/>
     </row>
-    <row r="8" spans="1:54" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="3">
+        <v>888</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="F8" s="3">
-        <v>888</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="I8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>253</v>
-      </c>
       <c r="K8" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>150</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>151</v>
@@ -2928,22 +2936,22 @@
         <v>106</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T8" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="V8" s="3">
         <v>888</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="X8" s="3" t="s">
         <v>67</v>
@@ -2975,10 +2983,10 @@
       </c>
       <c r="AH8" s="5"/>
       <c r="AI8" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK8" s="3" t="s">
         <v>59</v>
@@ -3002,91 +3010,91 @@
       </c>
       <c r="AS8" s="5"/>
       <c r="AT8" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU8" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV8" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="AW8" s="6"/>
       <c r="AX8" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AZ8"/>
       <c r="BA8"/>
       <c r="BB8"/>
     </row>
-    <row r="9" spans="1:54" ht="112" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="112" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="F9" s="3">
+        <v>888</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="F9" s="3">
-        <v>888</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="I9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="K9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="N9" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="O9" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>62</v>
       </c>
       <c r="Q9" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="V9" s="3">
         <v>888</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="X9" s="3">
         <v>888</v>
@@ -3117,13 +3125,13 @@
         <v>67</v>
       </c>
       <c r="AH9" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK9" s="3" t="s">
         <v>59</v>
@@ -3136,7 +3144,7 @@
       </c>
       <c r="AN9" s="3"/>
       <c r="AO9" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AP9" s="3">
         <v>888</v>
@@ -3149,52 +3157,52 @@
       </c>
       <c r="AS9" s="5"/>
       <c r="AT9" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="AU9" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV9" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="AW9" s="6"/>
       <c r="AX9" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AZ9"/>
       <c r="BA9"/>
       <c r="BB9"/>
     </row>
-    <row r="10" spans="1:54" ht="160" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>144</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F10" s="3">
+        <v>888</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="F10" s="3">
-        <v>888</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="I10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>303</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>67</v>
@@ -3203,37 +3211,37 @@
         <v>78</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>134</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="V10" s="3">
         <v>888</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="X10" s="3" t="s">
         <v>59</v>
@@ -3263,10 +3271,10 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="5"/>
       <c r="AI10" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK10" s="3" t="s">
         <v>67</v>
@@ -3290,13 +3298,13 @@
       </c>
       <c r="AS10" s="5"/>
       <c r="AT10" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV10" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="AW10" s="6"/>
       <c r="AX10" s="5"/>
@@ -3304,54 +3312,54 @@
       <c r="BA10"/>
       <c r="BB10"/>
     </row>
-    <row r="11" spans="1:54" ht="96" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="3">
+        <v>888</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="F11" s="3">
-        <v>888</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="I11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>315</v>
-      </c>
       <c r="K11" s="3" t="s">
         <v>67</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Q11" s="5" t="s">
         <v>62</v>
@@ -3360,19 +3368,19 @@
         <v>63</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T11" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="V11" s="3">
         <v>888</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>67</v>
@@ -3388,7 +3396,7 @@
         <v>888</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AD11" s="3" t="s">
         <v>59</v>
@@ -3404,10 +3412,10 @@
       </c>
       <c r="AH11" s="5"/>
       <c r="AI11" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK11" s="3" t="s">
         <v>59</v>
@@ -3431,13 +3439,13 @@
       </c>
       <c r="AS11" s="5"/>
       <c r="AT11" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV11" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="AW11" s="6"/>
       <c r="AX11" s="5"/>
@@ -3445,36 +3453,36 @@
       <c r="BA11"/>
       <c r="BB11"/>
     </row>
-    <row r="12" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" s="3">
+        <v>888</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="F12" s="3">
-        <v>888</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="I12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>67</v>
@@ -3489,7 +3497,7 @@
         <v>150</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>151</v>
@@ -3501,19 +3509,19 @@
         <v>90</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="V12" s="3">
         <v>888</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="X12" s="3" t="s">
         <v>67</v>
@@ -3544,13 +3552,13 @@
         <v>888</v>
       </c>
       <c r="AH12" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK12" s="3" t="s">
         <v>59</v>
@@ -3563,69 +3571,69 @@
       </c>
       <c r="AN12" s="3"/>
       <c r="AO12" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>888</v>
+      </c>
+      <c r="AQ12" s="3">
+        <v>888</v>
+      </c>
+      <c r="AR12" s="3">
+        <v>888</v>
+      </c>
+      <c r="AS12" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="AV12" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AW12" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="AX12" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="AP12" s="3">
-        <v>888</v>
-      </c>
-      <c r="AQ12" s="3">
-        <v>888</v>
-      </c>
-      <c r="AR12" s="3">
-        <v>888</v>
-      </c>
-      <c r="AS12" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="AT12" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="AU12" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AV12" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="AW12" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="AX12" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="AZ12"/>
       <c r="BA12"/>
       <c r="BB12"/>
     </row>
-    <row r="13" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="F13" s="3">
+        <v>888</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F13" s="3">
-        <v>888</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="I13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>263</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>67</v>
@@ -3634,16 +3642,16 @@
         <v>78</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q13" s="5" t="s">
         <v>62</v>
@@ -3652,19 +3660,19 @@
         <v>90</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="V13" s="3">
         <v>888</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>67</v>
@@ -3677,7 +3685,7 @@
       </c>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AC13" s="3" t="s">
         <v>59</v>
@@ -3712,7 +3720,7 @@
       </c>
       <c r="AN13" s="3"/>
       <c r="AO13" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AP13" s="3">
         <v>888</v>
@@ -3724,49 +3732,49 @@
         <v>888</v>
       </c>
       <c r="AS13" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT13" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AU13" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AV13" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AW13" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AX13" s="5"/>
       <c r="AZ13"/>
       <c r="BA13"/>
       <c r="BB13"/>
     </row>
-    <row r="14" spans="1:54" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>22</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C14" s="7">
         <v>2018</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>323</v>
-      </c>
       <c r="H14" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>67</v>
@@ -3778,7 +3786,7 @@
         <v>67</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M14" s="2">
         <v>7</v>
@@ -3787,40 +3795,40 @@
         <v>60</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q14" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="R14" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="U14" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="S14" s="9" t="s">
-        <v>335</v>
-      </c>
-      <c r="T14" s="7" t="s">
+      <c r="V14" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="U14" s="7" t="s">
+      <c r="W14" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="V14" s="8" t="s">
+      <c r="X14" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="W14" s="7" t="s">
+      <c r="Y14" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="X14" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y14" s="7" t="s">
-        <v>330</v>
-      </c>
       <c r="Z14" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AA14" s="7">
         <v>888</v>
@@ -3829,56 +3837,56 @@
         <v>888</v>
       </c>
       <c r="AC14" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AD14" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AE14" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AF14" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AG14" s="3" t="s">
         <v>67</v>
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="AJ14" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="AK14" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="AL14" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="AM14" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="AN14" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="AP14" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="AQ14" s="7">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="AT14" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="AJ14" s="7" t="s">
+      <c r="AU14" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="AK14" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="AL14" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="AM14" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="AN14" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="AP14" s="7" t="s">
+      <c r="AV14" s="7" t="s">
         <v>339</v>
-      </c>
-      <c r="AQ14" s="7">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="AT14" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="AU14" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV14" s="7" t="s">
-        <v>341</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -3886,7 +3894,7 @@
       <c r="BA14"/>
       <c r="BB14"/>
     </row>
-    <row r="15" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -3924,16 +3932,16 @@
         <v>106</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>120</v>
@@ -3942,7 +3950,7 @@
         <v>90</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T15" s="3" t="s">
         <v>64</v>
@@ -4015,25 +4023,25 @@
       </c>
       <c r="AS15" s="5"/>
       <c r="AT15" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AU15" s="3" t="s">
         <v>125</v>
       </c>
       <c r="AV15" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AW15" s="6" t="s">
         <v>127</v>
       </c>
       <c r="AX15" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AZ15"/>
       <c r="BA15"/>
       <c r="BB15"/>
     </row>
-    <row r="16" spans="1:54" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -4059,7 +4067,7 @@
         <v>133</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>134</v>
@@ -4071,7 +4079,7 @@
         <v>135</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>60</v>
@@ -4080,10 +4088,10 @@
         <v>136</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>63</v>
@@ -4149,7 +4157,7 @@
       </c>
       <c r="AN16" s="3"/>
       <c r="AO16" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="AP16" s="3">
         <v>888</v>
@@ -4168,17 +4176,17 @@
         <v>142</v>
       </c>
       <c r="AV16" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="AW16" s="5"/>
       <c r="AX16" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="AZ16"/>
       <c r="BA16"/>
       <c r="BB16"/>
     </row>
-    <row r="17" spans="1:54" ht="240" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -4213,7 +4221,7 @@
         <v>67</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>89</v>
@@ -4222,7 +4230,7 @@
         <v>150</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P17" s="5" t="s">
         <v>151</v>
@@ -4308,7 +4316,7 @@
         <v>155</v>
       </c>
       <c r="AU17" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV17" s="5" t="s">
         <v>156</v>
@@ -4328,46 +4336,46 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>160</v>
+        <v>380</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="3">
+        <v>888</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F18" s="3">
-        <v>888</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="P18" s="5" t="s">
         <v>151</v>
@@ -4385,13 +4393,13 @@
         <v>64</v>
       </c>
       <c r="U18" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="V18" s="3">
+        <v>888</v>
+      </c>
+      <c r="W18" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="V18" s="3">
-        <v>888</v>
-      </c>
-      <c r="W18" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="X18" s="3" t="s">
         <v>59</v>
@@ -4449,16 +4457,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT18" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AU18" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="AU18" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="AV18" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AW18" s="6"/>
       <c r="AX18" s="5"/>
@@ -4466,51 +4474,51 @@
       <c r="BA18"/>
       <c r="BB18"/>
     </row>
-    <row r="19" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="3">
+        <v>888</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F19" s="3">
-        <v>888</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="M19" s="5" t="s">
+      <c r="N19" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="N19" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="O19" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P19" s="5" t="s">
         <v>104</v>
@@ -4522,19 +4530,19 @@
         <v>90</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="T19" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V19" s="3">
         <v>888</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="X19" s="3" t="s">
         <v>59</v>
@@ -4547,29 +4555,29 @@
       </c>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG19" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="AC19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG19" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="AH19" s="5"/>
       <c r="AI19" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AJ19" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AK19" s="3" t="s">
         <v>67</v>
@@ -4592,94 +4600,94 @@
         <v>888</v>
       </c>
       <c r="AS19" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT19" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AU19" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV19" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="AW19" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="AW19" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="AX19" s="5"/>
       <c r="AZ19"/>
       <c r="BA19"/>
       <c r="BB19"/>
     </row>
-    <row r="20" spans="1:54" ht="144" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" ht="144" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="3">
+        <v>888</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F20" s="3">
-        <v>888</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="M20" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>60</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T20" s="3" t="s">
         <v>113</v>
       </c>
       <c r="U20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="V20" s="3">
+        <v>888</v>
+      </c>
+      <c r="W20" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="V20" s="3">
-        <v>888</v>
-      </c>
-      <c r="W20" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>59</v>
@@ -4714,7 +4722,7 @@
         <v>109</v>
       </c>
       <c r="AJ20" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AK20" s="3" t="s">
         <v>67</v>
@@ -4727,7 +4735,7 @@
       </c>
       <c r="AN20" s="3"/>
       <c r="AO20" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AP20" s="3">
         <v>888</v>
@@ -4739,16 +4747,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT20" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU20" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="AU20" s="3" t="s">
+      <c r="AV20" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="AV20" s="5" t="s">
-        <v>202</v>
       </c>
       <c r="AW20" s="6"/>
       <c r="AX20" s="5"/>
@@ -4761,49 +4769,49 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="3">
+        <v>888</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="H21" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="F21" s="3">
-        <v>888</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="K21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="N21" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>209</v>
       </c>
       <c r="O21" s="5">
         <v>93.4</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>106</v>
@@ -4812,19 +4820,19 @@
         <v>63</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="T21" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="V21" s="3">
         <v>888</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>59</v>
@@ -4854,10 +4862,10 @@
       <c r="AG21" s="3"/>
       <c r="AH21" s="5"/>
       <c r="AI21" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AJ21" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AK21" s="3" t="s">
         <v>59</v>
@@ -4870,63 +4878,63 @@
       </c>
       <c r="AN21" s="3"/>
       <c r="AO21" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP21" s="3">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="3">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="3">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="AT21" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="AU21" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="AV21" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="AW21" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="AX21" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="AP21" s="3">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="3">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="3">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="AT21" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AU21" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="AV21" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="AW21" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="AX21" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="AZ21"/>
       <c r="BA21"/>
       <c r="BB21"/>
     </row>
-    <row r="22" spans="1:54" ht="96" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="F22" s="3">
+        <v>888</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="F22" s="3">
-        <v>888</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>235</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>67</v>
@@ -4938,10 +4946,10 @@
         <v>67</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>60</v>
@@ -4950,7 +4958,7 @@
         <v>25</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q22" s="5" t="s">
         <v>79</v>
@@ -4965,13 +4973,13 @@
         <v>64</v>
       </c>
       <c r="U22" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="V22" s="3">
         <v>888</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="X22" s="3">
         <v>888</v>
@@ -4987,10 +4995,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AD22" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AE22" s="3" t="s">
         <v>67</v>
@@ -4999,7 +5007,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AH22" s="5"/>
       <c r="AI22" s="3">
@@ -5029,22 +5037,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AT22" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AU22" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AV22" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AW22" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AX22" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22"/>

</xml_diff>

<commit_message>
Recoded session numbers and language
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1137" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77C0E3AE-4625-7641-8383-81CCA887FD5F}"/>
+  <xr:revisionPtr revIDLastSave="1173" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C46E064C-4F78-6942-9654-072F07A8596A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="387">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -278,9 +278,6 @@
     <t>K - 2</t>
   </si>
   <si>
-    <t>40 lessons (not necessarily sessions)</t>
-  </si>
-  <si>
     <t>Funnix and Headsprout</t>
   </si>
   <si>
@@ -639,9 +636,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>English, though they spoke Mandarin (you need to confirm this).</t>
-  </si>
-  <si>
     <t>PhonoBlocks</t>
   </si>
   <si>
@@ -658,9 +652,6 @@
   </si>
   <si>
     <t xml:space="preserve">The data was presented in narrative (didn't use tables). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">El total de sesiones que ellos reportan (8) no cuadra con la cantidad de sesiones por semana y el total de semanas de intervención (que reportan). No sé si es un error de ellos, pero dice que fueron 8 sesiones en total, de 3 a 4 veces por semanas, por un total de 3 semanas. </t>
   </si>
   <si>
     <t>Kleinsz et al</t>
@@ -814,9 +805,6 @@
     <t>d = .27 - .97</t>
   </si>
   <si>
-    <t>Very little control over the number of sessions, frequency, and duration, which were not specified</t>
-  </si>
-  <si>
     <t>The p-values and effect sizes were only provided for some outcomes</t>
   </si>
   <si>
@@ -875,9 +863,6 @@
   </si>
   <si>
     <t>5 - 6</t>
-  </si>
-  <si>
-    <t>Maximum = 60</t>
   </si>
   <si>
     <t>20 - 30</t>
@@ -1234,6 +1219,15 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>El total de sesiones que ellos reportan (8) no cuadra con la cantidad de sesiones por semana y el total de semanas de intervención (que reportan). No sé si es un error de ellos, pero dice que fueron 8 sesiones en total, de 3 a 4 veces por semanas, por un total de 3 semanas. Participants were native mandarin speakers.</t>
+  </si>
+  <si>
+    <t>Very little control over the number of sessions, frequency, and duration, which were not specified. Not necessarily sessions; more like tutorials/lessons</t>
+  </si>
+  <si>
+    <t>60 lessons were the maximum number of sessions</t>
   </si>
 </sst>
 </file>
@@ -2509,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="K16" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2539,151 +2533,151 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AE1" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AL1" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="AR1" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>336</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
@@ -2700,7 +2694,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2712,10 +2706,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>15</v>
@@ -2727,19 +2721,19 @@
         <v>15</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2751,7 +2745,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>13</v>
@@ -2763,7 +2757,7 @@
         <v>14</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>15</v>
@@ -2775,13 +2769,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>15</v>
@@ -2797,13 +2791,13 @@
         <v>17</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2824,11 +2818,11 @@
         <v>19</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
@@ -2854,13 +2848,13 @@
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>15</v>
@@ -2872,19 +2866,19 @@
         <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R3" s="7" t="s">
         <v>27</v>
@@ -2896,7 +2890,7 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>28</v>
@@ -2911,7 +2905,7 @@
         <v>888</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AA3" s="5">
         <v>888</v>
@@ -2920,7 +2914,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>15</v>
@@ -2932,7 +2926,7 @@
         <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="AH3" s="7" t="s">
         <v>30</v>
@@ -2970,10 +2964,10 @@
         <v>24</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AW3" s="9" t="s">
         <v>31</v>
@@ -2997,19 +2991,19 @@
         <v>33</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F4" s="5">
         <v>888</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>15</v>
@@ -3021,22 +3015,22 @@
         <v>15</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>35</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>36</v>
@@ -3045,7 +3039,7 @@
         <v>27</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>37</v>
@@ -3054,7 +3048,7 @@
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>15</v>
@@ -3069,10 +3063,10 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE4" s="5" t="s">
         <v>15</v>
@@ -3081,10 +3075,10 @@
         <v>888</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3103,7 +3097,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3115,16 +3109,16 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AW4" s="9" t="s">
         <v>38</v>
@@ -3150,19 +3144,19 @@
         <v>42</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F5" s="5">
         <v>888</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>15</v>
@@ -3174,10 +3168,10 @@
         <v>15</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
@@ -3198,7 +3192,7 @@
         <v>47</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>48</v>
@@ -3210,10 +3204,10 @@
         <v>49</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3222,13 +3216,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>15</v>
@@ -3244,13 +3238,13 @@
         <v>51</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3264,7 +3258,7 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT5" s="5" t="s">
         <v>52</v>
@@ -3273,7 +3267,7 @@
         <v>53</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3286,52 +3280,52 @@
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="F6" s="5">
+        <v>888</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="F6" s="5">
-        <v>888</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="Q6" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>11</v>
@@ -3340,40 +3334,40 @@
         <v>12</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="W6" s="5">
+        <v>888</v>
+      </c>
+      <c r="X6" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="W6" s="5">
-        <v>888</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="Y6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>15</v>
@@ -3383,16 +3377,16 @@
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>15</v>
@@ -3410,13 +3404,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3429,34 +3423,34 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>15</v>
@@ -3465,40 +3459,40 @@
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R7" s="7" t="s">
         <v>47</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U7" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="V7" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="V7" s="5" t="s">
-        <v>344</v>
-      </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>15</v>
@@ -3510,10 +3504,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>15</v>
@@ -3526,16 +3520,16 @@
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>15</v>
@@ -3553,17 +3547,17 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
@@ -3574,74 +3568,74 @@
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="5">
+        <v>888</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F8" s="5">
-        <v>888</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="L8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q8" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>47</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V8" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="W8" s="5">
+        <v>888</v>
+      </c>
+      <c r="X8" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="W8" s="5">
-        <v>888</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="Y8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3649,19 +3643,19 @@
         <v>15</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>15</v>
@@ -3671,16 +3665,16 @@
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>15</v>
@@ -3698,17 +3692,17 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
@@ -3719,122 +3713,122 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="O9" s="5" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V9" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="W9" s="5">
+        <v>888</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="AI9" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="W9" s="5">
-        <v>888</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH9" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="AJ9" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3847,17 +3841,17 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>199</v>
+        <v>384</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
@@ -3868,34 +3862,34 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F10" s="5">
+        <v>888</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="F10" s="5">
-        <v>888</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>15</v>
@@ -3904,75 +3898,75 @@
         <v>26</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="P10" s="7" t="s">
         <v>71</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>15</v>
@@ -3990,13 +3984,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -4009,52 +4003,52 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F11" s="5">
+        <v>888</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="F11" s="5">
-        <v>888</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>224</v>
-      </c>
       <c r="L11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>11</v>
@@ -4063,19 +4057,19 @@
         <v>12</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="W11" s="5">
         <v>888</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>15</v>
@@ -4090,13 +4084,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>15</v>
@@ -4106,16 +4100,16 @@
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>15</v>
@@ -4133,17 +4127,17 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
@@ -4154,34 +4148,34 @@
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" s="5">
+        <v>888</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="F12" s="5">
-        <v>888</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>15</v>
@@ -4193,13 +4187,13 @@
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="R12" s="7" t="s">
         <v>47</v>
@@ -4208,19 +4202,19 @@
         <v>36</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="W12" s="5">
         <v>888</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>15</v>
@@ -4235,13 +4229,13 @@
         <v>888</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF12" s="4" t="s">
         <v>15</v>
@@ -4250,26 +4244,26 @@
         <v>888</v>
       </c>
       <c r="AH12" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AI12" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AP12" s="5">
         <v>888</v>
@@ -4281,22 +4275,22 @@
         <v>888</v>
       </c>
       <c r="AS12" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AU12" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="AW12" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="AV12" s="9" t="s">
+      <c r="AX12" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="AW12" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="AX12" s="7" t="s">
-        <v>213</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
@@ -4307,34 +4301,34 @@
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>176</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="F13" s="5">
         <v>888</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="H13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>15</v>
@@ -4343,16 +4337,16 @@
         <v>26</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P13" s="7" t="s">
-        <v>270</v>
+      <c r="P13" s="7">
+        <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>11</v>
@@ -4361,40 +4355,40 @@
         <v>36</v>
       </c>
       <c r="T13" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="V13" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="U13" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="V13" s="5" t="s">
+      <c r="W13" s="5">
+        <v>888</v>
+      </c>
+      <c r="X13" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="W13" s="5">
-        <v>888</v>
-      </c>
-      <c r="X13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB13" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="Y13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA13" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AB13" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="AC13" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>15</v>
@@ -4410,7 +4404,7 @@
         <v>62</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>15</v>
@@ -4420,33 +4414,35 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS13" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="AT13" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AU13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="AV13" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="AW13" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="AP13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS13" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="AT13" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="AU13" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="AV13" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="AW13" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="AX13" s="7"/>
+      <c r="AX13" s="7" t="s">
+        <v>386</v>
+      </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="6"/>
@@ -4456,28 +4452,28 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>15</v>
@@ -4489,7 +4485,7 @@
         <v>15</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4498,95 +4494,95 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="W14" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="U14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="Y14" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="X14" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="AA14" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="AB14" s="5">
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="AG14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="AT14" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AU14" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AJ14" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="AK14" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AN14" s="2" t="s">
+      <c r="AV14" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="AP14" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="AT14" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AU14" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4620,7 +4616,7 @@
         <v>58</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>15</v>
@@ -4629,22 +4625,22 @@
         <v>59</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
@@ -4653,10 +4649,10 @@
         <v>36</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V15" s="5" t="s">
         <v>60</v>
@@ -4665,28 +4661,28 @@
         <v>888</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AB15" s="5">
         <v>888</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF15" s="4" t="s">
         <v>15</v>
@@ -4702,7 +4698,7 @@
         <v>62</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>15</v>
@@ -4725,19 +4721,19 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AU15" s="5" t="s">
         <v>63</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AW15" s="9" t="s">
         <v>65</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
@@ -4763,16 +4759,16 @@
         <v>888</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>70</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>71</v>
@@ -4784,19 +4780,19 @@
         <v>72</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P16" s="5" t="s">
-        <v>73</v>
+      <c r="P16" s="5">
+        <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>12</v>
@@ -4805,63 +4801,63 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="V16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="W16" s="5">
+        <v>888</v>
+      </c>
+      <c r="X16" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="W16" s="5">
-        <v>888</v>
-      </c>
-      <c r="X16" s="5" t="s">
+      <c r="Y16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG16" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB16" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="5" t="s">
         <v>50</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4874,17 +4870,17 @@
       </c>
       <c r="AS16" s="7"/>
       <c r="AT16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU16" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AU16" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="AV16" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>249</v>
+        <v>385</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
@@ -4895,52 +4891,52 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="5">
+        <v>888</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="5">
-        <v>888</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="L17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>47</v>
@@ -4952,19 +4948,19 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="W17" s="5">
+        <v>888</v>
+      </c>
+      <c r="X17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="W17" s="5">
-        <v>888</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="Y17" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>15</v>
@@ -4993,20 +4989,20 @@
         <v>50</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -5019,19 +5015,19 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU17" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AV17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="AU17" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="AV17" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="AW17" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX17" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="AX17" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
@@ -5042,52 +5038,52 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="5">
+        <v>888</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="5">
-        <v>888</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="P18" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="P18" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="Q18" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R18" s="7" t="s">
         <v>11</v>
@@ -5099,37 +5095,37 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="W18" s="5">
+        <v>888</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="W18" s="5">
-        <v>888</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="Y18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>15</v>
@@ -5145,10 +5141,10 @@
         <v>62</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>15</v>
@@ -5165,16 +5161,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT18" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU18" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="AU18" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="AV18" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5187,49 +5183,49 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F19" s="5">
+        <v>888</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="F19" s="5">
-        <v>888</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="L19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="N19" s="7" t="s">
+      <c r="O19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="O19" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="P19" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q19" s="7" t="s">
         <v>45</v>
@@ -5241,59 +5237,59 @@
         <v>36</v>
       </c>
       <c r="T19" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W19" s="5">
         <v>888</v>
       </c>
       <c r="X19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="Y19" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AB19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>15</v>
@@ -5310,19 +5306,19 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
@@ -5334,76 +5330,76 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F20" s="5">
+        <v>888</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="F20" s="5">
-        <v>888</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="L20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="V20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="W20" s="5">
+        <v>888</v>
+      </c>
+      <c r="X20" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="W20" s="5">
-        <v>888</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="Y20" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>15</v>
@@ -5415,13 +5411,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>15</v>
@@ -5434,20 +5430,20 @@
         <v>50</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5459,16 +5455,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AU20" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AU20" s="5" t="s">
+      <c r="AV20" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="AV20" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5481,52 +5477,52 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F21" s="5">
+        <v>888</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="F21" s="5">
-        <v>888</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="L21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>47</v>
@@ -5535,22 +5531,22 @@
         <v>12</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>15</v>
@@ -5562,64 +5558,64 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AG21" s="5"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ21" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="AJ21" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="AK21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="AT21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="AU21" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AV21" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="AW21" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="AP21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="AT21" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="AU21" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="AV21" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="AW21" s="9" t="s">
+      <c r="AX21" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="AX21" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
@@ -5630,28 +5626,28 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>159</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>15</v>
@@ -5663,10 +5659,10 @@
         <v>15</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5675,7 +5671,7 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R22" s="7" t="s">
         <v>27</v>
@@ -5687,17 +5683,17 @@
         <v>26</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="V22" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="W22" s="5">
+        <v>888</v>
+      </c>
+      <c r="X22" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="W22" s="5">
-        <v>888</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>161</v>
-      </c>
       <c r="Y22" s="5">
         <v>888</v>
       </c>
@@ -5711,10 +5707,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>15</v>
@@ -5723,7 +5719,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5753,22 +5749,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AT22" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="AU22" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AV22" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="AX22" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="AU22" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="AV22" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="AW22" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="AX22" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>

</xml_diff>

<commit_message>
Recoded modality, how many by modality, supervision
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1173" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C46E064C-4F78-6942-9654-072F07A8596A}"/>
+  <xr:revisionPtr revIDLastSave="1184" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EBA09873-9B55-894F-8F82-C3603E888C5D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="384">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>13</t>
-  </si>
-  <si>
-    <t>Grupo</t>
   </si>
   <si>
     <t>Touch Sound</t>
@@ -600,9 +597,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>Not specified</t>
-  </si>
-  <si>
     <t>GraphoGame - Rime, GraphoGame - Rime,Phoneme</t>
   </si>
   <si>
@@ -922,9 +916,6 @@
     <t>Solheim et al</t>
   </si>
   <si>
-    <t>No Not supervised</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -1106,9 +1097,6 @@
     <t>PreK - K</t>
   </si>
   <si>
-    <t>No supervised</t>
-  </si>
-  <si>
     <t>Investigate the efficacy of an early reading intervention delivered alongside formal reading instruction to Norwegian 6-year old's to be at risk for RD at school entry through a group randomised controlled trial, with a two-year long term follow up after intervention.</t>
   </si>
   <si>
@@ -1228,6 +1216,9 @@
   </si>
   <si>
     <t>60 lessons were the maximum number of sessions</t>
+  </si>
+  <si>
+    <t>Not supervised</t>
   </si>
 </sst>
 </file>
@@ -2106,7 +2097,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX22" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}"/>
+  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}">
+    <filterColumn colId="20">
+      <filters>
+        <filter val="No Not supervised"/>
+        <filter val="No supervised"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX22">
     <sortCondition ref="B1:B22"/>
   </sortState>
@@ -2503,8 +2501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K16" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2533,157 +2531,157 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AJ1" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="AO1" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="AS1" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="AU1" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>331</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
       <c r="BB1" s="6"/>
     </row>
-    <row r="2" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>7</v>
       </c>
@@ -2694,7 +2692,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2706,10 +2704,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>15</v>
@@ -2721,19 +2719,19 @@
         <v>15</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2745,7 +2743,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>13</v>
@@ -2757,7 +2755,7 @@
         <v>14</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>15</v>
@@ -2769,13 +2767,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>15</v>
@@ -2791,13 +2789,13 @@
         <v>17</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2818,17 +2816,17 @@
         <v>19</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6"/>
     </row>
-    <row r="3" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -2848,13 +2846,13 @@
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>15</v>
@@ -2866,19 +2864,19 @@
         <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R3" s="7" t="s">
         <v>27</v>
@@ -2890,7 +2888,7 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>28</v>
@@ -2905,7 +2903,7 @@
         <v>888</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AA3" s="5">
         <v>888</v>
@@ -2914,7 +2912,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>15</v>
@@ -2926,7 +2924,7 @@
         <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AH3" s="7" t="s">
         <v>30</v>
@@ -2964,10 +2962,10 @@
         <v>24</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AW3" s="9" t="s">
         <v>31</v>
@@ -2977,7 +2975,7 @@
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
     </row>
-    <row r="4" spans="1:54" ht="372" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="372" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>9</v>
       </c>
@@ -2991,19 +2989,19 @@
         <v>33</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F4" s="5">
         <v>888</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>15</v>
@@ -3015,40 +3013,40 @@
         <v>15</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>35</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W4" s="5">
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>15</v>
@@ -3063,22 +3061,22 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG4" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="AD4" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>254</v>
-      </c>
       <c r="AH4" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3097,7 +3095,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3109,69 +3107,69 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AW4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX4" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="AX4" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6"/>
       <c r="BB4" s="6"/>
     </row>
-    <row r="5" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F5" s="5">
+        <v>888</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="F5" s="5">
-        <v>888</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
@@ -3180,34 +3178,34 @@
         <v>10</v>
       </c>
       <c r="Q5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" s="7" t="s">
+      <c r="U5" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="V5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="U5" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5">
+        <v>888</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="W5" s="5">
-        <v>888</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="Y5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3216,13 +3214,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>15</v>
@@ -3232,19 +3230,19 @@
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AJ5" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="AK5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3258,16 +3256,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AU5" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="AV5" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3275,57 +3273,57 @@
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
     </row>
-    <row r="6" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="F6" s="5">
+        <v>888</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="F6" s="5">
-        <v>888</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="Q6" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>11</v>
@@ -3334,40 +3332,40 @@
         <v>12</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V6" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="W6" s="5">
+        <v>888</v>
+      </c>
+      <c r="X6" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="W6" s="5">
-        <v>888</v>
-      </c>
-      <c r="X6" s="5" t="s">
-        <v>151</v>
-      </c>
       <c r="Y6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>15</v>
@@ -3377,16 +3375,16 @@
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>15</v>
@@ -3404,13 +3402,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3418,39 +3416,39 @@
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
     </row>
-    <row r="7" spans="1:54" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>164</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>15</v>
@@ -3459,40 +3457,40 @@
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>15</v>
@@ -3504,10 +3502,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>15</v>
@@ -3520,16 +3518,16 @@
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>15</v>
@@ -3547,95 +3545,95 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
     </row>
-    <row r="8" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F8" s="5">
+        <v>888</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="5">
-        <v>888</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="V8" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="V8" s="5" t="s">
+      <c r="W8" s="5">
+        <v>888</v>
+      </c>
+      <c r="X8" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="W8" s="5">
-        <v>888</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>172</v>
-      </c>
       <c r="Y8" s="5" t="s">
         <v>15</v>
       </c>
@@ -3643,19 +3641,19 @@
         <v>15</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>15</v>
@@ -3665,16 +3663,16 @@
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>15</v>
@@ -3692,143 +3690,143 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
     </row>
-    <row r="9" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>190</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V9" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="W9" s="5">
+        <v>888</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI9" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="W9" s="5">
-        <v>888</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH9" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="AJ9" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3841,55 +3839,55 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
     </row>
-    <row r="10" spans="1:54" ht="170" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" s="5">
+        <v>888</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="I10" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="F10" s="5">
-        <v>888</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>15</v>
@@ -3898,75 +3896,75 @@
         <v>26</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>15</v>
@@ -3984,13 +3982,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3998,57 +3996,57 @@
       <c r="BA10" s="6"/>
       <c r="BB10" s="6"/>
     </row>
-    <row r="11" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F11" s="5">
+        <v>888</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="I11" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="F11" s="5">
-        <v>888</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>221</v>
-      </c>
       <c r="L11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>11</v>
@@ -4057,19 +4055,19 @@
         <v>12</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="W11" s="5">
         <v>888</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>15</v>
@@ -4084,13 +4082,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>15</v>
@@ -4100,16 +4098,16 @@
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>15</v>
@@ -4127,55 +4125,55 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
       <c r="BB11" s="6"/>
     </row>
-    <row r="12" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" s="5">
+        <v>888</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="I12" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="F12" s="5">
-        <v>888</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>201</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>15</v>
@@ -4187,148 +4185,148 @@
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="P12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="R12" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V12" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="W12" s="5">
+        <v>888</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AH12" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="AI12" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="W12" s="5">
-        <v>888</v>
-      </c>
-      <c r="X12" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="Y12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC12" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AD12" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AE12" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AH12" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="AI12" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="AJ12" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS12" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW12" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX12" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="AP12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS12" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="AT12" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="AU12" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="AV12" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="AW12" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX12" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
       <c r="BB12" s="6"/>
     </row>
-    <row r="13" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F13" s="5">
         <v>888</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>15</v>
@@ -4337,7 +4335,7 @@
         <v>26</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4346,49 +4344,49 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="T13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="W13" s="5">
+        <v>888</v>
+      </c>
+      <c r="X13" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="U13" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="V13" s="5" t="s">
+      <c r="Y13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB13" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="W13" s="5">
-        <v>888</v>
-      </c>
-      <c r="X13" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA13" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AB13" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="AC13" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>15</v>
@@ -4398,13 +4396,13 @@
       </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>15</v>
@@ -4414,7 +4412,7 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AP13" s="5">
         <v>888</v>
@@ -4426,54 +4424,54 @@
         <v>888</v>
       </c>
       <c r="AS13" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT13" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AU13" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AV13" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AW13" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AX13" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="6"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>15</v>
@@ -4485,7 +4483,7 @@
         <v>15</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4494,95 +4492,95 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="V14" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="U14" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="Y14" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="Y14" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="AA14" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AB14" s="5">
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AG14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AT14" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AJ14" s="2" t="s">
+      <c r="AU14" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AK14" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="AN14" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="AP14" s="2" t="s">
+      <c r="AV14" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="AT14" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="AU14" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4590,115 +4588,115 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="5">
+        <v>888</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="5">
-        <v>888</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="L15" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="W15" s="5">
+        <v>888</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE15" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG15" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="W15" s="5">
-        <v>888</v>
-      </c>
-      <c r="X15" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y15" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA15" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AB15" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AD15" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG15" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>15</v>
@@ -4708,7 +4706,7 @@
       </c>
       <c r="AN15" s="5"/>
       <c r="AO15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AP15" s="5">
         <v>888</v>
@@ -4721,19 +4719,19 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AW15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
@@ -4744,43 +4742,43 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="5">
+        <v>888</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="5">
-        <v>888</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="N16" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
@@ -4789,10 +4787,10 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>12</v>
@@ -4801,63 +4799,63 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>285</v>
+        <v>383</v>
       </c>
       <c r="V16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="W16" s="5">
+        <v>888</v>
+      </c>
+      <c r="X16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="W16" s="5">
-        <v>888</v>
-      </c>
-      <c r="X16" s="5" t="s">
+      <c r="Y16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG16" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB16" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4870,76 +4868,76 @@
       </c>
       <c r="AS16" s="7"/>
       <c r="AT16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU16" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AU16" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="AV16" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="6"/>
     </row>
-    <row r="17" spans="1:54" ht="289" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" ht="289" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="5">
+        <v>888</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="5">
-        <v>888</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="L17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>35</v>
       </c>
       <c r="O17" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="P17" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="R17" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>12</v>
@@ -4948,19 +4946,19 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V17" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="W17" s="5">
+        <v>888</v>
+      </c>
+      <c r="X17" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="W17" s="5">
-        <v>888</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="Y17" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>15</v>
@@ -4986,23 +4984,23 @@
       <c r="AG17" s="5"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -5015,75 +5013,75 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AU17" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AV17" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="AU17" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="AV17" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="AW17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX17" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="AX17" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="5">
+        <v>888</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="5">
-        <v>888</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="P18" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="P18" s="7" t="s">
-        <v>102</v>
-      </c>
       <c r="Q18" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R18" s="7" t="s">
         <v>11</v>
@@ -5095,37 +5093,37 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="W18" s="5">
+        <v>888</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="W18" s="5">
-        <v>888</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="Y18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>15</v>
@@ -5135,16 +5133,16 @@
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>15</v>
@@ -5161,16 +5159,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AU18" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AU18" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="AV18" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5178,118 +5176,118 @@
       <c r="BA18" s="6"/>
       <c r="BB18" s="6"/>
     </row>
-    <row r="19" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F19" s="5">
+        <v>888</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="F19" s="5">
-        <v>888</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="L19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="N19" s="7" t="s">
+      <c r="O19" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="P19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="W19" s="5">
+        <v>888</v>
+      </c>
+      <c r="X19" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="P19" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T19" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="V19" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="W19" s="5">
-        <v>888</v>
-      </c>
-      <c r="X19" s="5" t="s">
+      <c r="Y19" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="Y19" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AB19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>15</v>
@@ -5306,19 +5304,19 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
@@ -5330,76 +5328,76 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F20" s="5">
+        <v>888</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="F20" s="5">
-        <v>888</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="L20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>346</v>
+        <v>383</v>
       </c>
       <c r="V20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="W20" s="5">
+        <v>888</v>
+      </c>
+      <c r="X20" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="W20" s="5">
-        <v>888</v>
-      </c>
-      <c r="X20" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="Y20" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>15</v>
@@ -5411,13 +5409,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>15</v>
@@ -5427,23 +5425,23 @@
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5455,16 +5453,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU20" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="AU20" s="5" t="s">
+      <c r="AV20" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="AV20" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5472,81 +5470,81 @@
       <c r="BA20" s="6"/>
       <c r="BB20" s="6"/>
     </row>
-    <row r="21" spans="1:54" ht="272" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F21" s="5">
+        <v>888</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="F21" s="5">
-        <v>888</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="L21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>15</v>
@@ -5558,111 +5556,111 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AG21" s="5"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ21" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="AJ21" s="5" t="s">
-        <v>139</v>
-      </c>
       <c r="AK21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AP21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="AT21" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="AU21" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AV21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="AW21" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="AP21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="AT21" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="AU21" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="AV21" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="AW21" s="9" t="s">
+      <c r="AX21" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="AX21" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
       <c r="BB21" s="6"/>
     </row>
-    <row r="22" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5671,29 +5669,29 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R22" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>26</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="V22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="W22" s="5">
+        <v>888</v>
+      </c>
+      <c r="X22" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="W22" s="5">
-        <v>888</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>160</v>
-      </c>
       <c r="Y22" s="5">
         <v>888</v>
       </c>
@@ -5707,10 +5705,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>15</v>
@@ -5719,7 +5717,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5749,22 +5747,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="AT22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AU22" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AV22" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="AX22" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="AU22" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="AV22" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="AW22" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="AX22" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>

</xml_diff>

<commit_message>
Recoded name of instruments and covariates' names
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1207" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DC762A6C-62CD-074E-83EB-6AB077FB8C7A}"/>
+  <xr:revisionPtr revIDLastSave="1228" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{27F86795-D8DE-C84F-BC39-0BFAA04C01E4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="381">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -139,9 +139,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>Flash-card words (designed by the investigator)</t>
-  </si>
-  <si>
     <t xml:space="preserve">No reportaron estadísticas. </t>
   </si>
   <si>
@@ -200,9 +197,6 @@
   </si>
   <si>
     <t>ANCOVA</t>
-  </si>
-  <si>
-    <t>Pre-test measure (reading skills)</t>
   </si>
   <si>
     <t xml:space="preserve">Blending CV, Blending VC, Rime articulation and Coda articulation. </t>
@@ -324,9 +318,6 @@
     <t>Timé3, Alouette, Semantic similarity judgment task, name for measuring reading comprehension was not provided</t>
   </si>
   <si>
-    <t>For each analysis, some of the other reading skills at pretest were used as covariates</t>
-  </si>
-  <si>
     <t>word identification, reading fluency, listening comprehension (interaction between group and time), reading comprehension (interaction between group and time)</t>
   </si>
   <si>
@@ -437,9 +428,6 @@
     <t>Phonological Awareness Literacy Screening PreK assessment, Get Ready to Read!-Revised, researcher-developed measures</t>
   </si>
   <si>
-    <t>pretest reading skills,  age, income, mother's age, mother's education</t>
-  </si>
-  <si>
     <t>Lowercase letter knowledge, letter sound awareness, letter sound fluency, letter sequencing, alliterations, phonics, vocabulary, Get ready to Read (instrument)</t>
   </si>
   <si>
@@ -579,9 +567,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>British Picture Vocabulary Subscale II, BAS II, Test of Word Reading Efficiency, experimental tasks (researcher-developed)</t>
-  </si>
-  <si>
     <t>Only the intervention groups were balanced (not the control group)</t>
   </si>
   <si>
@@ -646,9 +631,6 @@
     <t>Grapho-syllabic training, Comprehension training (CoT).</t>
   </si>
   <si>
-    <t>Experimental task (researcher-developed), ODéDys, THaPHo, Peabody Picture Vocabulary Test-Revised</t>
-  </si>
-  <si>
     <t>Wilcoxon signed-rank test</t>
   </si>
   <si>
@@ -1057,9 +1039,6 @@
     <t>Computer-assisted learning in young poor readers: The effect of grapho-syllabic training on the development of word reading and reading comprehension</t>
   </si>
   <si>
-    <t>Which Picture is the Correct one?, Woodcock Reading Mastery Test-Revised, Wordchains test, Test of Word Reading Efficiency (TOWRE) and a researcher develop task (a list of pseudowords).</t>
-  </si>
-  <si>
     <t>Randomized Control Trial (RCT) with pretest-posttest</t>
   </si>
   <si>
@@ -1076,9 +1055,6 @@
     <t>Investigate the efficacy of an early reading intervention delivered alongside formal reading instruction to Norwegian 6-year old's to be at risk for RD at school entry through a group randomised controlled trial, with a two-year long term follow up after intervention.</t>
   </si>
   <si>
-    <t>Researcher-developed task, Norwegian Vocabulary Test (abbreviated))</t>
-  </si>
-  <si>
     <t>Evaluate the effectiveness of using a researcher-developed iPad app with a 0- to 5-s constant time delay procedure to improve phonological awareness skills of young children with mild developmental delays in a small-group arrangement in a rural public elementary school in Southwest United States.</t>
   </si>
   <si>
@@ -1213,6 +1189,27 @@
   </si>
   <si>
     <t>Researcher-developed (no name provided)</t>
+  </si>
+  <si>
+    <t>British Picture Vocabulary Subscale II, BAS II, Test of Word Reading Efficiency, researcher-developed measures</t>
+  </si>
+  <si>
+    <t>researcher-developed measures, Norwegian Vocabulary Test (abbreviated))</t>
+  </si>
+  <si>
+    <t>Flash-card words (researcher-developed measures)</t>
+  </si>
+  <si>
+    <t>Which Picture is the Correct one?, Woodcock Reading Mastery Test-Revised, Wordchains test, Test of Word Reading Efficiency (TOWRE) and a researcher-developed measures (a list of pseudowords).</t>
+  </si>
+  <si>
+    <t>Researcher-developed measures, ODéDys, THaPHo, Peabody Picture Vocabulary Test-Revised</t>
+  </si>
+  <si>
+    <t>Pre-test reading skills</t>
+  </si>
+  <si>
+    <t>Pre-test reading skills,  age, income, mother's age, mother's education</t>
   </si>
 </sst>
 </file>
@@ -2091,7 +2088,20 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX22" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}"/>
+  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}">
+    <filterColumn colId="23">
+      <filters>
+        <filter val="British Picture Vocabulary Subscale II, BAS II, Test of Word Reading Efficiency, experimental tasks (researcher-developed)"/>
+        <filter val="Experimental task (researcher-developed), ODéDys, THaPHo, Peabody Picture Vocabulary Test-Revised"/>
+        <filter val="Flash-card words (designed by the investigator)"/>
+        <filter val="Peabody Picture Vocabulary Test (PPVT), Letter-sound knowledge, Wide Range Achievement Test Word Recognition Subtest, Segmenting and Blending, Common units tasks, Nonsense word recognition, Unique word recognition."/>
+        <filter val="Phonological Awareness Literacy Screening PreK assessment, Get Ready to Read!-Revised, researcher-developed measures"/>
+        <filter val="Researcher-developed task, Norwegian Vocabulary Test (abbreviated))"/>
+        <filter val="Timé3, Alouette, Semantic similarity judgment task, name for measuring reading comprehension was not provided"/>
+        <filter val="Which Picture is the Correct one?, Woodcock Reading Mastery Test-Revised, Wordchains test, Test of Word Reading Efficiency (TOWRE) and a researcher develop task (a list of pseudowords)."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX22">
     <sortCondition ref="B1:B22"/>
   </sortState>
@@ -2488,8 +2498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R10" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2518,157 +2528,157 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AM1" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AR1" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="AQ1" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>320</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
       <c r="BB1" s="6"/>
     </row>
-    <row r="2" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>7</v>
       </c>
@@ -2679,7 +2689,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2691,10 +2701,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>15</v>
@@ -2706,19 +2716,19 @@
         <v>15</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2730,7 +2740,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>13</v>
@@ -2742,7 +2752,7 @@
         <v>14</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>15</v>
@@ -2754,13 +2764,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>15</v>
@@ -2776,13 +2786,13 @@
         <v>17</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2803,17 +2813,17 @@
         <v>19</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6"/>
     </row>
-    <row r="3" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -2833,13 +2843,13 @@
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>15</v>
@@ -2851,19 +2861,19 @@
         <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R3" s="7" t="s">
         <v>27</v>
@@ -2875,46 +2885,46 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="W3" s="5">
         <v>888</v>
       </c>
       <c r="X3" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="AH3" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF3" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="AI3" s="5">
         <v>888</v>
@@ -2933,7 +2943,7 @@
       </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AP3" s="5">
         <v>888</v>
@@ -2949,46 +2959,46 @@
         <v>24</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AW3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AX3" s="7"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
     </row>
-    <row r="4" spans="1:54" ht="372" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="372" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="5">
+        <v>888</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="F4" s="5">
-        <v>888</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>15</v>
@@ -3000,40 +3010,40 @@
         <v>15</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>27</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W4" s="5">
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>15</v>
@@ -3048,10 +3058,10 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE4" s="5" t="s">
         <v>15</v>
@@ -3060,10 +3070,10 @@
         <v>888</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3082,7 +3092,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3094,22 +3104,22 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AW4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX4" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="AX4" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6"/>
@@ -3120,43 +3130,43 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F5" s="5">
+        <v>888</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="F5" s="5">
-        <v>888</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="L5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
@@ -3165,34 +3175,34 @@
         <v>10</v>
       </c>
       <c r="Q5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="T5" s="7" t="s">
+      <c r="U5" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="V5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5">
+        <v>888</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="W5" s="5">
-        <v>888</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="Y5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3201,13 +3211,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>15</v>
@@ -3217,19 +3227,19 @@
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>49</v>
+        <v>379</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3243,16 +3253,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AU5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3260,57 +3270,57 @@
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
     </row>
-    <row r="6" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F6" s="5">
+        <v>888</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="O6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="F6" s="5">
-        <v>888</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="Q6" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>11</v>
@@ -3319,40 +3329,40 @@
         <v>12</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="W6" s="5">
         <v>888</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>15</v>
@@ -3362,16 +3372,16 @@
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>15</v>
@@ -3389,13 +3399,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3403,39 +3413,39 @@
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
     </row>
-    <row r="7" spans="1:54" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>15</v>
@@ -3444,40 +3454,40 @@
         <v>26</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>15</v>
@@ -3489,10 +3499,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>15</v>
@@ -3505,16 +3515,16 @@
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>15</v>
@@ -3532,94 +3542,94 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
     </row>
-    <row r="8" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="5">
+        <v>888</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F8" s="5">
-        <v>888</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="O8" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="W8" s="5">
         <v>888</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>15</v>
@@ -3628,19 +3638,19 @@
         <v>15</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>15</v>
@@ -3650,16 +3660,16 @@
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>15</v>
@@ -3677,94 +3687,94 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
     </row>
-    <row r="9" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="W9" s="5">
         <v>888</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="Y9" s="5">
         <v>888</v>
@@ -3794,26 +3804,26 @@
         <v>15</v>
       </c>
       <c r="AH9" s="7" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="AJ9" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3826,55 +3836,55 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="AU9" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="AV9" s="7" t="s">
         <v>259</v>
-      </c>
-      <c r="AV9" s="7" t="s">
-        <v>265</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
     </row>
-    <row r="10" spans="1:54" ht="170" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="F10" s="5">
         <v>888</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>15</v>
@@ -3883,75 +3893,75 @@
         <v>26</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>330</v>
+        <v>377</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AG10" s="5"/>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>15</v>
@@ -3969,13 +3979,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3983,57 +3993,57 @@
       <c r="BA10" s="6"/>
       <c r="BB10" s="6"/>
     </row>
-    <row r="11" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="F11" s="5">
         <v>888</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>11</v>
@@ -4042,19 +4052,19 @@
         <v>12</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="W11" s="5">
         <v>888</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>15</v>
@@ -4069,13 +4079,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>15</v>
@@ -4085,16 +4095,16 @@
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>15</v>
@@ -4112,55 +4122,55 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
       <c r="BB11" s="6"/>
     </row>
-    <row r="12" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F12" s="5">
         <v>888</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>15</v>
@@ -4172,34 +4182,34 @@
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="W12" s="5">
         <v>888</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>194</v>
+        <v>378</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>15</v>
@@ -4214,13 +4224,13 @@
         <v>888</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF12" s="4" t="s">
         <v>15</v>
@@ -4229,26 +4239,26 @@
         <v>888</v>
       </c>
       <c r="AH12" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AI12" s="5" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AP12" s="5">
         <v>888</v>
@@ -4260,60 +4270,60 @@
         <v>888</v>
       </c>
       <c r="AS12" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="AU12" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AV12" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="AW12" s="9" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="AX12" s="7" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
       <c r="BB12" s="6"/>
     </row>
-    <row r="13" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F13" s="5">
+        <v>888</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="F13" s="5">
-        <v>888</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>15</v>
@@ -4322,7 +4332,7 @@
         <v>26</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4331,28 +4341,28 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="W13" s="5">
         <v>888</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>172</v>
+        <v>374</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>15</v>
@@ -4361,19 +4371,19 @@
         <v>15</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>15</v>
@@ -4383,13 +4393,13 @@
       </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>15</v>
@@ -4399,7 +4409,7 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="AP13" s="5">
         <v>888</v>
@@ -4411,54 +4421,54 @@
         <v>888</v>
       </c>
       <c r="AS13" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT13" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AU13" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="AV13" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AW13" s="9" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="AX13" s="7" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="6"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>15</v>
@@ -4470,7 +4480,7 @@
         <v>15</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4479,95 +4489,95 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z14" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="AA14" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="AB14" s="5">
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="AG14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="AJ14" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN14" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AK14" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="AN14" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="AP14" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AQ14" s="2">
         <v>888</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AT14" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="AU14" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="AV14" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4575,115 +4585,115 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="5">
+        <v>888</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="5">
-        <v>888</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="L15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V15" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="W15" s="5">
         <v>888</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB15" s="5">
         <v>888</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AG15" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>15</v>
@@ -4693,7 +4703,7 @@
       </c>
       <c r="AN15" s="5"/>
       <c r="AO15" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AP15" s="5">
         <v>888</v>
@@ -4706,66 +4716,66 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AU15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV15" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AW15" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AV15" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="AW15" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="AX15" s="7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
       <c r="BB15" s="6"/>
     </row>
-    <row r="16" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="F16" s="5">
+        <v>888</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="I16" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="5">
-        <v>888</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="L16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="N16" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
@@ -4774,10 +4784,10 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>12</v>
@@ -4786,63 +4796,63 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="V16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="W16" s="5">
+        <v>888</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG16" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="W16" s="5">
-        <v>888</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB16" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4855,17 +4865,17 @@
       </c>
       <c r="AS16" s="7"/>
       <c r="AT16" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
@@ -4876,55 +4886,55 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="F17" s="5">
+        <v>888</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="H17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="5">
-        <v>888</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="L17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="P17" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="R17" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>12</v>
@@ -4933,19 +4943,19 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W17" s="5">
         <v>888</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>15</v>
@@ -4971,23 +4981,23 @@
       <c r="AG17" s="5"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>88</v>
+        <v>379</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -5000,75 +5010,75 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU17" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="AV17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AW17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AU17" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="AV17" s="7" t="s">
+      <c r="AX17" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="AW17" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="AX17" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="5">
+        <v>888</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="L18" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="5">
-        <v>888</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="N18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="P18" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="Q18" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R18" s="7" t="s">
         <v>11</v>
@@ -5080,37 +5090,37 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="W18" s="5">
         <v>888</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Y18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>15</v>
@@ -5120,16 +5130,16 @@
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>15</v>
@@ -5146,16 +5156,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT18" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5163,118 +5173,118 @@
       <c r="BA18" s="6"/>
       <c r="BB18" s="6"/>
     </row>
-    <row r="19" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F19" s="5">
+        <v>888</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="H19" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="I19" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="F19" s="5">
-        <v>888</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="L19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="N19" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="O19" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="P19" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="W19" s="5">
+        <v>888</v>
+      </c>
+      <c r="X19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="N19" s="7" t="s">
+      <c r="Y19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="T19" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="V19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="W19" s="5">
-        <v>888</v>
-      </c>
-      <c r="X19" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y19" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>15</v>
@@ -5291,19 +5301,19 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
@@ -5315,76 +5325,76 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F20" s="5">
+        <v>888</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="I20" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F20" s="5">
-        <v>888</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>122</v>
-      </c>
       <c r="L20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="W20" s="5">
         <v>888</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>15</v>
@@ -5396,13 +5406,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>15</v>
@@ -5412,23 +5422,23 @@
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>125</v>
+        <v>380</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5440,16 +5450,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT20" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="AU20" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="AV20" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5457,81 +5467,81 @@
       <c r="BA20" s="6"/>
       <c r="BB20" s="6"/>
     </row>
-    <row r="21" spans="1:54" ht="272" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F21" s="5">
         <v>888</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>336</v>
+        <v>375</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>15</v>
@@ -5543,37 +5553,37 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AG21" s="5"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="AJ21" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="AK21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="AP21" s="5">
         <v>888</v>
@@ -5585,69 +5595,69 @@
         <v>888</v>
       </c>
       <c r="AS21" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT21" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV21" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="AW21" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="AX21" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
       <c r="BB21" s="6"/>
     </row>
-    <row r="22" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="H22" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5656,28 +5666,28 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R22" s="7" t="s">
         <v>27</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>26</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="W22" s="5">
         <v>888</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Y22" s="5">
         <v>888</v>
@@ -5692,10 +5702,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>15</v>
@@ -5704,7 +5714,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5734,22 +5744,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AT22" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AV22" s="7" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AW22" s="9" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AX22" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>

</xml_diff>

<commit_message>
Recoded names of improved and not improved reading skills
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1244" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7F1E8C9-D038-3343-9BD0-7F1373646C63}"/>
+  <xr:revisionPtr revIDLastSave="1288" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56013EC5-ADFC-A247-AFA1-9A2E3AD982E9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="374">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -103,9 +103,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Baseline scores</t>
-  </si>
-  <si>
     <t>Blending, Non-word reading</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>ANCOVA</t>
   </si>
   <si>
-    <t xml:space="preserve">Blending CV, Blending VC, Rime articulation and Coda articulation. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Segmenting CV, Segmenting VC, WRAT word reading, Unique words, High N nonwords, Low N nonwords and Letter-sounds. </t>
   </si>
   <si>
@@ -224,12 +218,6 @@
   </si>
   <si>
     <t>Rate (wpm) and accuracy of results</t>
-  </si>
-  <si>
-    <t>pretest scores</t>
-  </si>
-  <si>
-    <t>Comprehension, Vocabulary, Oral reading rate, reading accuracy</t>
   </si>
   <si>
     <t>Analysis of Covariance (ANCOVA) was only used for comprehension, vocabulary; only descriptive statistics were provided for other variables</t>
@@ -272,13 +260,7 @@
     <t>Adjusted means</t>
   </si>
   <si>
-    <t>pretest scores (between group)</t>
-  </si>
-  <si>
     <t>Oral Reading Fluency</t>
-  </si>
-  <si>
-    <t>Initial Sound Fluency, Letter Naming Fluency, Word Use Fluency), Phoneme Segmentation, Nonsense Word Fluency, and Retell Fluency</t>
   </si>
   <si>
     <t>Potocki et al</t>
@@ -313,9 +295,6 @@
   </si>
   <si>
     <t>Timé3, Alouette, Semantic similarity judgment task, name for measuring reading comprehension was not provided</t>
-  </si>
-  <si>
-    <t>word identification, reading fluency, listening comprehension (interaction between group and time), reading comprehension (interaction between group and time)</t>
   </si>
   <si>
     <t>eta squared = .06 - .14</t>
@@ -359,9 +338,6 @@
     <t>Not specified (instruments seemed to have been designed by the researchers)</t>
   </si>
   <si>
-    <t>High SES: RAN; low SES: letter sound knowledge</t>
-  </si>
-  <si>
     <t>Phonological awareness, letter name knowledge, reading of words, reading of pseudowords, reading of frequent wods</t>
   </si>
   <si>
@@ -425,9 +401,6 @@
     <t>Phonological Awareness Literacy Screening PreK assessment, Get Ready to Read!-Revised, researcher-developed measures</t>
   </si>
   <si>
-    <t>Lowercase letter knowledge, letter sound awareness, letter sound fluency, letter sequencing, alliterations, phonics, vocabulary, Get ready to Read (instrument)</t>
-  </si>
-  <si>
     <t>uppercase letter knowledge, uppercase letter naming fluency, lowercase letter naming fluency, rhyming</t>
   </si>
   <si>
@@ -480,12 +453,6 @@
   </si>
   <si>
     <t>12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Word recognition, Word reading aloud, and Word Spelling. </t>
-  </si>
-  <si>
-    <t>Word recognition, word reading aloud and word spelling.</t>
   </si>
   <si>
     <t>Wood et al</t>
@@ -528,9 +495,6 @@
     <t>Word reading aloud task</t>
   </si>
   <si>
-    <t>Word reading aloud</t>
-  </si>
-  <si>
     <t>Examine the long-term effect of grapho-syllabic training proposed to French 1st graders and followed to the end of second grade.</t>
   </si>
   <si>
@@ -540,19 +504,10 @@
     <t>18</t>
   </si>
   <si>
-    <t xml:space="preserve">Listening comprehension task, Silent word reading task, Word reading aloud and Reading Comprehension. </t>
-  </si>
-  <si>
-    <t>Silent word reading, word reading aloud and Reading comprehension</t>
-  </si>
-  <si>
     <t>Kyle et al</t>
   </si>
   <si>
     <t>Assessing the Effectiveness of Two Theoretically Motivated Computer-Assisted Reading Interventions in the United Kingdom: GG Rime and GG Phoneme</t>
-  </si>
-  <si>
-    <t>vocabulary, word reading, spelling, phonological awareness, and rhyme awareness</t>
   </si>
   <si>
     <t>Pretest-posttest with control group (2 pc interventions and 1 control)</t>
@@ -664,9 +619,6 @@
     <t>Swedish</t>
   </si>
   <si>
-    <t xml:space="preserve">Reading comprehension, Passage comprehension, Word decoding, Sight word reading, and Pseudoword reading. </t>
-  </si>
-  <si>
     <t>Karemaker et al</t>
   </si>
   <si>
@@ -688,9 +640,6 @@
     <t>Lexical decision task (LDT), Single word oral reading task (SWORT), and Phonological Awareness Test (PAT).</t>
   </si>
   <si>
-    <t>Written word recognition, Written word naming, and Phonological awareness</t>
-  </si>
-  <si>
     <t>An evaluation of the effectiveness of a computer-assisted reading intervention</t>
   </si>
   <si>
@@ -719,9 +668,6 @@
   </si>
   <si>
     <t>general ability (IQ)</t>
-  </si>
-  <si>
-    <t>decoding, phonological awareness, rapid naming</t>
   </si>
   <si>
     <t>spelling</t>
@@ -1080,9 +1026,6 @@
     <t>Syllabic awareness and word recognition</t>
   </si>
   <si>
-    <t>Silent word reading, word reading aloud, reading comprehension</t>
-  </si>
-  <si>
     <t>Reading comprehension, Passage comprehension, Word decoding, Sight word reading, and Pseudoword reading</t>
   </si>
   <si>
@@ -1197,9 +1140,6 @@
     <t>Researcher-developed measures, ODéDys, THaPHo, Peabody Picture Vocabulary Test-Revised</t>
   </si>
   <si>
-    <t>Pre-test reading skills</t>
-  </si>
-  <si>
     <t>Pre-test reading skills,  age, income, mother's age, mother's education</t>
   </si>
   <si>
@@ -1207,6 +1147,48 @@
   </si>
   <si>
     <t>Regression analysis</t>
+  </si>
+  <si>
+    <t>Pretest reading skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blending CV, Blending VC, rime articulation and Coda articulation. </t>
+  </si>
+  <si>
+    <t>Word recognition, aloud word reading, and word spelling</t>
+  </si>
+  <si>
+    <t>Silent word reading, aloud word reading, reading comprehension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listening comprehension task, Silent word reading task, aloud word reading and Reading Comprehension. </t>
+  </si>
+  <si>
+    <t>Silent word reading, aloud word reading and Reading comprehension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word recognition, aloud word reading, and Word Spelling. </t>
+  </si>
+  <si>
+    <t>aloud word reading</t>
+  </si>
+  <si>
+    <t>decoding skills, phonological skills, rapid naming</t>
+  </si>
+  <si>
+    <t>word identification, reading fluency, listening comprehension, reading comprehension</t>
+  </si>
+  <si>
+    <t>High SES: rapid naming; low SES: letter sound knowledge</t>
+  </si>
+  <si>
+    <t>reading comprehension, Vocabulary, Oral reading rate, reading accuracy</t>
+  </si>
+  <si>
+    <t>Initial Sound Fluency, Letter Naming Fluency, Word Use Fluency, Phoneme Segmentation, Nonsense Word Fluency, and Retell Fluency</t>
+  </si>
+  <si>
+    <t>lowercase letter knowledge, letter sound awareness, letter sound fluency, letter sequencing, alliterations, phonics, vocabulary</t>
   </si>
 </sst>
 </file>
@@ -2085,15 +2067,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX22" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}">
-    <filterColumn colId="34">
-      <filters>
-        <filter val="ANCOVA, Repeated-Measures ANOVAs and Linear Regression"/>
-        <filter val="regression analysis"/>
-        <filter val="Tobit modelling (censored regression)"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX22">
     <sortCondition ref="B1:B22"/>
   </sortState>
@@ -2490,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI21" sqref="AI21"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU3" sqref="AU3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2520,151 +2494,151 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="U1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AR1" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="AE1" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM1" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="AN1" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="AO1" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>311</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
@@ -2681,7 +2655,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2693,10 +2667,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>15</v>
@@ -2708,19 +2682,19 @@
         <v>15</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2732,7 +2706,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>13</v>
@@ -2744,7 +2718,7 @@
         <v>14</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>15</v>
@@ -2756,13 +2730,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>15</v>
@@ -2772,19 +2746,19 @@
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="5" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>16</v>
+        <v>360</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2799,76 +2773,76 @@
       </c>
       <c r="AS2" s="7"/>
       <c r="AT2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AU2" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="AV2" s="7" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6"/>
     </row>
-    <row r="3" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="5">
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="L3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>12</v>
@@ -2877,22 +2851,22 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="W3" s="5">
         <v>888</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
       <c r="Y3" s="5">
         <v>888</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AA3" s="5">
         <v>888</v>
@@ -2901,7 +2875,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>15</v>
@@ -2913,10 +2887,10 @@
         <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="AH3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AI3" s="5">
         <v>888</v>
@@ -2935,7 +2909,7 @@
       </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AP3" s="5">
         <v>888</v>
@@ -2948,94 +2922,94 @@
       </c>
       <c r="AS3" s="7"/>
       <c r="AT3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AW3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AX3" s="7"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
     </row>
-    <row r="4" spans="1:54" ht="372" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="372" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" s="5">
+        <v>888</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="F4" s="5">
-        <v>888</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="W4" s="5">
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>15</v>
@@ -3050,22 +3024,22 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH4" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="AH4" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3084,7 +3058,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3096,69 +3070,69 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AW4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AX4" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="AX4" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6"/>
       <c r="BB4" s="6"/>
     </row>
-    <row r="5" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F5" s="5">
+        <v>888</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="F5" s="5">
-        <v>888</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="L5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
@@ -3167,34 +3141,34 @@
         <v>10</v>
       </c>
       <c r="Q5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="S5" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="T5" s="7" t="s">
+      <c r="U5" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="V5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="5">
+        <v>888</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="W5" s="5">
-        <v>888</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="Y5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3203,13 +3177,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>15</v>
@@ -3219,19 +3193,19 @@
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3245,16 +3219,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>47</v>
+        <v>361</v>
       </c>
       <c r="AU5" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3262,57 +3236,57 @@
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
     </row>
-    <row r="6" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="F6" s="5">
         <v>888</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>355</v>
-      </c>
       <c r="J6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>11</v>
@@ -3321,40 +3295,40 @@
         <v>12</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="W6" s="5">
         <v>888</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>140</v>
+        <v>366</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>15</v>
@@ -3364,16 +3338,16 @@
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>15</v>
@@ -3391,13 +3365,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>141</v>
+        <v>362</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3405,81 +3379,81 @@
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
     </row>
-    <row r="7" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>15</v>
@@ -3491,10 +3465,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>15</v>
@@ -3507,16 +3481,16 @@
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>15</v>
@@ -3534,94 +3508,94 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>155</v>
+        <v>367</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
     </row>
-    <row r="8" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="F8" s="5">
         <v>888</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>337</v>
+        <v>363</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="W8" s="5">
         <v>888</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>159</v>
+        <v>364</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>15</v>
@@ -3630,19 +3604,19 @@
         <v>15</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>15</v>
@@ -3652,16 +3626,16 @@
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>15</v>
@@ -3679,94 +3653,94 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>160</v>
+        <v>365</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
     </row>
-    <row r="9" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="F9" s="5">
         <v>888</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="W9" s="5">
         <v>888</v>
       </c>
       <c r="X9" s="5" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="Y9" s="5">
         <v>888</v>
@@ -3796,26 +3770,26 @@
         <v>15</v>
       </c>
       <c r="AH9" s="7" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="AJ9" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3828,134 +3802,134 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
     </row>
-    <row r="10" spans="1:54" ht="170" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="170" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="F10" s="5">
         <v>888</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>357</v>
-      </c>
       <c r="J10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AG10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>15</v>
@@ -3973,13 +3947,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>199</v>
+        <v>319</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3987,57 +3961,57 @@
       <c r="BA10" s="6"/>
       <c r="BB10" s="6"/>
     </row>
-    <row r="11" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="F11" s="5">
         <v>888</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>11</v>
@@ -4046,19 +4020,19 @@
         <v>12</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="W11" s="5">
         <v>888</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>15</v>
@@ -4073,13 +4047,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>15</v>
@@ -4089,16 +4063,16 @@
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>15</v>
@@ -4116,94 +4090,94 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>207</v>
+        <v>325</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
       <c r="BB11" s="6"/>
     </row>
-    <row r="12" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="F12" s="5">
         <v>888</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N12" s="7">
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="W12" s="5">
         <v>888</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>15</v>
@@ -4218,41 +4192,41 @@
         <v>888</v>
       </c>
       <c r="AC12" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AH12" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AE12" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AF12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AH12" s="7" t="s">
-        <v>251</v>
-      </c>
       <c r="AI12" s="5" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="AP12" s="5">
         <v>888</v>
@@ -4264,69 +4238,69 @@
         <v>888</v>
       </c>
       <c r="AS12" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="AU12" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="AV12" s="9" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="AW12" s="9" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="AX12" s="7" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
       <c r="BB12" s="6"/>
     </row>
-    <row r="13" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="F13" s="5">
         <v>888</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4335,28 +4309,28 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="W13" s="5">
         <v>888</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>15</v>
@@ -4365,19 +4339,19 @@
         <v>15</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>15</v>
@@ -4387,13 +4361,13 @@
       </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>57</v>
+        <v>360</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>15</v>
@@ -4403,7 +4377,7 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="AP13" s="5">
         <v>888</v>
@@ -4415,22 +4389,22 @@
         <v>888</v>
       </c>
       <c r="AS13" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT13" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AU13" s="5" t="s">
-        <v>163</v>
+        <v>322</v>
       </c>
       <c r="AV13" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AW13" s="9" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="AX13" s="7" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
@@ -4441,28 +4415,28 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>15</v>
@@ -4474,7 +4448,7 @@
         <v>15</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4483,95 +4457,95 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="AB14" s="5">
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="AG14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="AK14" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="AM14" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="AN14" s="2" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="AP14" s="2" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="AQ14" s="2">
         <v>888</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="AT14" s="2" t="s">
-        <v>218</v>
+        <v>368</v>
       </c>
       <c r="AU14" s="2" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="AV14" s="2" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4579,115 +4553,115 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="F15" s="5">
+        <v>888</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="5">
-        <v>888</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>54</v>
-      </c>
       <c r="L15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V15" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W15" s="5">
         <v>888</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AB15" s="5">
         <v>888</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AG15" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>57</v>
+        <v>360</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>15</v>
@@ -4697,7 +4671,7 @@
       </c>
       <c r="AN15" s="5"/>
       <c r="AO15" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AP15" s="5">
         <v>888</v>
@@ -4710,66 +4684,66 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>58</v>
+        <v>371</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AW15" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
       <c r="BB15" s="6"/>
     </row>
-    <row r="16" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="5">
+        <v>888</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="I16" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="L16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="5">
-        <v>888</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="N16" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
@@ -4778,10 +4752,10 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>12</v>
@@ -4790,16 +4764,16 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="W16" s="5">
         <v>888</v>
       </c>
       <c r="X16" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Y16" s="5" t="s">
         <v>15</v>
@@ -4814,39 +4788,39 @@
         <v>888</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD16" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE16" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="AG16" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>71</v>
+        <v>360</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4859,76 +4833,76 @@
       </c>
       <c r="AS16" s="7"/>
       <c r="AT16" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>73</v>
+        <v>372</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="6"/>
     </row>
-    <row r="17" spans="1:54" ht="289" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" ht="289" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="5">
+        <v>888</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="L17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="P17" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="5">
-        <v>888</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="R17" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S17" s="5" t="s">
         <v>12</v>
@@ -4937,19 +4911,19 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="W17" s="5">
         <v>888</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>15</v>
@@ -4977,23 +4951,23 @@
       </c>
       <c r="AH17" s="7"/>
       <c r="AI17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -5006,75 +4980,75 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
-        <v>85</v>
+        <v>369</v>
       </c>
       <c r="AU17" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV17" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="AW17" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="AX17" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F18" s="5">
         <v>888</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="R18" s="7" t="s">
         <v>11</v>
@@ -5086,37 +5060,37 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="W18" s="5">
         <v>888</v>
       </c>
       <c r="X18" s="5" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="Y18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>15</v>
@@ -5126,16 +5100,16 @@
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>57</v>
+        <v>360</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>15</v>
@@ -5152,16 +5126,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT18" s="5" t="s">
-        <v>99</v>
+        <v>370</v>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5169,118 +5143,118 @@
       <c r="BA18" s="6"/>
       <c r="BB18" s="6"/>
     </row>
-    <row r="19" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F19" s="5">
+        <v>888</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="W19" s="5">
+        <v>888</v>
+      </c>
+      <c r="X19" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="Y19" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="F19" s="5">
-        <v>888</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="T19" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="V19" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="W19" s="5">
-        <v>888</v>
-      </c>
-      <c r="X19" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y19" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>15</v>
@@ -5297,100 +5271,100 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
       <c r="BA19" s="6"/>
       <c r="BB19" s="6"/>
     </row>
-    <row r="20" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="F20" s="5">
         <v>888</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="W20" s="5">
         <v>888</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>15</v>
@@ -5402,13 +5376,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>15</v>
@@ -5418,23 +5392,23 @@
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5446,16 +5420,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT20" s="5" t="s">
-        <v>121</v>
+        <v>373</v>
       </c>
       <c r="AU20" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="AV20" s="7" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5468,76 +5442,76 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="F21" s="5">
         <v>888</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N21" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>15</v>
@@ -5549,39 +5523,39 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AG21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AH21" s="7"/>
       <c r="AI21" s="2" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="AJ21" s="5" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="AK21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="AP21" s="5">
         <v>888</v>
@@ -5593,69 +5567,69 @@
         <v>888</v>
       </c>
       <c r="AS21" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT21" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV21" s="7" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="AW21" s="9" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="AX21" s="7" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
       <c r="BB21" s="6"/>
     </row>
-    <row r="22" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F22" s="5">
         <v>888</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5664,28 +5638,28 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="W22" s="5">
         <v>888</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="Y22" s="5">
         <v>888</v>
@@ -5700,10 +5674,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>15</v>
@@ -5712,7 +5686,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5742,22 +5716,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AT22" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="AV22" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AW22" s="9" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="AX22" s="7" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>

</xml_diff>

<commit_message>
Fix errors discovered through freq analysis
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1288" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{56013EC5-ADFC-A247-AFA1-9A2E3AD982E9}"/>
+  <xr:revisionPtr revIDLastSave="1354" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F5C7D54-2974-7D4F-BF90-8E5D5C29EBBE}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="368">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -85,9 +85,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>40</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
   </si>
   <si>
     <t>15</t>
-  </si>
-  <si>
-    <t>Tres</t>
   </si>
   <si>
     <t>4</t>
@@ -646,12 +640,6 @@
     <t>Determine whether the use of a computer computer-assisted intervention that uses visual mnemonics as part of the tutorial process helps the development of reading abilities.</t>
   </si>
   <si>
-    <t>group</t>
-  </si>
-  <si>
-    <t>supervised</t>
-  </si>
-  <si>
     <t>trainertext</t>
   </si>
   <si>
@@ -661,12 +649,6 @@
     <t>TOWRE, Phonological Assessment Battery, PhAB, BAS II Spelling Scale</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>general ability (IQ)</t>
   </si>
   <si>
@@ -908,9 +890,6 @@
   </si>
   <si>
     <t>Covariate</t>
-  </si>
-  <si>
-    <t>Specific v-value provided</t>
   </si>
   <si>
     <t>Effect size provided</t>
@@ -1071,9 +1050,6 @@
     <t>Pretest-posttest design with comparison group</t>
   </si>
   <si>
-    <t>Pretest-posttest design with 2 experimental groups</t>
-  </si>
-  <si>
     <t>Explore the effectiveness of a Web-based literacy programme that delivered two distinct phonics programmes.</t>
   </si>
   <si>
@@ -1189,13 +1165,19 @@
   </si>
   <si>
     <t>lowercase letter knowledge, letter sound awareness, letter sound fluency, letter sequencing, alliterations, phonics, vocabulary</t>
+  </si>
+  <si>
+    <t>pretest-posttest design with multiple comparison groups</t>
+  </si>
+  <si>
+    <t>Specific p-value provided</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1208,12 +1190,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1257,56 +1233,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="52">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1928,6 +1854,56 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -2066,62 +2042,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX22" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:AX22" xr:uid="{8501DEE6-440D-475F-B2A6-0BB0DA93BA93}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX23" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+  <autoFilter ref="A1:AX23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}">
+    <filterColumn colId="17">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX22">
     <sortCondition ref="B1:B22"/>
   </sortState>
   <tableColumns count="50">
-    <tableColumn id="1" xr3:uid="{0B078E7E-83E4-453C-8557-B689B2516465}" name="ID" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{3AD873ED-B3D7-417E-A6AB-800F1E5459F4}" name="Author" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{4044AAAA-9E80-4793-AC51-E5F5CD0694AD}" name="Year" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{8364FC52-A4F5-407C-918E-33C3CFAA4542}" name="Title" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{F5CA48F2-8F78-4303-B81F-A731AECB9DFA}" name="Purpose" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{AF745F93-691A-410F-9848-43E62584120C}" name="Cognitive processes to impact" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{ED5FC934-5B38-4BA8-9AE2-91F922F96E30}" name="Reading skills to impact" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{85807B29-1C14-4F47-B5D5-4AE5569A0A05}" name="Design" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{2B5A5073-6303-1046-A445-26BB37292EFE}" name="Design_coded" dataDxfId="0"/>
-    <tableColumn id="56" xr3:uid="{932A60C9-8B73-4E92-87A5-23592C00770D}" name="Inferred design" dataDxfId="43"/>
-    <tableColumn id="16" xr3:uid="{01B4398B-886B-4B39-9F7C-BB3550166D78}" name="Number of participants" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{45C5B1E8-14B1-4491-AEE9-F20EEC3E0F49}" name="Probabilistic sampling" dataDxfId="41"/>
-    <tableColumn id="19" xr3:uid="{51CA66B9-1DFA-464C-BC3B-6EA038A92C8A}" name="Grade" dataDxfId="40"/>
-    <tableColumn id="21" xr3:uid="{061D070E-4B42-4273-9AAD-4EC93B84AD81}" name="Age" dataDxfId="39"/>
-    <tableColumn id="22" xr3:uid="{31070516-608E-41E0-93C1-2CC77E80426F}" name="Language" dataDxfId="38"/>
-    <tableColumn id="23" xr3:uid="{C92854F5-2EF0-4285-B7F6-8C05B4A90195}" name="Session number" dataDxfId="37"/>
-    <tableColumn id="24" xr3:uid="{B30E45D7-CC2B-4FDC-81C4-AB4317E182CE}" name="Session duration" dataDxfId="36"/>
-    <tableColumn id="25" xr3:uid="{19C302C0-56F0-45E0-95EE-BCBDAF18F282}" name="sessions frequency" dataDxfId="35"/>
-    <tableColumn id="26" xr3:uid="{ACEA4A35-6C0A-4701-8F70-24864DBA8770}" name="Modality" dataDxfId="34"/>
-    <tableColumn id="27" xr3:uid="{A06FDE04-A553-4BEF-995A-31322B29A28C}" name="Participants in group modality" dataDxfId="33"/>
-    <tableColumn id="28" xr3:uid="{0FED9BC8-7DB8-4F8E-B677-DADF5940B6CC}" name="Supervision" dataDxfId="32"/>
-    <tableColumn id="29" xr3:uid="{4D548382-0ABC-4BD6-9A3D-78FCE85DCBC1}" name="Intervention name" dataDxfId="31"/>
-    <tableColumn id="30" xr3:uid="{63FCD5C3-B077-493B-B321-B0604366EB96}" name="Instruments to measure cognition" dataDxfId="30"/>
-    <tableColumn id="31" xr3:uid="{E3A52C0B-9BE7-4A14-93E7-C4247CE91B90}" name="Instruments to measure reading skills" dataDxfId="29"/>
-    <tableColumn id="32" xr3:uid="{0D56973D-C88D-40FE-A90F-B0AFB213AFDF}" name="Random assignment" dataDxfId="28"/>
-    <tableColumn id="33" xr3:uid="{ECFDDC08-D3B7-4CF9-AF2D-BA1AAE9641F6}" name="Assessment counterbalancing" dataDxfId="27"/>
-    <tableColumn id="34" xr3:uid="{EE5CE2B4-6D44-44A0-BC90-566EB9520766}" name="Variables for group balance" dataDxfId="26"/>
-    <tableColumn id="37" xr3:uid="{C28C160E-D7AE-41F1-9FB7-C3E66D709720}" name="Other methodological controls" dataDxfId="25"/>
-    <tableColumn id="38" xr3:uid="{2EA382FB-29FE-4AAB-A2D4-55C13414BFF5}" name="Descriptive statistics provided" dataDxfId="24"/>
-    <tableColumn id="39" xr3:uid="{09505FCD-0E9E-4883-A35E-0564AA34BA56}" name="Mean/Median" dataDxfId="23"/>
-    <tableColumn id="40" xr3:uid="{484DDF92-F6A0-4359-8958-DC5B1C8A3B0C}" name="Standard deviation" dataDxfId="22"/>
-    <tableColumn id="41" xr3:uid="{55D2984D-1B81-4C5D-887F-785B42549436}" name="Mean confidence interval" dataDxfId="21"/>
-    <tableColumn id="42" xr3:uid="{1C5ABDAC-5E8F-4586-AF3F-5CE38E434290}" name="Other descriptive statistics" dataDxfId="20"/>
-    <tableColumn id="57" xr3:uid="{C48DCD7B-4527-4E53-A3F7-E60E0ECEF558}" name="Comments about descriptive statistics" dataDxfId="19"/>
-    <tableColumn id="44" xr3:uid="{7A4931EC-DAB2-43FD-9563-B41C63AF994C}" name="Inferential statistics" dataDxfId="18"/>
-    <tableColumn id="45" xr3:uid="{04FD368E-6727-4A16-B432-6055946ADB4E}" name="Covariate" dataDxfId="17"/>
-    <tableColumn id="46" xr3:uid="{002B09FC-42A5-4B9E-B00B-4247469ED640}" name="Specific v-value provided" dataDxfId="16"/>
-    <tableColumn id="47" xr3:uid="{2491D4F3-A98E-4ED6-9CC0-5BEBA0AED5A2}" name="Effect size provided" dataDxfId="15"/>
-    <tableColumn id="48" xr3:uid="{ED100DE6-09FF-4604-99D6-73681EB7237F}" name="Mean difference confidence interval" dataDxfId="14"/>
-    <tableColumn id="49" xr3:uid="{51DB6773-4D14-4AE1-9DA6-3C452E8BD712}" name="Other statistical controls" dataDxfId="13"/>
-    <tableColumn id="58" xr3:uid="{5B74B444-7863-49DC-BECA-49FEE05F9984}" name="Comments inferential statistics" dataDxfId="12"/>
-    <tableColumn id="50" xr3:uid="{E36D3572-9344-404D-AEED-4C18E7A993EF}" name="Improved cognitive processes" dataDxfId="11"/>
-    <tableColumn id="51" xr3:uid="{2B520559-FCB3-4512-B091-68EA56AAEE21}" name="Cognitive processes that did not improve" dataDxfId="10"/>
-    <tableColumn id="52" xr3:uid="{1EA75320-37D8-4F15-940E-B6A10594C3A3}" name="Effect size cognition" dataDxfId="9"/>
-    <tableColumn id="59" xr3:uid="{D5BEAA29-1A8C-40F5-9AC8-5637860CE237}" name="Comments effect on cognition" dataDxfId="8"/>
-    <tableColumn id="53" xr3:uid="{C933BD5B-B918-4F2D-B8F7-CD8E7A132A17}" name="Improved reading skills" dataDxfId="7"/>
-    <tableColumn id="54" xr3:uid="{F39DD7A1-CBC3-4AF0-B362-68FFD32F347B}" name="Reading skills no improvement" dataDxfId="6"/>
-    <tableColumn id="55" xr3:uid="{A6F391AD-5850-47C2-9D08-4CFA06D01676}" name="Effect size reading skills" dataDxfId="5"/>
-    <tableColumn id="60" xr3:uid="{6050F297-C3B7-4DDE-A740-5139D8EAF8F5}" name="Comments effect on reading skills" dataDxfId="4"/>
-    <tableColumn id="61" xr3:uid="{C3B05082-6C97-4BD7-B093-5FB9EEC21E36}" name="General comments" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{0B078E7E-83E4-453C-8557-B689B2516465}" name="ID" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{3AD873ED-B3D7-417E-A6AB-800F1E5459F4}" name="Author" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{4044AAAA-9E80-4793-AC51-E5F5CD0694AD}" name="Year" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{8364FC52-A4F5-407C-918E-33C3CFAA4542}" name="Title" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{F5CA48F2-8F78-4303-B81F-A731AECB9DFA}" name="Purpose" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{AF745F93-691A-410F-9848-43E62584120C}" name="Cognitive processes to impact" dataDxfId="44"/>
+    <tableColumn id="12" xr3:uid="{ED5FC934-5B38-4BA8-9AE2-91F922F96E30}" name="Reading skills to impact" dataDxfId="43"/>
+    <tableColumn id="14" xr3:uid="{85807B29-1C14-4F47-B5D5-4AE5569A0A05}" name="Design" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{2B5A5073-6303-1046-A445-26BB37292EFE}" name="Design_coded" dataDxfId="41"/>
+    <tableColumn id="56" xr3:uid="{932A60C9-8B73-4E92-87A5-23592C00770D}" name="Inferred design" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{01B4398B-886B-4B39-9F7C-BB3550166D78}" name="Number of participants" dataDxfId="39"/>
+    <tableColumn id="17" xr3:uid="{45C5B1E8-14B1-4491-AEE9-F20EEC3E0F49}" name="Probabilistic sampling" dataDxfId="38"/>
+    <tableColumn id="19" xr3:uid="{51CA66B9-1DFA-464C-BC3B-6EA038A92C8A}" name="Grade" dataDxfId="37"/>
+    <tableColumn id="21" xr3:uid="{061D070E-4B42-4273-9AAD-4EC93B84AD81}" name="Age" dataDxfId="36"/>
+    <tableColumn id="22" xr3:uid="{31070516-608E-41E0-93C1-2CC77E80426F}" name="Language" dataDxfId="35"/>
+    <tableColumn id="23" xr3:uid="{C92854F5-2EF0-4285-B7F6-8C05B4A90195}" name="Session number" dataDxfId="34"/>
+    <tableColumn id="24" xr3:uid="{B30E45D7-CC2B-4FDC-81C4-AB4317E182CE}" name="Session duration" dataDxfId="33"/>
+    <tableColumn id="25" xr3:uid="{19C302C0-56F0-45E0-95EE-BCBDAF18F282}" name="sessions frequency" dataDxfId="32"/>
+    <tableColumn id="26" xr3:uid="{ACEA4A35-6C0A-4701-8F70-24864DBA8770}" name="Modality" dataDxfId="31"/>
+    <tableColumn id="27" xr3:uid="{A06FDE04-A553-4BEF-995A-31322B29A28C}" name="Participants in group modality" dataDxfId="30"/>
+    <tableColumn id="28" xr3:uid="{0FED9BC8-7DB8-4F8E-B677-DADF5940B6CC}" name="Supervision" dataDxfId="29"/>
+    <tableColumn id="29" xr3:uid="{4D548382-0ABC-4BD6-9A3D-78FCE85DCBC1}" name="Intervention name" dataDxfId="28"/>
+    <tableColumn id="30" xr3:uid="{63FCD5C3-B077-493B-B321-B0604366EB96}" name="Instruments to measure cognition" dataDxfId="27"/>
+    <tableColumn id="31" xr3:uid="{E3A52C0B-9BE7-4A14-93E7-C4247CE91B90}" name="Instruments to measure reading skills" dataDxfId="26"/>
+    <tableColumn id="32" xr3:uid="{0D56973D-C88D-40FE-A90F-B0AFB213AFDF}" name="Random assignment" dataDxfId="25"/>
+    <tableColumn id="33" xr3:uid="{ECFDDC08-D3B7-4CF9-AF2D-BA1AAE9641F6}" name="Assessment counterbalancing" dataDxfId="24"/>
+    <tableColumn id="34" xr3:uid="{EE5CE2B4-6D44-44A0-BC90-566EB9520766}" name="Variables for group balance" dataDxfId="23"/>
+    <tableColumn id="37" xr3:uid="{C28C160E-D7AE-41F1-9FB7-C3E66D709720}" name="Other methodological controls" dataDxfId="22"/>
+    <tableColumn id="38" xr3:uid="{2EA382FB-29FE-4AAB-A2D4-55C13414BFF5}" name="Descriptive statistics provided" dataDxfId="21"/>
+    <tableColumn id="39" xr3:uid="{09505FCD-0E9E-4883-A35E-0564AA34BA56}" name="Mean/Median" dataDxfId="20"/>
+    <tableColumn id="40" xr3:uid="{484DDF92-F6A0-4359-8958-DC5B1C8A3B0C}" name="Standard deviation" dataDxfId="19"/>
+    <tableColumn id="41" xr3:uid="{55D2984D-1B81-4C5D-887F-785B42549436}" name="Mean confidence interval" dataDxfId="18"/>
+    <tableColumn id="42" xr3:uid="{1C5ABDAC-5E8F-4586-AF3F-5CE38E434290}" name="Other descriptive statistics" dataDxfId="17"/>
+    <tableColumn id="57" xr3:uid="{C48DCD7B-4527-4E53-A3F7-E60E0ECEF558}" name="Comments about descriptive statistics" dataDxfId="16"/>
+    <tableColumn id="44" xr3:uid="{7A4931EC-DAB2-43FD-9563-B41C63AF994C}" name="Inferential statistics" dataDxfId="15"/>
+    <tableColumn id="45" xr3:uid="{04FD368E-6727-4A16-B432-6055946ADB4E}" name="Covariate" dataDxfId="14"/>
+    <tableColumn id="46" xr3:uid="{002B09FC-42A5-4B9E-B00B-4247469ED640}" name="Specific p-value provided" dataDxfId="13"/>
+    <tableColumn id="47" xr3:uid="{2491D4F3-A98E-4ED6-9CC0-5BEBA0AED5A2}" name="Effect size provided" dataDxfId="12"/>
+    <tableColumn id="48" xr3:uid="{ED100DE6-09FF-4604-99D6-73681EB7237F}" name="Mean difference confidence interval" dataDxfId="11"/>
+    <tableColumn id="49" xr3:uid="{51DB6773-4D14-4AE1-9DA6-3C452E8BD712}" name="Other statistical controls" dataDxfId="10"/>
+    <tableColumn id="58" xr3:uid="{5B74B444-7863-49DC-BECA-49FEE05F9984}" name="Comments inferential statistics" dataDxfId="9"/>
+    <tableColumn id="50" xr3:uid="{E36D3572-9344-404D-AEED-4C18E7A993EF}" name="Improved cognitive processes" dataDxfId="8"/>
+    <tableColumn id="51" xr3:uid="{2B520559-FCB3-4512-B091-68EA56AAEE21}" name="Cognitive processes that did not improve" dataDxfId="7"/>
+    <tableColumn id="52" xr3:uid="{1EA75320-37D8-4F15-940E-B6A10594C3A3}" name="Effect size cognition" dataDxfId="6"/>
+    <tableColumn id="59" xr3:uid="{D5BEAA29-1A8C-40F5-9AC8-5637860CE237}" name="Comments effect on cognition" dataDxfId="5"/>
+    <tableColumn id="53" xr3:uid="{C933BD5B-B918-4F2D-B8F7-CD8E7A132A17}" name="Improved reading skills" dataDxfId="4"/>
+    <tableColumn id="54" xr3:uid="{F39DD7A1-CBC3-4AF0-B362-68FFD32F347B}" name="Reading skills no improvement" dataDxfId="3"/>
+    <tableColumn id="55" xr3:uid="{A6F391AD-5850-47C2-9D08-4CFA06D01676}" name="Effect size reading skills" dataDxfId="2"/>
+    <tableColumn id="60" xr3:uid="{6050F297-C3B7-4DDE-A740-5139D8EAF8F5}" name="Comments effect on reading skills" dataDxfId="1"/>
+    <tableColumn id="61" xr3:uid="{C3B05082-6C97-4BD7-B093-5FB9EEC21E36}" name="General comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2464,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU3" sqref="AU3"/>
+    <sheetView tabSelected="1" topLeftCell="L5" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2494,157 +2476,157 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="AL1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="AE1" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AM1" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="AP1" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AQ1" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="AR1" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="AU1" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>293</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
       <c r="BB1" s="6"/>
     </row>
-    <row r="2" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>7</v>
       </c>
@@ -2655,7 +2637,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2667,61 +2649,61 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
       </c>
       <c r="S2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="5">
+        <v>888</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="5">
-        <v>888</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5">
+        <v>888</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="5">
-        <v>888</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="Y2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA2" s="5">
         <v>888</v>
@@ -2730,35 +2712,35 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="5" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2773,17 +2755,17 @@
       </c>
       <c r="AS2" s="7"/>
       <c r="AT2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AU2" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="AV2" s="7" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
@@ -2794,104 +2776,104 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" s="5">
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="L3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="7">
+        <v>3</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="5">
+        <v>888</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="W3" s="5">
+        <v>888</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="AH3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" s="5">
-        <v>888</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="W3" s="5">
-        <v>888</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z3" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF3" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="AI3" s="5">
         <v>888</v>
       </c>
@@ -2905,11 +2887,11 @@
         <v>888</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AP3" s="5">
         <v>888</v>
@@ -2922,97 +2904,97 @@
       </c>
       <c r="AS3" s="7"/>
       <c r="AT3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AW3" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AX3" s="7"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
     </row>
-    <row r="4" spans="1:54" ht="372" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="372" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F4" s="5">
+        <v>888</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="F4" s="5">
-        <v>888</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="W4" s="5">
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z4" s="4">
         <v>888</v>
@@ -3024,22 +3006,22 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AF4" s="4">
         <v>888</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3054,11 +3036,11 @@
         <v>888</v>
       </c>
       <c r="AM4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3070,22 +3052,22 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AW4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AX4" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="AX4" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="AZ4" s="6"/>
       <c r="BA4" s="6"/>
@@ -3096,79 +3078,79 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F5" s="5">
+        <v>888</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="F5" s="5">
-        <v>888</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="L5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>10</v>
+      <c r="P5" s="7">
+        <v>40</v>
       </c>
       <c r="Q5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="7">
+        <v>3</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="T5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="U5" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="T5" s="7" t="s">
+      <c r="W5" s="5">
+        <v>888</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U5" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="W5" s="5">
-        <v>888</v>
-      </c>
-      <c r="X5" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="Y5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3177,35 +3159,35 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3219,16 +3201,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="AU5" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3236,121 +3218,121 @@
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
     </row>
-    <row r="6" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="5">
+        <v>888</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="I6" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F6" s="5">
-        <v>888</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="L6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="7" t="s">
+      <c r="O6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="Q6" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="7">
+        <v>5</v>
+      </c>
+      <c r="S6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>233</v>
+      <c r="T6" s="5">
+        <v>888</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="W6" s="5">
         <v>888</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN6" s="5"/>
       <c r="AO6" s="7"/>
@@ -3365,13 +3347,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3379,121 +3361,121 @@
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
     </row>
-    <row r="7" spans="1:54" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>99</v>
+        <v>23</v>
+      </c>
+      <c r="N7" s="7">
+        <v>7</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB7" s="5">
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN7" s="5"/>
       <c r="AO7" s="7"/>
@@ -3508,137 +3490,137 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
     </row>
-    <row r="8" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="5">
+        <v>888</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F8" s="5">
-        <v>888</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="L8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q8" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="W8" s="5">
         <v>888</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN8" s="5"/>
       <c r="AO8" s="7"/>
@@ -3653,143 +3635,143 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
     </row>
-    <row r="9" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="H9" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="L9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="5">
+        <v>888</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="W9" s="5">
+        <v>888</v>
+      </c>
+      <c r="X9" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="Q9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V9" s="5" t="s">
+      <c r="Y9" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AI9" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="W9" s="5">
-        <v>888</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH9" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="AJ9" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3802,137 +3784,137 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AU9" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV9" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="AV9" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
     </row>
-    <row r="10" spans="1:54" ht="170" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="170" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F10" s="5">
+        <v>888</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="I10" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="F10" s="5">
-        <v>888</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="L10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="P10" s="7">
+        <v>25</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="5">
+        <v>888</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V10" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q10" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>346</v>
-      </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AG10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN10" s="5"/>
       <c r="AO10" s="7"/>
@@ -3947,13 +3929,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3961,121 +3943,121 @@
       <c r="BA10" s="6"/>
       <c r="BB10" s="6"/>
     </row>
-    <row r="11" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F11" s="5">
+        <v>888</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="I11" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="F11" s="5">
-        <v>888</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="L11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q11" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="R11" s="7">
+        <v>5</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T11" s="5">
+        <v>888</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="W11" s="5">
+        <v>888</v>
+      </c>
+      <c r="X11" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="R11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T11" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="U11" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V11" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="W11" s="5">
-        <v>888</v>
-      </c>
-      <c r="X11" s="5" t="s">
-        <v>190</v>
-      </c>
       <c r="Y11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB11" s="5">
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN11" s="5"/>
       <c r="AO11" s="7"/>
@@ -4090,217 +4072,217 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
       <c r="BB11" s="6"/>
     </row>
-    <row r="12" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="F12" s="5">
+        <v>888</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="I12" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F12" s="5">
-        <v>888</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>170</v>
-      </c>
       <c r="L12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N12" s="7">
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q12" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="R12" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="W12" s="5">
         <v>888</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB12" s="5">
         <v>888</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG12" s="5">
         <v>888</v>
       </c>
       <c r="AH12" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AI12" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS12" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="AW12" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="AX12" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="AP12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS12" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="AT12" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="AU12" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AV12" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="AW12" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="AX12" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
       <c r="BB12" s="6"/>
     </row>
-    <row r="13" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F13" s="5">
+        <v>888</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="I13" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="F13" s="5">
-        <v>888</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>150</v>
-      </c>
       <c r="L13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4309,75 +4291,75 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>11</v>
+        <v>197</v>
+      </c>
+      <c r="R13" s="7">
+        <v>5</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="W13" s="5">
         <v>888</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AM13" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AP13" s="5">
         <v>888</v>
@@ -4389,66 +4371,66 @@
         <v>888</v>
       </c>
       <c r="AS13" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT13" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AU13" s="5" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="AV13" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AW13" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AX13" s="7" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="6"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="2">
         <v>78</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4457,95 +4439,95 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="S14" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="X14" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="T14" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="Y14" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="AB14" s="5">
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="AG14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="AJ14" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP14" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="AK14" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AN14" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AP14" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="AQ14" s="2">
         <v>888</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="AT14" s="2" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="AU14" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AV14" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4553,125 +4535,125 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="F15" s="5">
+        <v>888</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="H15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="5">
-        <v>888</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="L15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V15" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="W15" s="5">
         <v>888</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB15" s="5">
         <v>888</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG15" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AM15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN15" s="5"/>
       <c r="AO15" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AP15" s="5">
         <v>888</v>
@@ -4684,66 +4666,66 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AW15" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
       <c r="BB15" s="6"/>
     </row>
-    <row r="16" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="F16" s="5">
+        <v>888</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="I16" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="5">
-        <v>888</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="L16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="N16" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
@@ -4752,75 +4734,75 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T16" s="5">
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="V16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W16" s="5">
+        <v>888</v>
+      </c>
+      <c r="X16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG16" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="W16" s="5">
-        <v>888</v>
-      </c>
-      <c r="X16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB16" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4833,109 +4815,109 @@
       </c>
       <c r="AS16" s="7"/>
       <c r="AT16" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="6"/>
     </row>
-    <row r="17" spans="1:54" ht="289" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" ht="289" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="F17" s="5">
+        <v>888</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="H17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="5">
-        <v>888</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="L17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="P17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O17" s="5" t="s">
+      <c r="R17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T17" s="5">
+        <v>888</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="P17" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q17" s="7" t="s">
+      <c r="W17" s="5">
+        <v>888</v>
+      </c>
+      <c r="X17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="R17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="S17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T17" s="5">
-        <v>888</v>
-      </c>
-      <c r="U17" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V17" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="W17" s="5">
-        <v>888</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="Y17" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB17" s="5">
         <v>888</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AD17" s="5">
         <v>888</v>
@@ -4947,27 +4929,27 @@
         <v>888</v>
       </c>
       <c r="AG17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH17" s="7"/>
       <c r="AI17" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -4980,139 +4962,139 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="AU17" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AW17" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AW17" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="AX17" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="5">
+        <v>888</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="I18" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="5">
-        <v>888</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="L18" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="N18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="P18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="Q18" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R18" s="7">
+        <v>3</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="T18" s="5">
+        <v>888</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="W18" s="5">
+        <v>888</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="Q18" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T18" s="5">
-        <v>888</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="W18" s="5">
-        <v>888</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="Y18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG18" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM18" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN18" s="5"/>
       <c r="AO18" s="7"/>
@@ -5126,16 +5108,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT18" s="5" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5143,121 +5125,121 @@
       <c r="BA18" s="6"/>
       <c r="BB18" s="6"/>
     </row>
-    <row r="19" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="E19" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F19" s="5">
+        <v>888</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="H19" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="F19" s="5">
-        <v>888</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" s="7" t="s">
+      <c r="L19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19" s="7">
+        <v>7</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="N19" s="7" t="s">
+      <c r="P19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="U19" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="W19" s="5">
+        <v>888</v>
+      </c>
+      <c r="X19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="Y19" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="P19" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="T19" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="V19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="W19" s="5">
-        <v>888</v>
-      </c>
-      <c r="X19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="Y19" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AB19" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AK19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN19" s="5"/>
       <c r="AO19" s="7"/>
@@ -5271,144 +5253,144 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
       <c r="BA19" s="6"/>
       <c r="BB19" s="6"/>
     </row>
-    <row r="20" spans="1:54" ht="136" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="E20" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F20" s="5">
+        <v>888</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="I20" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="F20" s="5">
-        <v>888</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="L20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>233</v>
+        <v>11</v>
+      </c>
+      <c r="T20" s="5">
+        <v>888</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="W20" s="5">
         <v>888</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB20" s="5">
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG20" s="5">
         <v>888</v>
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AK20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5420,16 +5402,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT20" s="5" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="AU20" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AV20" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5437,152 +5419,152 @@
       <c r="BA20" s="6"/>
       <c r="BB20" s="6"/>
     </row>
-    <row r="21" spans="1:54" ht="272" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" ht="272" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F21" s="5">
+        <v>888</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="F21" s="5">
-        <v>888</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="Z21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB21" s="5">
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AG21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AH21" s="7"/>
       <c r="AI21" s="2" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="AJ21" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AK21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AU21" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV21" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AW21" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX21" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="AP21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="AT21" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="AU21" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="AV21" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="AW21" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="AX21" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
@@ -5593,43 +5575,43 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="E22" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="H22" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>136</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5638,28 +5620,28 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>25</v>
+        <v>97</v>
+      </c>
+      <c r="R22" s="7">
+        <v>3</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="W22" s="5">
         <v>888</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Y22" s="5">
         <v>888</v>
@@ -5674,19 +5656,19 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="AE22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AF22" s="4">
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5702,7 +5684,7 @@
         <v>888</v>
       </c>
       <c r="AM22" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN22" s="5"/>
       <c r="AO22" s="7"/>
@@ -5716,29 +5698,36 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AT22" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="AV22" s="7" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AW22" s="9" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="AX22" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>
       <c r="BB22" s="6"/>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="AH23" s="5"/>
+      <c r="AO23" s="5"/>
+      <c r="AS23" s="5"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5896,18 +5885,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5929,25 +5918,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix minor errors in formatting of data
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1354" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F5C7D54-2974-7D4F-BF90-8E5D5C29EBBE}"/>
+  <xr:revisionPtr revIDLastSave="1362" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD0D9325-E03C-DF47-946D-5919684B4F69}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="367">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -443,9 +443,6 @@
     <t>28</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -724,9 +721,6 @@
     <t>1 - 3</t>
   </si>
   <si>
-    <t>9 y 12</t>
-  </si>
-  <si>
     <t>4 - 6</t>
   </si>
   <si>
@@ -1171,6 +1165,9 @@
   </si>
   <si>
     <t>Specific p-value provided</t>
+  </si>
+  <si>
+    <t>9 and 12</t>
   </si>
 </sst>
 </file>
@@ -2044,9 +2041,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX23" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:AX23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}">
-    <filterColumn colId="17">
+    <filterColumn colId="13">
       <filters>
-        <filter val="3"/>
+        <filter val="6"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2446,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L5" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2476,151 +2473,151 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AN1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="AS1" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="AV1" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>286</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
@@ -2637,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2652,7 +2649,7 @@
         <v>107</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>14</v>
@@ -2667,7 +2664,7 @@
         <v>109</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
@@ -2676,7 +2673,7 @@
         <v>109</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2688,7 +2685,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>12</v>
@@ -2700,7 +2697,7 @@
         <v>13</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>14</v>
@@ -2712,13 +2709,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>14</v>
@@ -2728,19 +2725,19 @@
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="AJ2" s="5" t="s">
-        <v>352</v>
-      </c>
       <c r="AK2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2761,17 +2758,17 @@
         <v>16</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6"/>
     </row>
-    <row r="3" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -2791,13 +2788,13 @@
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>14</v>
@@ -2812,13 +2809,13 @@
         <v>109</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>219</v>
+        <v>366</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>74</v>
@@ -2833,22 +2830,22 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="W3" s="5">
         <v>888</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="Y3" s="5">
         <v>888</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AA3" s="5">
         <v>888</v>
@@ -2857,7 +2854,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>14</v>
@@ -2869,7 +2866,7 @@
         <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AH3" s="7" t="s">
         <v>25</v>
@@ -2907,10 +2904,10 @@
         <v>21</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AW3" s="9" t="s">
         <v>26</v>
@@ -2934,19 +2931,19 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F4" s="5">
         <v>888</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>14</v>
@@ -2961,7 +2958,7 @@
         <v>109</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
@@ -2973,16 +2970,16 @@
         <v>30</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>31</v>
@@ -2991,7 +2988,7 @@
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>14</v>
@@ -3006,10 +3003,10 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE4" s="5" t="s">
         <v>14</v>
@@ -3018,10 +3015,10 @@
         <v>888</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3040,7 +3037,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3052,16 +3049,16 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AW4" s="9" t="s">
         <v>32</v>
@@ -3073,7 +3070,7 @@
       <c r="BA4" s="6"/>
       <c r="BB4" s="6"/>
     </row>
-    <row r="5" spans="1:54" ht="85" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -3087,19 +3084,19 @@
         <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F5" s="5">
         <v>888</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>14</v>
@@ -3111,7 +3108,7 @@
         <v>14</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>109</v>
@@ -3129,13 +3126,13 @@
         <v>3</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>41</v>
@@ -3147,10 +3144,10 @@
         <v>42</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3159,13 +3156,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>14</v>
@@ -3178,16 +3175,16 @@
         <v>43</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3201,16 +3198,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AU5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3218,7 +3215,7 @@
       <c r="BA5" s="6"/>
       <c r="BB5" s="6"/>
     </row>
-    <row r="6" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>13</v>
       </c>
@@ -3232,19 +3229,19 @@
         <v>124</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F6" s="5">
         <v>888</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>125</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>14</v>
@@ -3258,14 +3255,14 @@
       <c r="M6" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>127</v>
+      <c r="N6" s="7">
+        <v>6</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>73</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>74</v>
@@ -3280,37 +3277,37 @@
         <v>888</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="W6" s="5">
         <v>888</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>14</v>
@@ -3323,13 +3320,13 @@
         <v>102</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>14</v>
@@ -3347,13 +3344,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3369,25 +3366,25 @@
         <v>123</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>139</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>14</v>
@@ -3417,25 +3414,25 @@
         <v>40</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T7" s="7" t="s">
         <v>109</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>14</v>
@@ -3447,10 +3444,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>14</v>
@@ -3466,13 +3463,13 @@
         <v>102</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>14</v>
@@ -3490,23 +3487,23 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
       <c r="BB7" s="6"/>
     </row>
-    <row r="8" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>16</v>
       </c>
@@ -3514,46 +3511,46 @@
         <v>123</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="5">
+        <v>888</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="5">
-        <v>888</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="L8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>127</v>
+        <v>215</v>
+      </c>
+      <c r="N8" s="7">
+        <v>6</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>73</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q8" s="7" t="s">
         <v>74</v>
@@ -3562,22 +3559,22 @@
         <v>40</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T8" s="7" t="s">
         <v>109</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="W8" s="5">
         <v>888</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>14</v>
@@ -3586,19 +3583,19 @@
         <v>14</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>14</v>
@@ -3611,13 +3608,13 @@
         <v>102</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>14</v>
@@ -3635,17 +3632,17 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
@@ -3656,34 +3653,34 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>105</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>14</v>
@@ -3692,19 +3689,19 @@
         <v>109</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>11</v>
@@ -3713,65 +3710,65 @@
         <v>888</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V9" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="W9" s="5">
+        <v>888</v>
+      </c>
+      <c r="X9" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="W9" s="5">
-        <v>888</v>
-      </c>
-      <c r="X9" s="5" t="s">
+      <c r="Y9" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AI9" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="Y9" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH9" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>160</v>
-      </c>
       <c r="AJ9" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3784,17 +3781,17 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
@@ -3805,34 +3802,34 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" s="5">
+        <v>888</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="F10" s="5">
-        <v>888</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>14</v>
@@ -3844,13 +3841,13 @@
         <v>109</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P10" s="7">
         <v>25</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="R10" s="7" t="s">
         <v>109</v>
@@ -3862,40 +3859,40 @@
         <v>888</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AG10" s="5" t="s">
         <v>14</v>
@@ -3905,13 +3902,13 @@
         <v>102</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>14</v>
@@ -3929,13 +3926,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3948,34 +3945,34 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F11" s="5">
+        <v>888</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F11" s="5">
-        <v>888</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>14</v>
@@ -3984,7 +3981,7 @@
         <v>109</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
@@ -3993,7 +3990,7 @@
         <v>109</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R11" s="7">
         <v>5</v>
@@ -4005,17 +4002,17 @@
         <v>888</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V11" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="W11" s="5">
+        <v>888</v>
+      </c>
+      <c r="X11" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="W11" s="5">
-        <v>888</v>
-      </c>
-      <c r="X11" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="Y11" s="5" t="s">
         <v>14</v>
       </c>
@@ -4029,13 +4026,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>14</v>
@@ -4048,13 +4045,13 @@
         <v>102</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>14</v>
@@ -4072,17 +4069,17 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
@@ -4093,34 +4090,34 @@
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="5">
+        <v>888</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="F12" s="5">
-        <v>888</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>14</v>
@@ -4144,98 +4141,98 @@
         <v>40</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T12" s="7" t="s">
         <v>109</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V12" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="W12" s="5">
+        <v>888</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AH12" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AI12" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="W12" s="5">
-        <v>888</v>
-      </c>
-      <c r="X12" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="Y12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC12" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="AD12" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="AE12" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="AF12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AH12" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI12" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="AJ12" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS12" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="AW12" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AP12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS12" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="AT12" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="AU12" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AV12" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="AW12" s="9" t="s">
+      <c r="AX12" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="AX12" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
@@ -4246,34 +4243,34 @@
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F13" s="5">
+        <v>888</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="F13" s="5">
-        <v>888</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>14</v>
@@ -4282,7 +4279,7 @@
         <v>23</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4291,28 +4288,28 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R13" s="7">
         <v>5</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T13" s="7" t="s">
         <v>109</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="W13" s="5">
         <v>888</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>14</v>
@@ -4321,19 +4318,19 @@
         <v>14</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>14</v>
@@ -4346,10 +4343,10 @@
         <v>43</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>14</v>
@@ -4359,34 +4356,34 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AP13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS13" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT13" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU13" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="AV13" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AW13" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="AP13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS13" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="AT13" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="AU13" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="AV13" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="AW13" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="AX13" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
@@ -4397,28 +4394,28 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>14</v>
@@ -4439,34 +4436,34 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="W14" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="X14" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="Y14" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z14" s="2" t="s">
         <v>14</v>
@@ -4478,13 +4475,13 @@
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF14" s="2" t="s">
         <v>14</v>
@@ -4494,40 +4491,40 @@
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AJ14" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AT14" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="AU14" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AK14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN14" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AP14" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="2" t="s">
+      <c r="AV14" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="AT14" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="AU14" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4561,7 +4558,7 @@
         <v>49</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>14</v>
@@ -4570,7 +4567,7 @@
         <v>50</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>40</v>
@@ -4585,19 +4582,19 @@
         <v>109</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T15" s="5" t="s">
         <v>109</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V15" s="5" t="s">
         <v>51</v>
@@ -4606,28 +4603,28 @@
         <v>888</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB15" s="5">
         <v>888</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF15" s="4" t="s">
         <v>14</v>
@@ -4640,10 +4637,10 @@
         <v>43</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>14</v>
@@ -4666,19 +4663,19 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AW15" s="9" t="s">
         <v>54</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
@@ -4704,16 +4701,16 @@
         <v>888</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>59</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>60</v>
@@ -4734,7 +4731,7 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R16" s="5" t="s">
         <v>109</v>
@@ -4746,7 +4743,7 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>62</v>
@@ -4770,13 +4767,13 @@
         <v>888</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF16" s="4" t="s">
         <v>14</v>
@@ -4789,20 +4786,20 @@
         <v>43</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4818,14 +4815,14 @@
         <v>65</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
@@ -4857,10 +4854,10 @@
         <v>71</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>72</v>
@@ -4869,7 +4866,7 @@
         <v>14</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>30</v>
@@ -4893,7 +4890,7 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V17" s="5" t="s">
         <v>75</v>
@@ -4905,7 +4902,7 @@
         <v>76</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>14</v>
@@ -4936,13 +4933,13 @@
         <v>43</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>14</v>
@@ -4962,10 +4959,10 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AU17" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV17" s="7" t="s">
         <v>77</v>
@@ -4980,12 +4977,12 @@
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="1:54" ht="119" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>18</v>
@@ -5000,22 +4997,22 @@
         <v>888</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>83</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>84</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>85</v>
@@ -5042,7 +5039,7 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V18" s="5" t="s">
         <v>88</v>
@@ -5054,25 +5051,25 @@
         <v>89</v>
       </c>
       <c r="Y18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>14</v>
@@ -5085,13 +5082,13 @@
         <v>43</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>14</v>
@@ -5108,16 +5105,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT18" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AU18" s="5" t="s">
         <v>90</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5139,7 +5136,7 @@
         <v>93</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F19" s="5">
         <v>888</v>
@@ -5151,7 +5148,7 @@
         <v>95</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J19" s="7" t="s">
         <v>14</v>
@@ -5163,7 +5160,7 @@
         <v>14</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N19" s="7">
         <v>7</v>
@@ -5181,13 +5178,13 @@
         <v>40</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T19" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V19" s="5" t="s">
         <v>88</v>
@@ -5199,25 +5196,25 @@
         <v>99</v>
       </c>
       <c r="Y19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z19" s="4">
         <v>888</v>
       </c>
       <c r="AA19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AB19" s="5" t="s">
         <v>100</v>
       </c>
       <c r="AC19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF19" s="4" t="s">
         <v>14</v>
@@ -5230,13 +5227,13 @@
         <v>102</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>14</v>
@@ -5253,19 +5250,19 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT19" s="5" t="s">
         <v>94</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV19" s="7" t="s">
         <v>103</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
@@ -5286,19 +5283,19 @@
         <v>106</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F20" s="5">
         <v>888</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>107</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J20" s="7" t="s">
         <v>14</v>
@@ -5310,10 +5307,10 @@
         <v>14</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
@@ -5334,10 +5331,10 @@
         <v>888</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="W20" s="5">
         <v>888</v>
@@ -5346,7 +5343,7 @@
         <v>110</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>14</v>
@@ -5358,13 +5355,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>14</v>
@@ -5377,13 +5374,13 @@
         <v>43</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>14</v>
@@ -5402,10 +5399,10 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT20" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="AU20" s="5" t="s">
         <v>111</v>
@@ -5419,12 +5416,12 @@
       <c r="BA20" s="6"/>
       <c r="BB20" s="6"/>
     </row>
-    <row r="21" spans="1:54" ht="272" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:54" ht="272" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>105</v>
@@ -5433,19 +5430,19 @@
         <v>114</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F21" s="5">
         <v>888</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>95</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J21" s="7" t="s">
         <v>14</v>
@@ -5459,8 +5456,8 @@
       <c r="M21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="N21" s="7" t="s">
-        <v>85</v>
+      <c r="N21" s="7">
+        <v>6</v>
       </c>
       <c r="O21" s="5" t="s">
         <v>116</v>
@@ -5478,22 +5475,22 @@
         <v>11</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>14</v>
@@ -5505,35 +5502,35 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AG21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AH21" s="7"/>
       <c r="AI21" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="AJ21" s="5" t="s">
         <v>118</v>
       </c>
       <c r="AK21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
@@ -5549,16 +5546,16 @@
         <v>888</v>
       </c>
       <c r="AS21" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT21" s="5" t="s">
         <v>119</v>
       </c>
       <c r="AU21" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AV21" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AW21" s="9" t="s">
         <v>121</v>
@@ -5570,33 +5567,33 @@
       <c r="BA21" s="6"/>
       <c r="BB21" s="6"/>
     </row>
-    <row r="22" spans="1:54" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>14</v>
@@ -5608,10 +5605,10 @@
         <v>14</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5626,22 +5623,22 @@
         <v>3</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="W22" s="5">
         <v>888</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y22" s="5">
         <v>888</v>
@@ -5656,19 +5653,19 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD22" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AE22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG22" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="AE22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF22" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG22" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5698,22 +5695,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AT22" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU22" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="AV22" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX22" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="AU22" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="AV22" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="AW22" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="AX22" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>
@@ -5885,18 +5882,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5918,25 +5915,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove "and" from list of values
This was done in order to facilitate the splitting of string and count them.
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1362" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AD0D9325-E03C-DF47-946D-5919684B4F69}"/>
+  <xr:revisionPtr revIDLastSave="1373" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDE28069-9E1F-1B47-B043-EAD7745FE878}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="370">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Examine the effectiveness of word structure practice using application software with fourth grade readers.</t>
-  </si>
-  <si>
-    <t>Word identification skills, fluency, vocabulary, and comprehension</t>
   </si>
   <si>
     <t>Quasi-experimental study</t>
@@ -522,9 +519,6 @@
     <t>A Design Case Study of a Tangible System Supporting Young English Language Learners</t>
   </si>
   <si>
-    <t>Reading and spelling</t>
-  </si>
-  <si>
     <t>Case study design with a pre- and post-test.</t>
   </si>
   <si>
@@ -990,15 +984,9 @@
     <t>Determine whether the final version website with games based on these five media properties and played at home could meaningfully promote literacy development among low- and middle-SES preschool and kindergarten students</t>
   </si>
   <si>
-    <t>Phonological skills and reading skills</t>
-  </si>
-  <si>
     <t>Phonological Skills</t>
   </si>
   <si>
-    <t>Syllabic awareness and word recognition</t>
-  </si>
-  <si>
     <t>Reading comprehension, Passage comprehension, Word decoding, Sight word reading, and Pseudoword reading</t>
   </si>
   <si>
@@ -1020,12 +1008,6 @@
     <t>Written word recognition, Written word naming, and phonological skills</t>
   </si>
   <si>
-    <t>phonemic skills, phonics, fluency, vocabulary, and reading comprehension</t>
-  </si>
-  <si>
-    <t>Letter identification, letter sound knowledge, letter sequencing, alliteration, rhyming, phonics, vocabulary, print awareness, phonic awareness, and phonemic skills</t>
-  </si>
-  <si>
     <t>Letter sound knowledge, phonemic skills, phoneme-blending, word reading, rapid automatized naming, vocabulary</t>
   </si>
   <si>
@@ -1168,6 +1150,33 @@
   </si>
   <si>
     <t>9 and 12</t>
+  </si>
+  <si>
+    <t>Syllabic awareness, word recognition</t>
+  </si>
+  <si>
+    <t>Reading, spelling</t>
+  </si>
+  <si>
+    <t>Reading comprehension, Passage comprehension, Word decoding, Sight word reading, Pseudoword reading</t>
+  </si>
+  <si>
+    <t>Written word recognition, Written word naming, phonological skills</t>
+  </si>
+  <si>
+    <t>Phonological skills, reading skills</t>
+  </si>
+  <si>
+    <t>vocabulary, word reading, spelling, phonological skills, rhyme awareness</t>
+  </si>
+  <si>
+    <t>Word identification skills, fluency, vocabulary, comprehension</t>
+  </si>
+  <si>
+    <t>phonemic skills, phonics, fluency, vocabulary, reading comprehension</t>
+  </si>
+  <si>
+    <t>Letter identification, letter sound knowledge, letter sequencing, alliteration, rhyming, phonics, vocabulary, print awareness, phonic awareness, phonemic skills</t>
   </si>
 </sst>
 </file>
@@ -2040,13 +2049,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:AX23" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
-  <autoFilter ref="A1:AX23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="6"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AX23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AX22">
     <sortCondition ref="B1:B22"/>
   </sortState>
@@ -2443,16 +2446,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="G21" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" style="6" customWidth="1"/>
-    <col min="2" max="5" width="28.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="139.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="6" width="28.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="139.33203125" style="2" customWidth="1"/>
     <col min="8" max="33" width="28.5" style="2" customWidth="1"/>
     <col min="34" max="34" width="8.83203125" style="6"/>
     <col min="35" max="40" width="28.5" style="2" customWidth="1"/>
@@ -2473,157 +2475,157 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="AN1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="AS1" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="AV1" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>284</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
       <c r="BB1" s="6"/>
     </row>
-    <row r="2" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>7</v>
       </c>
@@ -2634,7 +2636,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2646,10 +2648,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>14</v>
@@ -2661,19 +2663,19 @@
         <v>14</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2685,7 +2687,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>12</v>
@@ -2697,7 +2699,7 @@
         <v>13</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>14</v>
@@ -2709,13 +2711,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>14</v>
@@ -2725,19 +2727,19 @@
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2758,17 +2760,17 @@
         <v>16</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
       <c r="BB2" s="6"/>
     </row>
-    <row r="3" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>8</v>
       </c>
@@ -2788,13 +2790,13 @@
         <v>888</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>14</v>
@@ -2806,19 +2808,19 @@
         <v>14</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R3" s="7">
         <v>3</v>
@@ -2830,22 +2832,22 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="W3" s="5">
         <v>888</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="Y3" s="5">
         <v>888</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AA3" s="5">
         <v>888</v>
@@ -2854,7 +2856,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>14</v>
@@ -2866,7 +2868,7 @@
         <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="AH3" s="7" t="s">
         <v>25</v>
@@ -2904,10 +2906,10 @@
         <v>21</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AW3" s="9" t="s">
         <v>26</v>
@@ -2917,7 +2919,7 @@
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
     </row>
-    <row r="4" spans="1:54" ht="372" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="372" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>9</v>
       </c>
@@ -2931,19 +2933,19 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F4" s="5">
         <v>888</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>14</v>
@@ -2955,31 +2957,31 @@
         <v>14</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>30</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>31</v>
@@ -2988,7 +2990,7 @@
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>14</v>
@@ -3003,22 +3005,22 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>888</v>
+      </c>
+      <c r="AG4" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="AD4" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>888</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="AH4" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3037,7 +3039,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3049,16 +3051,16 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AW4" s="9" t="s">
         <v>32</v>
@@ -3070,7 +3072,7 @@
       <c r="BA4" s="6"/>
       <c r="BB4" s="6"/>
     </row>
-    <row r="5" spans="1:54" ht="85" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>11</v>
       </c>
@@ -3084,19 +3086,19 @@
         <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="F5" s="5">
         <v>888</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>307</v>
+        <v>365</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>14</v>
@@ -3108,10 +3110,10 @@
         <v>14</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
@@ -3126,13 +3128,13 @@
         <v>3</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>41</v>
@@ -3144,10 +3146,10 @@
         <v>42</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3156,13 +3158,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>14</v>
@@ -3175,16 +3177,16 @@
         <v>43</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3198,16 +3200,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="AU5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3220,52 +3222,52 @@
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" s="5">
+        <v>888</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F6" s="5">
-        <v>888</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>126</v>
-      </c>
       <c r="L6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N6" s="7">
         <v>6</v>
       </c>
       <c r="O6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="R6" s="7">
         <v>5</v>
@@ -3277,37 +3279,37 @@
         <v>888</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="W6" s="5">
         <v>888</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>14</v>
@@ -3317,16 +3319,16 @@
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>14</v>
@@ -3344,13 +3346,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3358,39 +3360,39 @@
       <c r="BA6" s="6"/>
       <c r="BB6" s="6"/>
     </row>
-    <row r="7" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>138</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>14</v>
@@ -3402,37 +3404,37 @@
         <v>7</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>14</v>
@@ -3444,10 +3446,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>14</v>
@@ -3460,16 +3462,16 @@
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>14</v>
@@ -3487,17 +3489,17 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
@@ -3508,73 +3510,73 @@
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="5">
+        <v>888</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="F8" s="5">
-        <v>888</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="L8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N8" s="7">
         <v>6</v>
       </c>
       <c r="O8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="W8" s="5">
         <v>888</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>14</v>
@@ -3583,19 +3585,19 @@
         <v>14</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>14</v>
@@ -3605,16 +3607,16 @@
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>14</v>
@@ -3632,76 +3634,76 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
       <c r="BB8" s="6"/>
     </row>
-    <row r="9" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="I9" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="L9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>11</v>
@@ -3710,65 +3712,65 @@
         <v>888</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V9" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="W9" s="5">
+        <v>888</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI9" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="W9" s="5">
-        <v>888</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH9" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="AI9" s="5" t="s">
-        <v>159</v>
-      </c>
       <c r="AJ9" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3781,55 +3783,55 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
     </row>
-    <row r="10" spans="1:54" ht="170" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="170" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F10" s="5">
+        <v>888</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="I10" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="F10" s="5">
-        <v>888</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>14</v>
@@ -3838,19 +3840,19 @@
         <v>23</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="P10" s="7">
         <v>25</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>11</v>
@@ -3859,56 +3861,56 @@
         <v>888</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="W10" s="5">
         <v>888</v>
       </c>
       <c r="X10" s="5" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AG10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>14</v>
@@ -3926,13 +3928,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3940,57 +3942,57 @@
       <c r="BA10" s="6"/>
       <c r="BB10" s="6"/>
     </row>
-    <row r="11" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F11" s="5">
+        <v>888</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="I11" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F11" s="5">
-        <v>888</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>184</v>
-      </c>
       <c r="L11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R11" s="7">
         <v>5</v>
@@ -4002,16 +4004,16 @@
         <v>888</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="W11" s="5">
         <v>888</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>14</v>
@@ -4026,13 +4028,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>14</v>
@@ -4042,16 +4044,16 @@
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>14</v>
@@ -4069,55 +4071,55 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
       <c r="BB11" s="6"/>
     </row>
-    <row r="12" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F12" s="5">
+        <v>888</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="I12" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="F12" s="5">
-        <v>888</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>14</v>
@@ -4129,34 +4131,34 @@
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="R12" s="7" t="s">
         <v>40</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="W12" s="5">
         <v>888</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>14</v>
@@ -4171,13 +4173,13 @@
         <v>888</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF12" s="4" t="s">
         <v>14</v>
@@ -4186,91 +4188,91 @@
         <v>888</v>
       </c>
       <c r="AH12" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AI12" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS12" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AT12" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="AU12" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="AW12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="AX12" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="AP12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR12" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS12" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AT12" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AU12" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="AV12" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="AW12" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="AX12" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
       <c r="BB12" s="6"/>
     </row>
-    <row r="13" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F13" s="5">
+        <v>888</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="F13" s="5">
-        <v>888</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>14</v>
@@ -4279,7 +4281,7 @@
         <v>23</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4288,28 +4290,28 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R13" s="7">
         <v>5</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="W13" s="5">
         <v>888</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>14</v>
@@ -4318,19 +4320,19 @@
         <v>14</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>14</v>
@@ -4343,10 +4345,10 @@
         <v>43</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>14</v>
@@ -4356,66 +4358,66 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="AP13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS13" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AT13" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AU13" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AV13" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AW13" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="AP13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR13" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS13" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AT13" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AU13" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="AV13" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AW13" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="AX13" s="7" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
       <c r="BB13" s="6"/>
     </row>
-    <row r="14" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>14</v>
@@ -4427,7 +4429,7 @@
         <v>14</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4436,34 +4438,34 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V14" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="X14" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="W14" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="Y14" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z14" s="2" t="s">
         <v>14</v>
@@ -4475,13 +4477,13 @@
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF14" s="2" t="s">
         <v>14</v>
@@ -4491,40 +4493,40 @@
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AK14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AN14" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="AP14" s="2" t="s">
+      <c r="AT14" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="AV14" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AT14" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="AU14" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4532,7 +4534,7 @@
       <c r="BA14" s="6"/>
       <c r="BB14" s="6"/>
     </row>
-    <row r="15" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -4552,95 +4554,95 @@
         <v>888</v>
       </c>
       <c r="G15" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>50</v>
-      </c>
       <c r="L15" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>40</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="W15" s="5">
+        <v>888</v>
+      </c>
+      <c r="X15" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE15" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG15" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="W15" s="5">
-        <v>888</v>
-      </c>
-      <c r="X15" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="Y15" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA15" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AB15" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC15" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD15" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AE15" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG15" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>14</v>
@@ -4650,7 +4652,7 @@
       </c>
       <c r="AN15" s="5"/>
       <c r="AO15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AP15" s="5">
         <v>888</v>
@@ -4663,66 +4665,66 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AW15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
       <c r="BB15" s="6"/>
     </row>
-    <row r="16" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="102" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="5">
+        <v>888</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="5">
-        <v>888</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="L16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="N16" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
@@ -4731,10 +4733,10 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>11</v>
@@ -4743,63 +4745,63 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="V16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="W16" s="5">
+        <v>888</v>
+      </c>
+      <c r="X16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="W16" s="5">
-        <v>888</v>
-      </c>
-      <c r="X16" s="5" t="s">
+      <c r="Y16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC16" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD16" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG16" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB16" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC16" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AE16" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="AH16" s="7"/>
       <c r="AI16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4812,73 +4814,73 @@
       </c>
       <c r="AS16" s="7"/>
       <c r="AT16" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
       <c r="BB16" s="6"/>
     </row>
-    <row r="17" spans="1:54" ht="289" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:54" ht="289" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="5">
+        <v>888</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="5">
-        <v>888</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="L17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="O17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>40</v>
@@ -4890,19 +4892,19 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="W17" s="5">
+        <v>888</v>
+      </c>
+      <c r="X17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="W17" s="5">
-        <v>888</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="Y17" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>14</v>
@@ -4933,20 +4935,20 @@
         <v>43</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -4959,75 +4961,75 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="AU17" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV17" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AW17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AX17" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="AX17" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
       <c r="BB17" s="6"/>
     </row>
-    <row r="18" spans="1:54" ht="119" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:54" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="5">
+        <v>888</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="5">
-        <v>888</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="P18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="P18" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="Q18" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R18" s="7">
         <v>3</v>
@@ -5039,37 +5041,37 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="W18" s="5">
+        <v>888</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="W18" s="5">
-        <v>888</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="Y18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>14</v>
@@ -5082,13 +5084,13 @@
         <v>43</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>14</v>
@@ -5105,16 +5107,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AT18" s="5" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5122,54 +5124,54 @@
       <c r="BA18" s="6"/>
       <c r="BB18" s="6"/>
     </row>
-    <row r="19" spans="1:54" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F19" s="5">
+        <v>888</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F19" s="5">
-        <v>888</v>
-      </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="L19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N19" s="7">
         <v>7</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q19" s="7" t="s">
         <v>39</v>
@@ -5178,62 +5180,62 @@
         <v>40</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T19" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W19" s="5">
         <v>888</v>
       </c>
       <c r="X19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="Y19" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AB19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>14</v>
@@ -5250,79 +5252,79 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
       <c r="BA19" s="6"/>
       <c r="BB19" s="6"/>
     </row>
-    <row r="20" spans="1:54" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:54" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F20" s="5">
+        <v>888</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="F20" s="5">
-        <v>888</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="L20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>11</v>
@@ -5331,19 +5333,19 @@
         <v>888</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="W20" s="5">
         <v>888</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>14</v>
@@ -5355,13 +5357,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>14</v>
@@ -5374,20 +5376,20 @@
         <v>43</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5399,16 +5401,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AT20" s="5" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="AU20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AV20" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="AV20" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5421,52 +5423,52 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F21" s="5">
+        <v>888</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F21" s="5">
-        <v>888</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="L21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N21" s="7">
         <v>6</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>40</v>
@@ -5475,22 +5477,22 @@
         <v>11</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>14</v>
@@ -5502,98 +5504,98 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AG21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AH21" s="7"/>
       <c r="AI21" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="AJ21" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AK21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AT21" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU21" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AV21" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AW21" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AP21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AT21" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="AU21" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AV21" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="AW21" s="9" t="s">
+      <c r="AX21" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="AX21" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
       <c r="BB21" s="6"/>
     </row>
-    <row r="22" spans="1:54" ht="102" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:54" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>14</v>
@@ -5605,10 +5607,10 @@
         <v>14</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5617,28 +5619,28 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R22" s="7">
         <v>3</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="W22" s="5">
         <v>888</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Y22" s="5">
         <v>888</v>
@@ -5653,10 +5655,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>14</v>
@@ -5665,7 +5667,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5695,28 +5697,28 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AT22" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU22" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AV22" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX22" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="AU22" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="AV22" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AW22" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="AX22" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>
       <c r="BB22" s="6"/>
     </row>
-    <row r="23" spans="1:54" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -5736,6 +5738,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100099F4328816B724ABB65184634EDCB7A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1bd4f96a89e0bf3f95a675bb701c673a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17c5fd42-a044-4f07-a556-35a9304bdabd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e0b4ba08ccf20d12e7907069f81316d" ns2:_="">
     <xsd:import namespace="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
@@ -5881,12 +5889,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5897,6 +5899,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8BD45EC-7A23-43D7-AAF9-EC9E08ECF9A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5914,22 +5932,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix the recoding of "skills to impact"
</commit_message>
<xml_diff>
--- a/Datos/article_data_2019-09-14.xlsx
+++ b/Datos/article_data_2019-09-14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1373" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDE28069-9E1F-1B47-B043-EAD7745FE878}"/>
+  <xr:revisionPtr revIDLastSave="1469" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDC1DD59-0A89-CC45-8918-F29370F266C9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16120" yWindow="0" windowWidth="15880" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="367">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -267,9 +267,6 @@
     <t>Determine the effects of a computerized training program on the reading skills of normal readers, poor decoders, poor comprehenders, and general poor readers (inferred).</t>
   </si>
   <si>
-    <t>Silent word reading, reading fluency, listening comprehension, reading comprehension</t>
-  </si>
-  <si>
     <t>pretest-posttest with multiple comparison groups</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
 program using computer-assisted reciprocal peer tutoring with embedded audio prompting</t>
   </si>
   <si>
-    <t>phoneme segmentation fluency</t>
-  </si>
-  <si>
     <t>Multiple probe across students design</t>
   </si>
   <si>
@@ -469,9 +463,6 @@
   </si>
   <si>
     <t>This was a SSD</t>
-  </si>
-  <si>
-    <t>Word recognition</t>
   </si>
   <si>
     <t>Classical training design involving three phases (pre-test, training, post-test)</t>
@@ -984,33 +975,15 @@
     <t>Determine whether the final version website with games based on these five media properties and played at home could meaningfully promote literacy development among low- and middle-SES preschool and kindergarten students</t>
   </si>
   <si>
-    <t>Phonological Skills</t>
-  </si>
-  <si>
     <t>Reading comprehension, Passage comprehension, Word decoding, Sight word reading, and Pseudoword reading</t>
   </si>
   <si>
-    <t>Sight-word reading</t>
-  </si>
-  <si>
-    <t>Written word recognition, Listening comprehension, Reading comprehension, decoding skills, phonological skills, decoding fluency, vocabulary, comprehension monitoring</t>
-  </si>
-  <si>
     <t>vocabulary, word reading, spelling, phonological skills, and rhyme awareness</t>
   </si>
   <si>
-    <t>Decoding, Phonological skills, Naming speed, Spelling</t>
-  </si>
-  <si>
-    <t>phonological skills, letter name knowledge, letter sound knowledge, rapid automatized naming, word reading, pseudowords reading, frequent word reading</t>
-  </si>
-  <si>
     <t>Written word recognition, Written word naming, and phonological skills</t>
   </si>
   <si>
-    <t>Letter sound knowledge, phonemic skills, phoneme-blending, word reading, rapid automatized naming, vocabulary</t>
-  </si>
-  <si>
     <t>Design_coded</t>
   </si>
   <si>
@@ -1110,9 +1083,6 @@
     <t>Word recognition, aloud word reading, and word spelling</t>
   </si>
   <si>
-    <t>Silent word reading, aloud word reading, reading comprehension</t>
-  </si>
-  <si>
     <t xml:space="preserve">Listening comprehension task, Silent word reading task, aloud word reading and Reading Comprehension. </t>
   </si>
   <si>
@@ -1152,38 +1122,59 @@
     <t>9 and 12</t>
   </si>
   <si>
-    <t>Syllabic awareness, word recognition</t>
-  </si>
-  <si>
-    <t>Reading, spelling</t>
-  </si>
-  <si>
-    <t>Reading comprehension, Passage comprehension, Word decoding, Sight word reading, Pseudoword reading</t>
-  </si>
-  <si>
-    <t>Written word recognition, Written word naming, phonological skills</t>
-  </si>
-  <si>
-    <t>Phonological skills, reading skills</t>
-  </si>
-  <si>
-    <t>vocabulary, word reading, spelling, phonological skills, rhyme awareness</t>
-  </si>
-  <si>
-    <t>Word identification skills, fluency, vocabulary, comprehension</t>
-  </si>
-  <si>
-    <t>phonemic skills, phonics, fluency, vocabulary, reading comprehension</t>
-  </si>
-  <si>
-    <t>Letter identification, letter sound knowledge, letter sequencing, alliteration, rhyming, phonics, vocabulary, print awareness, phonic awareness, phonemic skills</t>
+    <t>phonological skills</t>
+  </si>
+  <si>
+    <t>word reading</t>
+  </si>
+  <si>
+    <t>Phonological skills, word reading</t>
+  </si>
+  <si>
+    <t>Word reading</t>
+  </si>
+  <si>
+    <t>Word reading, Reading comprehension</t>
+  </si>
+  <si>
+    <t>Reading comprehension, word reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> word reading, Reading comprehension, phonological skills, vocabulary</t>
+  </si>
+  <si>
+    <t>Phonological skills, reading fluency, vocabulary, reading comprehension</t>
+  </si>
+  <si>
+    <t>word reading, reading fluency, reading comprehension</t>
+  </si>
+  <si>
+    <t>phonics, phonological skills, word reading, rapid automatized naming, vocabulary</t>
+  </si>
+  <si>
+    <t>phonics, phonological skills, vocabulary</t>
+  </si>
+  <si>
+    <t>phonological skills, phonics, rapid automatized naming, word reading</t>
+  </si>
+  <si>
+    <t>vocabulary, word reading, spelling, phonological skills</t>
+  </si>
+  <si>
+    <t>Word reading, reading fluency, vocabulary, reading comprehension</t>
+  </si>
+  <si>
+    <t>Phonological skills, reading skills (not specified)</t>
+  </si>
+  <si>
+    <t>Reading skills (not specified), spelling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1197,16 +1188,29 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1214,11 +1218,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1234,6 +1249,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2446,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G21" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="G5" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2475,151 +2492,151 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AJ1" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO1" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="AK1" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="AL1" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="AS1" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="AU1" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="AV1" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="AW1" s="5" t="s">
-        <v>282</v>
-      </c>
       <c r="AX1" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
@@ -2636,7 +2653,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -2644,14 +2661,14 @@
       <c r="F2" s="5">
         <v>888</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>14</v>
@@ -2663,19 +2680,19 @@
         <v>14</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="R2" s="7">
         <v>5</v>
@@ -2687,7 +2704,7 @@
         <v>888</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V2" s="5" t="s">
         <v>12</v>
@@ -2699,7 +2716,7 @@
         <v>13</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>14</v>
@@ -2711,13 +2728,13 @@
         <v>888</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF2" s="4" t="s">
         <v>14</v>
@@ -2727,19 +2744,19 @@
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="5" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM2" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AN2" s="5"/>
       <c r="AO2" s="7"/>
@@ -2760,11 +2777,11 @@
         <v>16</v>
       </c>
       <c r="AV2" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AW2" s="9"/>
       <c r="AX2" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AZ2" s="6"/>
       <c r="BA2" s="6"/>
@@ -2789,14 +2806,14 @@
       <c r="F3" s="5">
         <v>888</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>307</v>
+      <c r="G3" s="12" t="s">
+        <v>354</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>14</v>
@@ -2808,19 +2825,19 @@
         <v>14</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R3" s="7">
         <v>3</v>
@@ -2832,22 +2849,22 @@
         <v>888</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="W3" s="5">
         <v>888</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="Y3" s="5">
         <v>888</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AA3" s="5">
         <v>888</v>
@@ -2856,7 +2873,7 @@
         <v>888</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD3" s="5" t="s">
         <v>14</v>
@@ -2868,7 +2885,7 @@
         <v>888</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AH3" s="7" t="s">
         <v>25</v>
@@ -2906,10 +2923,10 @@
         <v>21</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV3" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AW3" s="9" t="s">
         <v>26</v>
@@ -2933,19 +2950,19 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F4" s="5">
         <v>888</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>305</v>
+      <c r="G4" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>14</v>
@@ -2957,31 +2974,31 @@
         <v>14</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>30</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>31</v>
@@ -2990,7 +3007,7 @@
         <v>888</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>14</v>
@@ -3005,10 +3022,10 @@
         <v>888</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE4" s="5" t="s">
         <v>14</v>
@@ -3017,10 +3034,10 @@
         <v>888</v>
       </c>
       <c r="AG4" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AH4" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AI4" s="5">
         <v>888</v>
@@ -3039,7 +3056,7 @@
       </c>
       <c r="AN4" s="5"/>
       <c r="AO4" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AP4" s="5">
         <v>888</v>
@@ -3051,16 +3068,16 @@
         <v>888</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT4" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AU4" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AW4" s="9" t="s">
         <v>32</v>
@@ -3086,19 +3103,19 @@
         <v>36</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F5" s="5">
         <v>888</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="12" t="s">
         <v>365</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>14</v>
@@ -3110,10 +3127,10 @@
         <v>14</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>9</v>
@@ -3128,13 +3145,13 @@
         <v>3</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T5" s="7" t="s">
         <v>40</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>41</v>
@@ -3146,10 +3163,10 @@
         <v>42</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AA5" s="5">
         <v>888</v>
@@ -3158,13 +3175,13 @@
         <v>888</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>14</v>
@@ -3177,16 +3194,16 @@
         <v>43</v>
       </c>
       <c r="AJ5" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AN5" s="5"/>
       <c r="AO5" s="7"/>
@@ -3200,16 +3217,16 @@
         <v>888</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT5" s="5" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="AU5" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="AW5" s="9"/>
       <c r="AX5" s="7"/>
@@ -3222,52 +3239,52 @@
         <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="F6" s="5">
+        <v>888</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F6" s="5">
-        <v>888</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="L6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N6" s="7">
         <v>6</v>
       </c>
       <c r="O6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="R6" s="7">
         <v>5</v>
@@ -3279,37 +3296,37 @@
         <v>888</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="W6" s="5">
         <v>888</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AB6" s="5">
         <v>888</v>
       </c>
       <c r="AC6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF6" s="4" t="s">
         <v>14</v>
@@ -3319,16 +3336,16 @@
       </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ6" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM6" s="5" t="s">
         <v>14</v>
@@ -3346,13 +3363,13 @@
       </c>
       <c r="AS6" s="7"/>
       <c r="AT6" s="5" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="AU6" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV6" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AW6" s="9"/>
       <c r="AX6" s="7"/>
@@ -3365,34 +3382,34 @@
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="F7" s="5">
         <v>888</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>136</v>
+      <c r="G7" s="12" t="s">
+        <v>352</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>14</v>
@@ -3404,37 +3421,37 @@
         <v>7</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P7" s="7">
         <v>6</v>
       </c>
       <c r="Q7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="W7" s="5">
         <v>888</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>14</v>
@@ -3446,10 +3463,10 @@
         <v>888</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE7" s="5" t="s">
         <v>14</v>
@@ -3462,16 +3479,16 @@
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM7" s="5" t="s">
         <v>14</v>
@@ -3489,17 +3506,17 @@
       </c>
       <c r="AS7" s="7"/>
       <c r="AT7" s="5" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV7" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="AW7" s="9"/>
       <c r="AX7" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
@@ -3510,73 +3527,73 @@
         <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F8" s="5">
         <v>888</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>347</v>
+      <c r="G8" s="11" t="s">
+        <v>355</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N8" s="7">
         <v>6</v>
       </c>
       <c r="O8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q8" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>40</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="W8" s="5">
         <v>888</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="Y8" s="5" t="s">
         <v>14</v>
@@ -3585,19 +3602,19 @@
         <v>14</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AB8" s="5">
         <v>888</v>
       </c>
       <c r="AC8" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF8" s="4" t="s">
         <v>14</v>
@@ -3607,16 +3624,16 @@
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ8" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM8" s="5" t="s">
         <v>14</v>
@@ -3634,17 +3651,17 @@
       </c>
       <c r="AS8" s="7"/>
       <c r="AT8" s="5" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV8" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="AW8" s="9"/>
       <c r="AX8" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
@@ -3655,55 +3672,55 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" s="5">
+        <v>888</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="L9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="F9" s="5">
-        <v>888</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>11</v>
@@ -3712,65 +3729,65 @@
         <v>888</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="W9" s="5">
         <v>888</v>
       </c>
       <c r="X9" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>888</v>
+      </c>
+      <c r="Z9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>888</v>
+      </c>
+      <c r="AC9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="Y9" s="5">
-        <v>888</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>888</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH9" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="AI9" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AJ9" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK9" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL9" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="AP9" s="5">
         <v>888</v>
@@ -3783,17 +3800,17 @@
       </c>
       <c r="AS9" s="7"/>
       <c r="AT9" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AU9" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="AW9" s="9"/>
       <c r="AX9" s="7" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
@@ -3804,34 +3821,34 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F10" s="5">
         <v>888</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>363</v>
+      <c r="G10" s="11" t="s">
+        <v>356</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>14</v>
@@ -3840,19 +3857,19 @@
         <v>23</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P10" s="7">
         <v>25</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S10" s="5" t="s">
         <v>11</v>
@@ -3861,56 +3878,56 @@
         <v>888</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V10" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="W10" s="5">
+        <v>888</v>
+      </c>
+      <c r="X10" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="W10" s="5">
-        <v>888</v>
-      </c>
-      <c r="X10" s="5" t="s">
-        <v>339</v>
-      </c>
       <c r="Y10" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AB10" s="5">
         <v>888</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF10" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AG10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AH10" s="7"/>
       <c r="AI10" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ10" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL10" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM10" s="5" t="s">
         <v>14</v>
@@ -3928,13 +3945,13 @@
       </c>
       <c r="AS10" s="7"/>
       <c r="AT10" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="AU10" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV10" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AW10" s="9"/>
       <c r="AX10" s="7"/>
@@ -3947,52 +3964,52 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="5">
+        <v>888</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="F11" s="5">
-        <v>888</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>182</v>
-      </c>
       <c r="L11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="R11" s="7">
         <v>5</v>
@@ -4004,16 +4021,16 @@
         <v>888</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="W11" s="5">
         <v>888</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Y11" s="5" t="s">
         <v>14</v>
@@ -4028,13 +4045,13 @@
         <v>888</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD11" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE11" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF11" s="4" t="s">
         <v>14</v>
@@ -4044,16 +4061,16 @@
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK11" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM11" s="5" t="s">
         <v>14</v>
@@ -4071,17 +4088,17 @@
       </c>
       <c r="AS11" s="7"/>
       <c r="AT11" s="4" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="AU11" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV11" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="AW11" s="9"/>
       <c r="AX11" s="7" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
@@ -4092,34 +4109,34 @@
         <v>19</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="5">
+        <v>888</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" s="5">
-        <v>888</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>14</v>
@@ -4131,34 +4148,34 @@
         <v>7</v>
       </c>
       <c r="O12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q12" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="R12" s="7" t="s">
         <v>40</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="W12" s="5">
         <v>888</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="Y12" s="5" t="s">
         <v>14</v>
@@ -4173,13 +4190,13 @@
         <v>888</v>
       </c>
       <c r="AC12" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF12" s="4" t="s">
         <v>14</v>
@@ -4188,26 +4205,26 @@
         <v>888</v>
       </c>
       <c r="AH12" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AI12" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AJ12" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK12" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL12" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AP12" s="5">
         <v>888</v>
@@ -4219,22 +4236,22 @@
         <v>888</v>
       </c>
       <c r="AS12" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AU12" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="AW12" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="AV12" s="9" t="s">
+      <c r="AX12" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="AW12" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="AX12" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
@@ -4245,34 +4262,34 @@
         <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F13" s="5">
+        <v>888</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="F13" s="5">
-        <v>888</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>14</v>
@@ -4281,7 +4298,7 @@
         <v>23</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>9</v>
@@ -4290,28 +4307,28 @@
         <v>60</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="R13" s="7">
         <v>5</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="W13" s="5">
         <v>888</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="Y13" s="5" t="s">
         <v>14</v>
@@ -4320,19 +4337,19 @@
         <v>14</v>
       </c>
       <c r="AA13" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AC13" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD13" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE13" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>14</v>
@@ -4345,10 +4362,10 @@
         <v>43</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK13" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL13" s="5" t="s">
         <v>14</v>
@@ -4358,7 +4375,7 @@
       </c>
       <c r="AN13" s="5"/>
       <c r="AO13" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AP13" s="5">
         <v>888</v>
@@ -4370,22 +4387,22 @@
         <v>888</v>
       </c>
       <c r="AS13" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT13" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AU13" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="AV13" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AW13" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AX13" s="7" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
@@ -4396,28 +4413,28 @@
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C14" s="2">
         <v>2018</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>310</v>
+        <v>194</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>364</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>14</v>
@@ -4429,7 +4446,7 @@
         <v>14</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N14" s="2">
         <v>7</v>
@@ -4438,34 +4455,34 @@
         <v>9</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z14" s="2" t="s">
         <v>14</v>
@@ -4477,13 +4494,13 @@
         <v>888</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF14" s="2" t="s">
         <v>14</v>
@@ -4493,40 +4510,40 @@
       </c>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="AJ14" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AK14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AN14" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AT14" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AV14" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="AP14" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AQ14" s="2">
-        <v>888</v>
-      </c>
-      <c r="AR14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="AT14" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="AU14" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="AW14" s="2"/>
       <c r="AX14" s="2"/>
@@ -4553,14 +4570,14 @@
       <c r="F15" s="5">
         <v>888</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>367</v>
+      <c r="G15" s="12" t="s">
+        <v>358</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>48</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>14</v>
@@ -4569,34 +4586,34 @@
         <v>49</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M15" s="7" t="s">
         <v>40</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="R15" s="5">
         <v>5</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V15" s="5" t="s">
         <v>50</v>
@@ -4605,28 +4622,28 @@
         <v>888</v>
       </c>
       <c r="X15" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="AA15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AB15" s="5">
         <v>888</v>
       </c>
       <c r="AC15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF15" s="4" t="s">
         <v>14</v>
@@ -4639,10 +4656,10 @@
         <v>43</v>
       </c>
       <c r="AJ15" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK15" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL15" s="5" t="s">
         <v>14</v>
@@ -4665,19 +4682,19 @@
       </c>
       <c r="AS15" s="7"/>
       <c r="AT15" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AU15" s="5" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AW15" s="9" t="s">
         <v>53</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
@@ -4702,17 +4719,17 @@
       <c r="F16" s="5">
         <v>888</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>368</v>
+      <c r="G16" s="11" t="s">
+        <v>359</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>58</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>59</v>
@@ -4724,7 +4741,7 @@
         <v>60</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>9</v>
@@ -4733,10 +4750,10 @@
         <v>40</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S16" s="5" t="s">
         <v>11</v>
@@ -4745,7 +4762,7 @@
         <v>888</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="V16" s="5" t="s">
         <v>61</v>
@@ -4769,13 +4786,13 @@
         <v>888</v>
       </c>
       <c r="AC16" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD16" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE16" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF16" s="4" t="s">
         <v>14</v>
@@ -4788,20 +4805,20 @@
         <v>43</v>
       </c>
       <c r="AJ16" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK16" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL16" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN16" s="5"/>
       <c r="AO16" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AP16" s="5">
         <v>888</v>
@@ -4817,14 +4834,14 @@
         <v>64</v>
       </c>
       <c r="AU16" s="5" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AW16" s="7"/>
       <c r="AX16" s="7" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
@@ -4849,38 +4866,38 @@
       <c r="F17" s="5">
         <v>888</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="L17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="N17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="O17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q17" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>40</v>
@@ -4892,19 +4909,19 @@
         <v>888</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="W17" s="5">
+        <v>888</v>
+      </c>
+      <c r="X17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="W17" s="5">
-        <v>888</v>
-      </c>
-      <c r="X17" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="Y17" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>14</v>
@@ -4935,20 +4952,20 @@
         <v>43</v>
       </c>
       <c r="AJ17" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK17" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL17" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN17" s="5"/>
       <c r="AO17" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AP17" s="5">
         <v>888</v>
@@ -4961,19 +4978,19 @@
       </c>
       <c r="AS17" s="7"/>
       <c r="AT17" s="5" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="AU17" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV17" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AW17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX17" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="AX17" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
@@ -4984,52 +5001,52 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="5">
+        <v>888</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="5">
-        <v>888</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="K18" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="K18" s="7" t="s">
+      <c r="L18" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="L18" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="M18" s="7" t="s">
+      <c r="N18" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="N18" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="O18" s="5" t="s">
+      <c r="P18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="P18" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="Q18" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R18" s="7">
         <v>3</v>
@@ -5041,37 +5058,37 @@
         <v>888</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="W18" s="5">
+        <v>888</v>
+      </c>
+      <c r="X18" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="W18" s="5">
-        <v>888</v>
-      </c>
-      <c r="X18" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="Y18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AA18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AB18" s="5">
         <v>888</v>
       </c>
       <c r="AC18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF18" s="4" t="s">
         <v>14</v>
@@ -5084,13 +5101,13 @@
         <v>43</v>
       </c>
       <c r="AJ18" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="AK18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL18" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM18" s="5" t="s">
         <v>14</v>
@@ -5107,16 +5124,16 @@
         <v>888</v>
       </c>
       <c r="AS18" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT18" s="5" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="AU18" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AV18" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AW18" s="9"/>
       <c r="AX18" s="7"/>
@@ -5129,49 +5146,49 @@
         <v>6</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="E19" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F19" s="5">
         <v>888</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="L19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="N19" s="7">
         <v>7</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q19" s="7" t="s">
         <v>39</v>
@@ -5180,62 +5197,62 @@
         <v>40</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T19" s="10" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W19" s="5">
         <v>888</v>
       </c>
       <c r="X19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>888</v>
+      </c>
+      <c r="AA19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB19" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="Y19" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>888</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="AB19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG19" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="AC19" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="AD19" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG19" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AJ19" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AK19" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL19" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM19" s="5" t="s">
         <v>14</v>
@@ -5252,19 +5269,19 @@
         <v>888</v>
       </c>
       <c r="AS19" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AU19" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV19" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AX19" s="7"/>
       <c r="AZ19" s="6"/>
@@ -5276,55 +5293,55 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F20" s="5">
+        <v>888</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="F20" s="5">
-        <v>888</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="L20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>11</v>
@@ -5333,19 +5350,19 @@
         <v>888</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="W20" s="5">
         <v>888</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>14</v>
@@ -5357,13 +5374,13 @@
         <v>888</v>
       </c>
       <c r="AC20" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD20" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE20" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF20" s="4" t="s">
         <v>14</v>
@@ -5376,20 +5393,20 @@
         <v>43</v>
       </c>
       <c r="AJ20" s="5" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="AK20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AL20" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AN20" s="5"/>
       <c r="AO20" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AP20" s="5">
         <v>888</v>
@@ -5401,16 +5418,16 @@
         <v>888</v>
       </c>
       <c r="AS20" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT20" s="5" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="AU20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AV20" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="AV20" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="AW20" s="9"/>
       <c r="AX20" s="7"/>
@@ -5423,52 +5440,52 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F21" s="5">
+        <v>888</v>
+      </c>
+      <c r="G21" t="s">
+        <v>360</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="F21" s="5">
-        <v>888</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>114</v>
-      </c>
       <c r="L21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N21" s="7">
         <v>6</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P21" s="7">
         <v>93.4</v>
       </c>
       <c r="Q21" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>40</v>
@@ -5477,22 +5494,22 @@
         <v>11</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="W21" s="5">
         <v>888</v>
       </c>
       <c r="X21" s="5" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>14</v>
@@ -5504,66 +5521,66 @@
         <v>888</v>
       </c>
       <c r="AC21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF21" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AG21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AH21" s="7"/>
       <c r="AI21" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="AJ21" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AK21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AL21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AM21" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AN21" s="5"/>
       <c r="AO21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="AP21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>888</v>
+      </c>
+      <c r="AS21" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="AT21" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AU21" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV21" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="AW21" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="AP21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AQ21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AR21" s="5">
-        <v>888</v>
-      </c>
-      <c r="AS21" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="AT21" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="AU21" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="AV21" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="AW21" s="9" t="s">
+      <c r="AX21" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="AX21" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
@@ -5574,28 +5591,28 @@
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5">
+        <v>888</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F22" s="5">
-        <v>888</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="I22" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>14</v>
@@ -5607,10 +5624,10 @@
         <v>14</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>9</v>
@@ -5619,28 +5636,28 @@
         <v>25</v>
       </c>
       <c r="Q22" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R22" s="7">
         <v>3</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="W22" s="5">
         <v>888</v>
       </c>
       <c r="X22" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="Y22" s="5">
         <v>888</v>
@@ -5655,10 +5672,10 @@
         <v>888</v>
       </c>
       <c r="AC22" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AD22" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AE22" s="5" t="s">
         <v>14</v>
@@ -5667,7 +5684,7 @@
         <v>888</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="5">
@@ -5697,22 +5714,22 @@
         <v>888</v>
       </c>
       <c r="AS22" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AT22" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AU22" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AV22" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AW22" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AX22" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AY22" s="2"/>
       <c r="BA22" s="6"/>
@@ -5738,9 +5755,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5890,26 +5910,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5933,9 +5942,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>